<commit_message>
Add footprints and schematic symbols
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Altium projects\Moi\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC53A6-8602-4C21-8A83-4EB5BE7E1BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7199A3B-28CC-452F-A919-A2A9471DCF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3238" uniqueCount="755">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -2175,27 +2175,6 @@
     <t>RTC crystal</t>
   </si>
   <si>
-    <t>NPN</t>
-  </si>
-  <si>
-    <t>PNP</t>
-  </si>
-  <si>
-    <t>NMOS</t>
-  </si>
-  <si>
-    <t>PMOS</t>
-  </si>
-  <si>
-    <t>DIODE</t>
-  </si>
-  <si>
-    <t>SCHOTTKY</t>
-  </si>
-  <si>
-    <t>ZENER</t>
-  </si>
-  <si>
     <t>MMSD4148T1G</t>
   </si>
   <si>
@@ -2209,6 +2188,132 @@
   </si>
   <si>
     <t>General purpose PN diode</t>
+  </si>
+  <si>
+    <t>D_PN</t>
+  </si>
+  <si>
+    <t>D_ZENER</t>
+  </si>
+  <si>
+    <t>D_SCHOTTKY</t>
+  </si>
+  <si>
+    <t>NPN_SOT23</t>
+  </si>
+  <si>
+    <t>PNP_SOT23</t>
+  </si>
+  <si>
+    <t>NMOS_SOT23</t>
+  </si>
+  <si>
+    <t>PMOS_SOT23</t>
+  </si>
+  <si>
+    <t>LED_0603</t>
+  </si>
+  <si>
+    <t>LED_RED</t>
+  </si>
+  <si>
+    <t>LED_GREEN</t>
+  </si>
+  <si>
+    <t>LED_BLUE</t>
+  </si>
+  <si>
+    <t>733910060</t>
+  </si>
+  <si>
+    <t>MMBT2222A-FDICT-ND</t>
+  </si>
+  <si>
+    <t>MMBT2222A-7-F</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>AEC-Q101 Qualified</t>
+  </si>
+  <si>
+    <t>General purpose NPN transistor in SOT23 package</t>
+  </si>
+  <si>
+    <t>MMBT2907A-7-F</t>
+  </si>
+  <si>
+    <t>General purpose PNP transistor in SOT23 package</t>
+  </si>
+  <si>
+    <t>MMBT2907A-FDICT-ND</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>BSS138CT-ND</t>
+  </si>
+  <si>
+    <t>FBEAD</t>
+  </si>
+  <si>
+    <t>FBTH1608HL221-T</t>
+  </si>
+  <si>
+    <t>0603_IND</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>587-FBTH1608HL221-TCT-ND</t>
+  </si>
+  <si>
+    <t>650mA max, AEC-Q200 Qualified</t>
+  </si>
+  <si>
+    <t>Ferrite bead</t>
+  </si>
+  <si>
+    <t>BSS84</t>
+  </si>
+  <si>
+    <t>BSS84CT-ND</t>
+  </si>
+  <si>
+    <t>FDN360P</t>
+  </si>
+  <si>
+    <t>FDN360PCT-ND</t>
+  </si>
+  <si>
+    <t>Vds 50V, Id 220mA</t>
+  </si>
+  <si>
+    <t>Vds 50V, Id 130mA</t>
+  </si>
+  <si>
+    <t>Vds 30V, Id 2A</t>
+  </si>
+  <si>
+    <t>FDN337N</t>
+  </si>
+  <si>
+    <t>FDN337NCT-ND</t>
+  </si>
+  <si>
+    <t>Vds 30V, Id 2.2A</t>
+  </si>
+  <si>
+    <t>General purpose N-Channel MOSFET in SOT23 packagge</t>
+  </si>
+  <si>
+    <t>General purpose P-Channel MOSFET in SOT23 packagge</t>
   </si>
 </sst>
 </file>
@@ -7826,7 +7931,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7834,7 +7939,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
@@ -7901,7 +8006,7 @@
         <v>604</v>
       </c>
       <c r="D2" t="s">
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="E2" t="s">
         <v>625</v>
@@ -7969,9 +8074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8579,7 +8684,7 @@
         <v>574</v>
       </c>
       <c r="B16" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="C16" t="s">
         <v>580</v>
@@ -8995,9 +9100,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9184,8 +9289,8 @@
       <c r="E5" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="F5" s="10">
-        <v>733910060</v>
+      <c r="F5" s="10" t="s">
+        <v>724</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>48</v>
@@ -9475,7 +9580,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A6:D6 F6" numberStoredAsText="1"/>
+    <ignoredError sqref="A6:D6 F5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9567,16 +9672,16 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -9637,6 +9742,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2" t="s">
+        <v>720</v>
+      </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
@@ -9645,6 +9756,16 @@
       </c>
       <c r="J2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -12401,24 +12522,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9A30D3-6C2F-40AA-A14D-6B8FBBCB1DF8}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -12551,6 +12673,44 @@
       </c>
       <c r="M3" t="s">
         <v>680</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>736</v>
+      </c>
+      <c r="B4" t="s">
+        <v>738</v>
+      </c>
+      <c r="C4" t="s">
+        <v>738</v>
+      </c>
+      <c r="D4" t="s">
+        <v>737</v>
+      </c>
+      <c r="E4" t="s">
+        <v>739</v>
+      </c>
+      <c r="F4" t="s">
+        <v>737</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>740</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>741</v>
+      </c>
+      <c r="M4" t="s">
+        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -12564,7 +12724,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12766,22 +12926,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12831,49 +12992,108 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>708</v>
+        <v>716</v>
+      </c>
+      <c r="B2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E2" t="s">
+        <v>728</v>
+      </c>
+      <c r="F2" t="s">
+        <v>726</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
+      <c r="H2" t="s">
+        <v>725</v>
+      </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
       <c r="J2" t="s">
         <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>729</v>
+      </c>
+      <c r="M2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>709</v>
+        <v>717</v>
+      </c>
+      <c r="B3" t="s">
+        <v>727</v>
+      </c>
+      <c r="C3" t="s">
+        <v>727</v>
+      </c>
+      <c r="D3" t="s">
+        <v>731</v>
+      </c>
+      <c r="E3" t="s">
+        <v>728</v>
+      </c>
+      <c r="F3" t="s">
+        <v>731</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>733</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>729</v>
+      </c>
+      <c r="M3" t="s">
+        <v>732</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FF62D7-1327-4F91-B133-5C6C7A06CCE3}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12923,21 +13143,154 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>710</v>
+        <v>718</v>
+      </c>
+      <c r="B2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2" t="s">
+        <v>734</v>
+      </c>
+      <c r="E2" t="s">
+        <v>709</v>
+      </c>
+      <c r="F2" t="s">
+        <v>734</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
+      <c r="H2" t="s">
+        <v>735</v>
+      </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>747</v>
+      </c>
+      <c r="M2" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>711</v>
+        <v>718</v>
+      </c>
+      <c r="B3" t="s">
+        <v>727</v>
+      </c>
+      <c r="C3" t="s">
+        <v>727</v>
+      </c>
+      <c r="D3" t="s">
+        <v>750</v>
+      </c>
+      <c r="E3" t="s">
+        <v>709</v>
+      </c>
+      <c r="F3" t="s">
+        <v>750</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>751</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>752</v>
+      </c>
+      <c r="M3" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>719</v>
+      </c>
+      <c r="B4" t="s">
+        <v>727</v>
+      </c>
+      <c r="C4" t="s">
+        <v>727</v>
+      </c>
+      <c r="D4" t="s">
+        <v>743</v>
+      </c>
+      <c r="E4" t="s">
+        <v>709</v>
+      </c>
+      <c r="F4" t="s">
+        <v>743</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>744</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>748</v>
+      </c>
+      <c r="M4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B5" t="s">
+        <v>727</v>
+      </c>
+      <c r="C5" t="s">
+        <v>727</v>
+      </c>
+      <c r="D5" t="s">
+        <v>745</v>
+      </c>
+      <c r="E5" t="s">
+        <v>709</v>
+      </c>
+      <c r="F5" t="s">
+        <v>745</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>746</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>749</v>
+      </c>
+      <c r="M5" t="s">
+        <v>754</v>
       </c>
     </row>
   </sheetData>
@@ -12951,12 +13304,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -13016,37 +13369,37 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2" t="s">
+        <v>711</v>
+      </c>
+      <c r="D2" t="s">
+        <v>708</v>
+      </c>
+      <c r="E2" t="s">
+        <v>709</v>
+      </c>
+      <c r="F2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>710</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
         <v>712</v>
-      </c>
-      <c r="B2" t="s">
-        <v>718</v>
-      </c>
-      <c r="C2" t="s">
-        <v>718</v>
-      </c>
-      <c r="D2" t="s">
-        <v>715</v>
-      </c>
-      <c r="E2" t="s">
-        <v>716</v>
-      </c>
-      <c r="F2" t="s">
-        <v>715</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>717</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -13056,7 +13409,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a lot of JST GH connectors and other stuff
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Altium projects\Moi\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7199A3B-28CC-452F-A919-A2A9471DCF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A0E411-54A3-4A7E-9BA0-305DEE714437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3238" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="862">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -1965,9 +1965,6 @@
     <t>A33219-ND</t>
   </si>
   <si>
-    <t>250V 5A max</t>
-  </si>
-  <si>
     <t>2 pin vertical molex style connector</t>
   </si>
   <si>
@@ -2314,6 +2311,330 @@
   </si>
   <si>
     <t>General purpose P-Channel MOSFET in SOT23 packagge</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>PNP</t>
+  </si>
+  <si>
+    <t>NMOS</t>
+  </si>
+  <si>
+    <t>PMOS</t>
+  </si>
+  <si>
+    <t>RN52-I/RM116</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>RN52-I/RM116-ND</t>
+  </si>
+  <si>
+    <t>Bluetooth 3.0 audio codec module</t>
+  </si>
+  <si>
+    <t>RN52-IRM116</t>
+  </si>
+  <si>
+    <t>BM02B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1578-1-ND</t>
+  </si>
+  <si>
+    <t>455-1580-1-ND</t>
+  </si>
+  <si>
+    <t>455-1582-1-ND</t>
+  </si>
+  <si>
+    <t>455-1584-1-ND</t>
+  </si>
+  <si>
+    <t>455-1586-1-ND</t>
+  </si>
+  <si>
+    <t>455-1588-1-ND</t>
+  </si>
+  <si>
+    <t>455-1564-1-ND</t>
+  </si>
+  <si>
+    <t>455-1566-1-ND</t>
+  </si>
+  <si>
+    <t>455-1568-1-ND</t>
+  </si>
+  <si>
+    <t>455-1570-1-ND</t>
+  </si>
+  <si>
+    <t>455-1572-1-ND</t>
+  </si>
+  <si>
+    <t>455-1574-1-ND</t>
+  </si>
+  <si>
+    <t>BM04B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>BM06B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>BM08B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>BM10B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>BM12B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>SM02B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM04B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM06B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM08B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM10B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM12B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>Conn-2pos</t>
+  </si>
+  <si>
+    <t>Conn-4pos</t>
+  </si>
+  <si>
+    <t>Conn-6pos</t>
+  </si>
+  <si>
+    <t>Conn-8pos</t>
+  </si>
+  <si>
+    <t>Conn-10pos</t>
+  </si>
+  <si>
+    <t>Conn-12pos</t>
+  </si>
+  <si>
+    <t>50 V 1 A max</t>
+  </si>
+  <si>
+    <t>250 V 5 A max</t>
+  </si>
+  <si>
+    <t>2 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>4 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>6 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>8 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>10 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>12 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>2 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>4 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>6 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>8 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>10 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>12 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>Conn-3pos</t>
+  </si>
+  <si>
+    <t>Conn-5pos</t>
+  </si>
+  <si>
+    <t>Conn-7pos</t>
+  </si>
+  <si>
+    <t>Conn-9pos</t>
+  </si>
+  <si>
+    <t>Conn-11pos</t>
+  </si>
+  <si>
+    <t>Conn-13pos</t>
+  </si>
+  <si>
+    <t>Conn-14pos</t>
+  </si>
+  <si>
+    <t>Conn-15pos</t>
+  </si>
+  <si>
+    <t>3 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>5 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>7 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>9 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>11 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>13 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>14 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>15 pin vertical JST GH connector</t>
+  </si>
+  <si>
+    <t>3 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>5 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>7 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>9 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>11 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>13 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>14 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>15 pin horizontal JST GH connector</t>
+  </si>
+  <si>
+    <t>BM03B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1579-1-ND</t>
+  </si>
+  <si>
+    <t>BM05B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1581-1-ND</t>
+  </si>
+  <si>
+    <t>BM07B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1583-1-ND</t>
+  </si>
+  <si>
+    <t>BM09B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1585-1-ND</t>
+  </si>
+  <si>
+    <t>BM11B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1587-1-ND</t>
+  </si>
+  <si>
+    <t>BM13B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1589-1-ND</t>
+  </si>
+  <si>
+    <t>BM14B-GHS-TBT(LF)(SN)(N)</t>
+  </si>
+  <si>
+    <t>455-1590-1-ND</t>
+  </si>
+  <si>
+    <t>BM15B-GHS-TBT(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1591-1-ND</t>
+  </si>
+  <si>
+    <t>SM03B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1565-1-ND</t>
+  </si>
+  <si>
+    <t>SM05B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1567-1-ND</t>
+  </si>
+  <si>
+    <t>SM07B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1569-1-ND</t>
+  </si>
+  <si>
+    <t>SM09B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1571-1-ND</t>
+  </si>
+  <si>
+    <t>SM11B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1573-1-ND</t>
+  </si>
+  <si>
+    <t>SM13B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>SM14B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1576-1-ND</t>
+  </si>
+  <si>
+    <t>SM15B-GHS-TB(LF)(SN)</t>
   </si>
 </sst>
 </file>
@@ -2684,8 +3005,8 @@
   <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7927,27 +8248,26 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" customWidth="1"/>
+    <col min="13" max="13" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8063,6 +8383,41 @@
       </c>
       <c r="M3" t="s">
         <v>623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>762</v>
+      </c>
+      <c r="B4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C4" t="s">
+        <v>758</v>
+      </c>
+      <c r="D4" t="s">
+        <v>762</v>
+      </c>
+      <c r="E4" t="s">
+        <v>759</v>
+      </c>
+      <c r="F4" t="s">
+        <v>758</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>760</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -8074,7 +8429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
@@ -9059,36 +9414,36 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>669</v>
+      </c>
+      <c r="B2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C2" t="s">
         <v>670</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>669</v>
+      </c>
+      <c r="M2" t="s">
         <v>670</v>
-      </c>
-      <c r="C2" t="s">
-        <v>671</v>
-      </c>
-      <c r="D2" t="s">
-        <v>670</v>
-      </c>
-      <c r="M2" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>671</v>
+      </c>
+      <c r="B3" t="s">
+        <v>671</v>
+      </c>
+      <c r="C3" t="s">
+        <v>671</v>
+      </c>
+      <c r="D3" t="s">
+        <v>671</v>
+      </c>
+      <c r="M3" t="s">
         <v>672</v>
-      </c>
-      <c r="B3" t="s">
-        <v>672</v>
-      </c>
-      <c r="C3" t="s">
-        <v>672</v>
-      </c>
-      <c r="D3" t="s">
-        <v>672</v>
-      </c>
-      <c r="M3" t="s">
-        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -9098,18 +9453,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.7109375" style="10" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -9200,7 +9556,7 @@
         <v>634</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9235,33 +9591,33 @@
         <v>16</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>654</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>655</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>7</v>
@@ -9270,7 +9626,7 @@
         <v>16</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -9287,16 +9643,16 @@
         <v>733910060</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>7</v>
@@ -9305,36 +9661,36 @@
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>660</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>667</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>659</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>668</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>7</v>
@@ -9343,36 +9699,36 @@
         <v>16</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>666</v>
-      </c>
       <c r="G7" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>7</v>
@@ -9381,15 +9737,15 @@
         <v>16</v>
       </c>
       <c r="K7" s="10" t="s">
+        <v>662</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>663</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>636</v>
+        <v>788</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>636</v>
@@ -9419,36 +9775,36 @@
         <v>16</v>
       </c>
       <c r="K8" s="10" t="s">
+        <v>795</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>638</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>643</v>
+        <v>789</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>635</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>7</v>
@@ -9457,36 +9813,36 @@
         <v>16</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>638</v>
+        <v>795</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>645</v>
+        <v>790</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>635</v>
       </c>
       <c r="F10" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>645</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>646</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>7</v>
@@ -9495,36 +9851,36 @@
         <v>16</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>638</v>
+        <v>795</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>649</v>
+        <v>791</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>635</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>7</v>
@@ -9533,36 +9889,36 @@
         <v>16</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>638</v>
+        <v>795</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>650</v>
+        <v>789</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>635</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>7</v>
@@ -9571,14 +9927,1068 @@
         <v>16</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>638</v>
+        <v>795</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>788</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>789</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>842</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>842</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>842</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>842</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>788</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>789</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>852</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>852</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>852</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>852</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M33" s="10" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M34" s="10" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>774</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>857</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>831</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A6:D6 F5" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -9743,10 +11153,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
@@ -9760,12 +11170,12 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
   </sheetData>
@@ -12592,28 +14002,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>673</v>
+      </c>
+      <c r="B2" t="s">
         <v>674</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D2" t="s">
+        <v>674</v>
+      </c>
+      <c r="E2" t="s">
         <v>675</v>
       </c>
-      <c r="C2" t="s">
-        <v>675</v>
-      </c>
-      <c r="D2" t="s">
-        <v>675</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>674</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>676</v>
-      </c>
-      <c r="F2" t="s">
-        <v>675</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>677</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -12622,42 +14032,42 @@
         <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="L2" t="s">
+        <v>677</v>
+      </c>
+      <c r="M2" t="s">
+        <v>679</v>
+      </c>
+      <c r="N2" t="s">
         <v>678</v>
-      </c>
-      <c r="M2" t="s">
-        <v>680</v>
-      </c>
-      <c r="N2" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E3" t="s">
+        <v>681</v>
+      </c>
+      <c r="F3" t="s">
         <v>682</v>
       </c>
-      <c r="F3" t="s">
-        <v>683</v>
-      </c>
       <c r="G3" t="s">
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -12666,51 +14076,51 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>735</v>
+      </c>
+      <c r="B4" t="s">
+        <v>737</v>
+      </c>
+      <c r="C4" t="s">
+        <v>737</v>
+      </c>
+      <c r="D4" t="s">
         <v>736</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>738</v>
       </c>
-      <c r="C4" t="s">
-        <v>738</v>
-      </c>
-      <c r="D4" t="s">
-        <v>737</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>736</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>739</v>
       </c>
-      <c r="F4" t="s">
-        <v>737</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
         <v>740</v>
       </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>741</v>
-      </c>
-      <c r="M4" t="s">
-        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -12788,28 +14198,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2" t="s">
+        <v>699</v>
+      </c>
+      <c r="D2" t="s">
         <v>688</v>
       </c>
-      <c r="B2" t="s">
-        <v>700</v>
-      </c>
-      <c r="C2" t="s">
-        <v>700</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>689</v>
       </c>
-      <c r="E2" t="s">
-        <v>690</v>
-      </c>
       <c r="F2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -12818,42 +14228,42 @@
         <v>16</v>
       </c>
       <c r="K2" t="s">
+        <v>691</v>
+      </c>
+      <c r="L2" t="s">
+        <v>690</v>
+      </c>
+      <c r="M2" t="s">
         <v>692</v>
       </c>
-      <c r="L2" t="s">
-        <v>691</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>693</v>
-      </c>
-      <c r="N2" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D3" t="s">
+        <v>694</v>
+      </c>
+      <c r="E3" t="s">
+        <v>689</v>
+      </c>
+      <c r="F3" t="s">
+        <v>694</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>695</v>
-      </c>
-      <c r="E3" t="s">
-        <v>690</v>
-      </c>
-      <c r="F3" t="s">
-        <v>695</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>696</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -12862,39 +14272,39 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
+        <v>696</v>
+      </c>
+      <c r="L3" t="s">
         <v>697</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>698</v>
-      </c>
-      <c r="M3" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>701</v>
+      </c>
+      <c r="B4" t="s">
+        <v>701</v>
+      </c>
+      <c r="C4" t="s">
+        <v>701</v>
+      </c>
+      <c r="D4" t="s">
+        <v>701</v>
+      </c>
+      <c r="E4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F4" t="s">
+        <v>701</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>702</v>
-      </c>
-      <c r="B4" t="s">
-        <v>702</v>
-      </c>
-      <c r="C4" t="s">
-        <v>702</v>
-      </c>
-      <c r="D4" t="s">
-        <v>702</v>
-      </c>
-      <c r="E4" t="s">
-        <v>701</v>
-      </c>
-      <c r="F4" t="s">
-        <v>702</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>703</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -12903,16 +14313,16 @@
         <v>16</v>
       </c>
       <c r="K4" t="s">
+        <v>703</v>
+      </c>
+      <c r="L4" t="s">
         <v>704</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>705</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>706</v>
-      </c>
-      <c r="N4" t="s">
-        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -12926,7 +14336,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12992,78 +14402,84 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C2" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2" t="s">
+        <v>725</v>
+      </c>
+      <c r="E2" t="s">
         <v>727</v>
       </c>
-      <c r="C2" t="s">
-        <v>727</v>
-      </c>
-      <c r="D2" t="s">
-        <v>726</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>725</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>724</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
         <v>728</v>
       </c>
-      <c r="F2" t="s">
-        <v>726</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>725</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>754</v>
+      </c>
+      <c r="M2" t="s">
         <v>729</v>
-      </c>
-      <c r="M2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B3" t="s">
+        <v>726</v>
+      </c>
+      <c r="C3" t="s">
+        <v>726</v>
+      </c>
+      <c r="D3" t="s">
+        <v>730</v>
+      </c>
+      <c r="E3" t="s">
         <v>727</v>
       </c>
-      <c r="C3" t="s">
-        <v>727</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>732</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>728</v>
+      </c>
+      <c r="L3" t="s">
+        <v>755</v>
+      </c>
+      <c r="M3" t="s">
         <v>731</v>
-      </c>
-      <c r="E3" t="s">
-        <v>728</v>
-      </c>
-      <c r="F3" t="s">
-        <v>731</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>733</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>729</v>
-      </c>
-      <c r="M3" t="s">
-        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -13078,7 +14494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13143,29 +14559,29 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D2" t="s">
+        <v>733</v>
+      </c>
+      <c r="E2" t="s">
+        <v>708</v>
+      </c>
+      <c r="F2" t="s">
+        <v>733</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>734</v>
       </c>
-      <c r="E2" t="s">
-        <v>709</v>
-      </c>
-      <c r="F2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>735</v>
-      </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
@@ -13173,75 +14589,81 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>747</v>
+        <v>746</v>
+      </c>
+      <c r="L2" t="s">
+        <v>756</v>
       </c>
       <c r="M2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D3" t="s">
+        <v>749</v>
+      </c>
+      <c r="E3" t="s">
+        <v>708</v>
+      </c>
+      <c r="F3" t="s">
+        <v>749</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>750</v>
       </c>
-      <c r="E3" t="s">
-        <v>709</v>
-      </c>
-      <c r="F3" t="s">
-        <v>750</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
         <v>751</v>
       </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>756</v>
+      </c>
+      <c r="M3" t="s">
         <v>752</v>
-      </c>
-      <c r="M3" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D4" t="s">
+        <v>742</v>
+      </c>
+      <c r="E4" t="s">
+        <v>708</v>
+      </c>
+      <c r="F4" t="s">
+        <v>742</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>743</v>
       </c>
-      <c r="E4" t="s">
-        <v>709</v>
-      </c>
-      <c r="F4" t="s">
-        <v>743</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>744</v>
-      </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
@@ -13249,37 +14671,40 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>748</v>
+        <v>747</v>
+      </c>
+      <c r="L4" t="s">
+        <v>757</v>
       </c>
       <c r="M4" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D5" t="s">
+        <v>744</v>
+      </c>
+      <c r="E5" t="s">
+        <v>708</v>
+      </c>
+      <c r="F5" t="s">
+        <v>744</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
         <v>745</v>
       </c>
-      <c r="E5" t="s">
-        <v>709</v>
-      </c>
-      <c r="F5" t="s">
-        <v>745</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>746</v>
-      </c>
       <c r="I5" t="s">
         <v>7</v>
       </c>
@@ -13287,10 +14712,13 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>749</v>
+        <v>748</v>
+      </c>
+      <c r="L5" t="s">
+        <v>757</v>
       </c>
       <c r="M5" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -13369,47 +14797,47 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B2" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2" t="s">
+        <v>710</v>
+      </c>
+      <c r="D2" t="s">
+        <v>707</v>
+      </c>
+      <c r="E2" t="s">
+        <v>708</v>
+      </c>
+      <c r="F2" t="s">
+        <v>707</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>709</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
         <v>711</v>
-      </c>
-      <c r="C2" t="s">
-        <v>711</v>
-      </c>
-      <c r="D2" t="s">
-        <v>708</v>
-      </c>
-      <c r="E2" t="s">
-        <v>709</v>
-      </c>
-      <c r="F2" t="s">
-        <v>708</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>710</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add components for knob
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Altium projects\Moi\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A0E411-54A3-4A7E-9BA0-305DEE714437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DE1890-2B2E-4140-8DF3-0E7E697B26DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="880">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -2635,6 +2635,60 @@
   </si>
   <si>
     <t>SM15B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>MT6701</t>
+  </si>
+  <si>
+    <t>SOP-8</t>
+  </si>
+  <si>
+    <t>MT6701CT-STD</t>
+  </si>
+  <si>
+    <t>MagnTek</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>C2856764</t>
+  </si>
+  <si>
+    <t>Hall effect absolute magnetic encoder</t>
+  </si>
+  <si>
+    <t>TMC6300</t>
+  </si>
+  <si>
+    <t>QFN-20 (3x3)</t>
+  </si>
+  <si>
+    <t>TMC6300-LA-T</t>
+  </si>
+  <si>
+    <t>Trinamic Motion Control GmbH</t>
+  </si>
+  <si>
+    <t>1460-TMC6300-LA-TCT-ND</t>
+  </si>
+  <si>
+    <t>2-11V 2A 3-phase BLDC motor driver</t>
+  </si>
+  <si>
+    <t>Motor Driver</t>
+  </si>
+  <si>
+    <t>HX711</t>
+  </si>
+  <si>
+    <t>Avia Semicon</t>
+  </si>
+  <si>
+    <t>SOP-16</t>
+  </si>
+  <si>
+    <t>C43656</t>
   </si>
 </sst>
 </file>
@@ -3005,7 +3059,7 @@
   <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -8427,11 +8481,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8439,10 +8493,10 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -9336,6 +9390,114 @@
       </c>
       <c r="O23" t="s">
         <v>621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>862</v>
+      </c>
+      <c r="B24" t="s">
+        <v>863</v>
+      </c>
+      <c r="C24" t="s">
+        <v>863</v>
+      </c>
+      <c r="D24" t="s">
+        <v>864</v>
+      </c>
+      <c r="E24" t="s">
+        <v>865</v>
+      </c>
+      <c r="F24" t="s">
+        <v>864</v>
+      </c>
+      <c r="G24" t="s">
+        <v>866</v>
+      </c>
+      <c r="H24" t="s">
+        <v>867</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" t="s">
+        <v>868</v>
+      </c>
+      <c r="O24" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>869</v>
+      </c>
+      <c r="B25" t="s">
+        <v>869</v>
+      </c>
+      <c r="C25" t="s">
+        <v>870</v>
+      </c>
+      <c r="D25" t="s">
+        <v>871</v>
+      </c>
+      <c r="E25" t="s">
+        <v>872</v>
+      </c>
+      <c r="F25" t="s">
+        <v>871</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>873</v>
+      </c>
+      <c r="I25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" t="s">
+        <v>874</v>
+      </c>
+      <c r="O25" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>876</v>
+      </c>
+      <c r="B26" t="s">
+        <v>878</v>
+      </c>
+      <c r="C26" t="s">
+        <v>878</v>
+      </c>
+      <c r="D26" t="s">
+        <v>876</v>
+      </c>
+      <c r="E26" t="s">
+        <v>877</v>
+      </c>
+      <c r="F26" t="s">
+        <v>876</v>
+      </c>
+      <c r="G26" t="s">
+        <v>866</v>
+      </c>
+      <c r="H26" t="s">
+        <v>879</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -9455,8 +9617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 128mbit flash chip and USB-C connector
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Altium projects\Moi\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DE1890-2B2E-4140-8DF3-0E7E697B26DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED03587D-9A53-4F64-B519-5AEDC533ADA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3674" uniqueCount="902">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -1911,9 +1911,6 @@
     <t>Multiwatt-15</t>
   </si>
   <si>
-    <t>80W @ 80 Ohm Class AB power amplifier</t>
-  </si>
-  <si>
     <t>Audio</t>
   </si>
   <si>
@@ -2679,16 +2676,85 @@
     <t>Motor Driver</t>
   </si>
   <si>
-    <t>HX711</t>
-  </si>
-  <si>
-    <t>Avia Semicon</t>
-  </si>
-  <si>
-    <t>SOP-16</t>
-  </si>
-  <si>
-    <t>C43656</t>
+    <t>MCP3564R</t>
+  </si>
+  <si>
+    <t>20-TSSOP</t>
+  </si>
+  <si>
+    <t>MCP3564RT-E/ST</t>
+  </si>
+  <si>
+    <t>150-MCP3564RT-E/STCT-ND</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Low-noise 24-bit Delta-Sigma ADC, 2/4/8 ch single ended, 1/2/4 ch differential</t>
+  </si>
+  <si>
+    <t>TAS5630BDKDR</t>
+  </si>
+  <si>
+    <t>TAS5630BDKD</t>
+  </si>
+  <si>
+    <t>296-29894-1-ND</t>
+  </si>
+  <si>
+    <t>44-HSSOP PowerPAD</t>
+  </si>
+  <si>
+    <t>80W @ 8 Ohm Class AB power amplifier</t>
+  </si>
+  <si>
+    <t>300W stereo, 400W mono Class D power amplifier</t>
+  </si>
+  <si>
+    <t>PCM4222PFBR</t>
+  </si>
+  <si>
+    <t>296-21703-1-ND</t>
+  </si>
+  <si>
+    <t>Stereo 24-bit 124 dB SNR Audio ADC</t>
+  </si>
+  <si>
+    <t>PCM4104PFBR</t>
+  </si>
+  <si>
+    <t>296-39146-1-ND</t>
+  </si>
+  <si>
+    <t>4-channel 24-bit 118 dB SNR Audio DAC</t>
+  </si>
+  <si>
+    <t>48-TQFP (7x7)</t>
+  </si>
+  <si>
+    <t>PCM4222</t>
+  </si>
+  <si>
+    <t>PCM4104</t>
+  </si>
+  <si>
+    <t>SMF2000</t>
+  </si>
+  <si>
+    <t>Trenz Electronic</t>
+  </si>
+  <si>
+    <t>TEM0001-01A-010C</t>
+  </si>
+  <si>
+    <t>FPGA Module with Cortex M3 MCU</t>
+  </si>
+  <si>
+    <t>LED_YELLOW</t>
+  </si>
+  <si>
+    <t>3 pin vertical 2.54 mm header</t>
   </si>
 </sst>
 </file>
@@ -3059,8 +3125,8 @@
   <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8302,11 +8368,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8380,19 +8446,19 @@
         <v>604</v>
       </c>
       <c r="D2" t="s">
+        <v>623</v>
+      </c>
+      <c r="E2" t="s">
         <v>624</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>623</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>625</v>
-      </c>
-      <c r="F2" t="s">
-        <v>624</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>626</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -8401,7 +8467,7 @@
         <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8427,7 +8493,7 @@
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -8436,33 +8502,33 @@
         <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C4" t="s">
+        <v>757</v>
+      </c>
+      <c r="D4" t="s">
+        <v>761</v>
+      </c>
+      <c r="E4" t="s">
         <v>758</v>
       </c>
-      <c r="D4" t="s">
-        <v>762</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>757</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>759</v>
-      </c>
-      <c r="F4" t="s">
-        <v>758</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>760</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -8471,21 +8537,51 @@
         <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>761</v>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>896</v>
+      </c>
+      <c r="B5" t="s">
+        <v>896</v>
+      </c>
+      <c r="C5" t="s">
+        <v>896</v>
+      </c>
+      <c r="D5" t="s">
+        <v>896</v>
+      </c>
+      <c r="E5" t="s">
+        <v>897</v>
+      </c>
+      <c r="F5" t="s">
+        <v>898</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>899</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8496,12 +8592,12 @@
     <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="66" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.5703125" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -9386,36 +9482,36 @@
         <v>16</v>
       </c>
       <c r="M23" t="s">
+        <v>885</v>
+      </c>
+      <c r="O23" t="s">
         <v>620</v>
-      </c>
-      <c r="O23" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>861</v>
+      </c>
+      <c r="B24" t="s">
         <v>862</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>862</v>
+      </c>
+      <c r="D24" t="s">
         <v>863</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
+        <v>864</v>
+      </c>
+      <c r="F24" t="s">
         <v>863</v>
       </c>
-      <c r="D24" t="s">
-        <v>864</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>865</v>
       </c>
-      <c r="F24" t="s">
-        <v>864</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>866</v>
-      </c>
-      <c r="H24" t="s">
-        <v>867</v>
       </c>
       <c r="I24" t="s">
         <v>7</v>
@@ -9424,7 +9520,7 @@
         <v>16</v>
       </c>
       <c r="M24" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="O24" t="s">
         <v>521</v>
@@ -9432,28 +9528,28 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>868</v>
+      </c>
+      <c r="B25" t="s">
+        <v>868</v>
+      </c>
+      <c r="C25" t="s">
         <v>869</v>
       </c>
-      <c r="B25" t="s">
-        <v>869</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>870</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>871</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>870</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
         <v>872</v>
-      </c>
-      <c r="F25" t="s">
-        <v>871</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" t="s">
-        <v>873</v>
       </c>
       <c r="I25" t="s">
         <v>7</v>
@@ -9462,48 +9558,168 @@
         <v>16</v>
       </c>
       <c r="M25" t="s">
+        <v>873</v>
+      </c>
+      <c r="O25" t="s">
         <v>874</v>
-      </c>
-      <c r="O25" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>875</v>
+      </c>
+      <c r="B26" t="s">
         <v>876</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>876</v>
+      </c>
+      <c r="D26" t="s">
+        <v>877</v>
+      </c>
+      <c r="E26" t="s">
+        <v>758</v>
+      </c>
+      <c r="F26" t="s">
+        <v>877</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" t="s">
         <v>878</v>
-      </c>
-      <c r="C26" t="s">
-        <v>878</v>
-      </c>
-      <c r="D26" t="s">
-        <v>876</v>
-      </c>
-      <c r="E26" t="s">
-        <v>877</v>
-      </c>
-      <c r="F26" t="s">
-        <v>876</v>
-      </c>
-      <c r="G26" t="s">
-        <v>866</v>
-      </c>
-      <c r="H26" t="s">
-        <v>879</v>
       </c>
       <c r="I26" t="s">
         <v>7</v>
       </c>
       <c r="J26" t="s">
         <v>16</v>
+      </c>
+      <c r="M26" t="s">
+        <v>880</v>
+      </c>
+      <c r="O26" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>882</v>
+      </c>
+      <c r="B27" t="s">
+        <v>882</v>
+      </c>
+      <c r="C27" t="s">
+        <v>884</v>
+      </c>
+      <c r="D27" t="s">
+        <v>881</v>
+      </c>
+      <c r="E27" t="s">
+        <v>527</v>
+      </c>
+      <c r="F27" t="s">
+        <v>881</v>
+      </c>
+      <c r="G27" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" t="s">
+        <v>883</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" t="s">
+        <v>886</v>
+      </c>
+      <c r="O27" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>894</v>
+      </c>
+      <c r="B28" t="s">
+        <v>893</v>
+      </c>
+      <c r="C28" t="s">
+        <v>893</v>
+      </c>
+      <c r="D28" t="s">
+        <v>887</v>
+      </c>
+      <c r="E28" t="s">
+        <v>527</v>
+      </c>
+      <c r="F28" t="s">
+        <v>887</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>888</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" t="s">
+        <v>889</v>
+      </c>
+      <c r="O28" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>895</v>
+      </c>
+      <c r="B29" t="s">
+        <v>893</v>
+      </c>
+      <c r="C29" t="s">
+        <v>893</v>
+      </c>
+      <c r="D29" t="s">
+        <v>890</v>
+      </c>
+      <c r="E29" t="s">
+        <v>527</v>
+      </c>
+      <c r="F29" t="s">
+        <v>890</v>
+      </c>
+      <c r="G29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" t="s">
+        <v>891</v>
+      </c>
+      <c r="I29" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" t="s">
+        <v>892</v>
+      </c>
+      <c r="O29" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9513,7 +9729,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9576,36 +9792,36 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>668</v>
+      </c>
+      <c r="B2" t="s">
+        <v>668</v>
+      </c>
+      <c r="C2" t="s">
         <v>669</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>668</v>
+      </c>
+      <c r="M2" t="s">
         <v>669</v>
-      </c>
-      <c r="C2" t="s">
-        <v>670</v>
-      </c>
-      <c r="D2" t="s">
-        <v>669</v>
-      </c>
-      <c r="M2" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>670</v>
+      </c>
+      <c r="B3" t="s">
+        <v>670</v>
+      </c>
+      <c r="C3" t="s">
+        <v>670</v>
+      </c>
+      <c r="D3" t="s">
+        <v>670</v>
+      </c>
+      <c r="M3" t="s">
         <v>671</v>
-      </c>
-      <c r="B3" t="s">
-        <v>671</v>
-      </c>
-      <c r="C3" t="s">
-        <v>671</v>
-      </c>
-      <c r="D3" t="s">
-        <v>671</v>
-      </c>
-      <c r="M3" t="s">
-        <v>672</v>
       </c>
     </row>
   </sheetData>
@@ -9615,11 +9831,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9697,16 +9913,16 @@
         <v>18</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>7</v>
@@ -9715,36 +9931,36 @@
         <v>16</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>630</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>7</v>
@@ -9753,33 +9969,33 @@
         <v>16</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>653</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>654</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>7</v>
@@ -9788,7 +10004,7 @@
         <v>16</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -9805,16 +10021,16 @@
         <v>733910060</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>7</v>
@@ -9823,36 +10039,36 @@
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>659</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>666</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>658</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>667</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>7</v>
@@ -9861,36 +10077,36 @@
         <v>16</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>664</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>665</v>
-      </c>
       <c r="G7" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>7</v>
@@ -9899,36 +10115,36 @@
         <v>16</v>
       </c>
       <c r="K7" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>662</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>636</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>635</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>637</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>7</v>
@@ -9937,36 +10153,36 @@
         <v>16</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>7</v>
@@ -9975,36 +10191,36 @@
         <v>16</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>644</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>635</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>645</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>7</v>
@@ -10013,36 +10229,36 @@
         <v>16</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>7</v>
@@ -10051,36 +10267,36 @@
         <v>16</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>7</v>
@@ -10089,36 +10305,36 @@
         <v>16</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>763</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>763</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>763</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>763</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>764</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>7</v>
@@ -10127,36 +10343,36 @@
         <v>16</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>832</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>833</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>7</v>
@@ -10165,36 +10381,36 @@
         <v>16</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>7</v>
@@ -10203,36 +10419,36 @@
         <v>16</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="10" t="s">
         <v>834</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>835</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>7</v>
@@ -10241,36 +10457,36 @@
         <v>16</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>7</v>
@@ -10279,36 +10495,36 @@
         <v>16</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>836</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>837</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>7</v>
@@ -10317,36 +10533,36 @@
         <v>16</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>7</v>
@@ -10355,36 +10571,36 @@
         <v>16</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>838</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>839</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>7</v>
@@ -10393,36 +10609,36 @@
         <v>16</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>7</v>
@@ -10431,36 +10647,36 @@
         <v>16</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>840</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>840</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>840</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>840</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>841</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>7</v>
@@ -10469,36 +10685,36 @@
         <v>16</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>7</v>
@@ -10507,36 +10723,36 @@
         <v>16</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>842</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>842</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>842</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>842</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>843</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>7</v>
@@ -10545,36 +10761,36 @@
         <v>16</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>844</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>845</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>7</v>
@@ -10583,36 +10799,36 @@
         <v>16</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>846</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>847</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>7</v>
@@ -10621,36 +10837,36 @@
         <v>16</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>7</v>
@@ -10659,36 +10875,36 @@
         <v>16</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>848</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>848</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>848</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>848</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>849</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>7</v>
@@ -10697,36 +10913,36 @@
         <v>16</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>7</v>
@@ -10735,36 +10951,36 @@
         <v>16</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>850</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>850</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>850</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>850</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>851</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>7</v>
@@ -10773,36 +10989,36 @@
         <v>16</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>7</v>
@@ -10811,36 +11027,36 @@
         <v>16</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="10" t="s">
         <v>852</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>853</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>7</v>
@@ -10849,36 +11065,36 @@
         <v>16</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>7</v>
@@ -10887,36 +11103,36 @@
         <v>16</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M33" s="10" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" s="10" t="s">
         <v>854</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>854</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>854</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>854</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>855</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>7</v>
@@ -10925,36 +11141,36 @@
         <v>16</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>7</v>
@@ -10963,36 +11179,36 @@
         <v>16</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>856</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>856</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>856</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>856</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>857</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>7</v>
@@ -11001,36 +11217,36 @@
         <v>16</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>786</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>786</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>786</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>787</v>
-      </c>
       <c r="F37" s="10" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>7</v>
@@ -11039,30 +11255,30 @@
         <v>16</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M37" s="10" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>7</v>
@@ -11071,36 +11287,36 @@
         <v>16</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B39" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" s="10" t="s">
         <v>859</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>859</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>859</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>787</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>859</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>860</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>7</v>
@@ -11109,30 +11325,30 @@
         <v>16</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>7</v>
@@ -11141,10 +11357,27 @@
         <v>16</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>831</v>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="10" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -11244,11 +11477,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11315,10 +11548,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
@@ -11332,12 +11565,17 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>722</v>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -14164,28 +14402,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2" t="s">
         <v>673</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>673</v>
+      </c>
+      <c r="D2" t="s">
+        <v>673</v>
+      </c>
+      <c r="E2" t="s">
         <v>674</v>
       </c>
-      <c r="C2" t="s">
-        <v>674</v>
-      </c>
-      <c r="D2" t="s">
-        <v>674</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>673</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>675</v>
-      </c>
-      <c r="F2" t="s">
-        <v>674</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>676</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -14194,42 +14432,42 @@
         <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L2" t="s">
+        <v>676</v>
+      </c>
+      <c r="M2" t="s">
+        <v>678</v>
+      </c>
+      <c r="N2" t="s">
         <v>677</v>
-      </c>
-      <c r="M2" t="s">
-        <v>679</v>
-      </c>
-      <c r="N2" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F3" t="s">
         <v>681</v>
       </c>
-      <c r="F3" t="s">
-        <v>682</v>
-      </c>
       <c r="G3" t="s">
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -14238,51 +14476,51 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="L3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>734</v>
+      </c>
+      <c r="B4" t="s">
+        <v>736</v>
+      </c>
+      <c r="C4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D4" t="s">
         <v>735</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>737</v>
       </c>
-      <c r="C4" t="s">
-        <v>737</v>
-      </c>
-      <c r="D4" t="s">
-        <v>736</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>735</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>738</v>
       </c>
-      <c r="F4" t="s">
-        <v>736</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
         <v>739</v>
       </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>740</v>
-      </c>
-      <c r="M4" t="s">
-        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -14360,28 +14598,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>686</v>
+      </c>
+      <c r="B2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2" t="s">
+        <v>698</v>
+      </c>
+      <c r="D2" t="s">
         <v>687</v>
       </c>
-      <c r="B2" t="s">
-        <v>699</v>
-      </c>
-      <c r="C2" t="s">
-        <v>699</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>688</v>
       </c>
-      <c r="E2" t="s">
-        <v>689</v>
-      </c>
       <c r="F2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -14390,42 +14628,42 @@
         <v>16</v>
       </c>
       <c r="K2" t="s">
+        <v>690</v>
+      </c>
+      <c r="L2" t="s">
+        <v>689</v>
+      </c>
+      <c r="M2" t="s">
         <v>691</v>
       </c>
-      <c r="L2" t="s">
-        <v>690</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>692</v>
-      </c>
-      <c r="N2" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D3" t="s">
+        <v>693</v>
+      </c>
+      <c r="E3" t="s">
+        <v>688</v>
+      </c>
+      <c r="F3" t="s">
+        <v>693</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>694</v>
-      </c>
-      <c r="E3" t="s">
-        <v>689</v>
-      </c>
-      <c r="F3" t="s">
-        <v>694</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>695</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -14434,39 +14672,39 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
+        <v>695</v>
+      </c>
+      <c r="L3" t="s">
         <v>696</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>697</v>
-      </c>
-      <c r="M3" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>700</v>
+      </c>
+      <c r="B4" t="s">
+        <v>700</v>
+      </c>
+      <c r="C4" t="s">
+        <v>700</v>
+      </c>
+      <c r="D4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E4" t="s">
+        <v>699</v>
+      </c>
+      <c r="F4" t="s">
+        <v>700</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>701</v>
-      </c>
-      <c r="B4" t="s">
-        <v>701</v>
-      </c>
-      <c r="C4" t="s">
-        <v>701</v>
-      </c>
-      <c r="D4" t="s">
-        <v>701</v>
-      </c>
-      <c r="E4" t="s">
-        <v>700</v>
-      </c>
-      <c r="F4" t="s">
-        <v>701</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>702</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -14475,16 +14713,16 @@
         <v>16</v>
       </c>
       <c r="K4" t="s">
+        <v>702</v>
+      </c>
+      <c r="L4" t="s">
         <v>703</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>704</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>705</v>
-      </c>
-      <c r="N4" t="s">
-        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -14564,84 +14802,84 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B2" t="s">
+        <v>725</v>
+      </c>
+      <c r="C2" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2" t="s">
+        <v>724</v>
+      </c>
+      <c r="E2" t="s">
         <v>726</v>
       </c>
-      <c r="C2" t="s">
-        <v>726</v>
-      </c>
-      <c r="D2" t="s">
-        <v>725</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>724</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>723</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
         <v>727</v>
       </c>
-      <c r="F2" t="s">
-        <v>725</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>724</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>753</v>
+      </c>
+      <c r="M2" t="s">
         <v>728</v>
-      </c>
-      <c r="L2" t="s">
-        <v>754</v>
-      </c>
-      <c r="M2" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B3" t="s">
+        <v>725</v>
+      </c>
+      <c r="C3" t="s">
+        <v>725</v>
+      </c>
+      <c r="D3" t="s">
+        <v>729</v>
+      </c>
+      <c r="E3" t="s">
         <v>726</v>
       </c>
-      <c r="C3" t="s">
-        <v>726</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>729</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>731</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>727</v>
+      </c>
+      <c r="L3" t="s">
+        <v>754</v>
+      </c>
+      <c r="M3" t="s">
         <v>730</v>
-      </c>
-      <c r="E3" t="s">
-        <v>727</v>
-      </c>
-      <c r="F3" t="s">
-        <v>730</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>732</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>728</v>
-      </c>
-      <c r="L3" t="s">
-        <v>755</v>
-      </c>
-      <c r="M3" t="s">
-        <v>731</v>
       </c>
     </row>
   </sheetData>
@@ -14721,29 +14959,29 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D2" t="s">
+        <v>732</v>
+      </c>
+      <c r="E2" t="s">
+        <v>707</v>
+      </c>
+      <c r="F2" t="s">
+        <v>732</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
         <v>733</v>
       </c>
-      <c r="E2" t="s">
-        <v>708</v>
-      </c>
-      <c r="F2" t="s">
-        <v>733</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>734</v>
-      </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
@@ -14751,81 +14989,81 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="L2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="M2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D3" t="s">
+        <v>748</v>
+      </c>
+      <c r="E3" t="s">
+        <v>707</v>
+      </c>
+      <c r="F3" t="s">
+        <v>748</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>749</v>
       </c>
-      <c r="E3" t="s">
-        <v>708</v>
-      </c>
-      <c r="F3" t="s">
-        <v>749</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
         <v>750</v>
       </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>755</v>
+      </c>
+      <c r="M3" t="s">
         <v>751</v>
-      </c>
-      <c r="L3" t="s">
-        <v>756</v>
-      </c>
-      <c r="M3" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D4" t="s">
+        <v>741</v>
+      </c>
+      <c r="E4" t="s">
+        <v>707</v>
+      </c>
+      <c r="F4" t="s">
+        <v>741</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>742</v>
       </c>
-      <c r="E4" t="s">
-        <v>708</v>
-      </c>
-      <c r="F4" t="s">
-        <v>742</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>743</v>
-      </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
@@ -14833,40 +15071,40 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="M4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D5" t="s">
+        <v>743</v>
+      </c>
+      <c r="E5" t="s">
+        <v>707</v>
+      </c>
+      <c r="F5" t="s">
+        <v>743</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
         <v>744</v>
       </c>
-      <c r="E5" t="s">
-        <v>708</v>
-      </c>
-      <c r="F5" t="s">
-        <v>744</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>745</v>
-      </c>
       <c r="I5" t="s">
         <v>7</v>
       </c>
@@ -14874,13 +15112,13 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="L5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="M5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -14959,47 +15197,47 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D2" t="s">
+        <v>706</v>
+      </c>
+      <c r="E2" t="s">
+        <v>707</v>
+      </c>
+      <c r="F2" t="s">
+        <v>706</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>708</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
         <v>710</v>
-      </c>
-      <c r="C2" t="s">
-        <v>710</v>
-      </c>
-      <c r="D2" t="s">
-        <v>707</v>
-      </c>
-      <c r="E2" t="s">
-        <v>708</v>
-      </c>
-      <c r="F2" t="s">
-        <v>707</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>709</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix mounting holes and solder pads
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FFECD5-D914-49B5-BAC4-C704291E019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFF8173-5A19-498E-81C6-2EC6CE9B5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -3866,7 +3866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D232E866-2FB1-4CC1-9431-42BF8C928F34}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
@@ -13720,9 +13720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15451,7 +15451,7 @@
         <v>899</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.4">
@@ -15480,7 +15480,7 @@
         <v>947</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.4">
@@ -15509,7 +15509,7 @@
         <v>947</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -16108,7 +16108,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Fix a couple footprints, add GC9A01
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFF8173-5A19-498E-81C6-2EC6CE9B5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE3CCB3-437B-48A7-9380-AB80360B9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4318" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4331" uniqueCount="997">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3029,6 +3029,18 @@
   </si>
   <si>
     <t>Mounting_Hole_Plated</t>
+  </si>
+  <si>
+    <t>GC9A01</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>240x240 px round IPS display</t>
   </si>
 </sst>
 </file>
@@ -4657,11 +4669,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4677,7 +4689,7 @@
     <col min="10" max="10" width="12.53515625" customWidth="1"/>
     <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.3828125" customWidth="1"/>
-    <col min="13" max="13" width="23.921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.84375" customWidth="1"/>
     <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4811,6 +4823,47 @@
         <v>898</v>
       </c>
       <c r="O6" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>993</v>
+      </c>
+      <c r="B7" t="s">
+        <v>993</v>
+      </c>
+      <c r="C7" t="s">
+        <v>993</v>
+      </c>
+      <c r="D7" t="s">
+        <v>993</v>
+      </c>
+      <c r="E7" t="s">
+        <v>994</v>
+      </c>
+      <c r="F7" t="s">
+        <v>993</v>
+      </c>
+      <c r="G7" t="s">
+        <v>994</v>
+      </c>
+      <c r="H7" t="s">
+        <v>994</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>995</v>
+      </c>
+      <c r="M7" t="s">
+        <v>996</v>
+      </c>
+      <c r="O7" t="s">
         <v>902</v>
       </c>
     </row>
@@ -13720,7 +13773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
     </sheetView>

</xml_diff>

<commit_message>
Add generic resistor footprints
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE3CCB3-437B-48A7-9380-AB80360B9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AA0D9A-ECED-40C3-B169-898E01472514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4331" uniqueCount="997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4379" uniqueCount="1006">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3041,6 +3041,33 @@
   </si>
   <si>
     <t>240x240 px round IPS display</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>Generic resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>General purpose resistor</t>
+  </si>
+  <si>
+    <t>Generic 0402 resistor</t>
+  </si>
+  <si>
+    <t>Generic 0603 resistor</t>
+  </si>
+  <si>
+    <t>Generic 0805 resistor</t>
+  </si>
+  <si>
+    <t>Generic 1206 resistor</t>
   </si>
 </sst>
 </file>
@@ -4671,7 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
@@ -4956,11 +4983,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O127"/>
+  <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E128" sqref="E128"/>
+      <selection pane="bottomLeft" activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -10571,6 +10598,158 @@
       </c>
       <c r="O127" t="s">
         <v>901</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>51</v>
+      </c>
+      <c r="B128" t="s">
+        <v>997</v>
+      </c>
+      <c r="C128" t="s">
+        <v>997</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E128" t="s">
+        <v>994</v>
+      </c>
+      <c r="F128" t="s">
+        <v>999</v>
+      </c>
+      <c r="G128" t="s">
+        <v>994</v>
+      </c>
+      <c r="H128" t="s">
+        <v>994</v>
+      </c>
+      <c r="I128" t="s">
+        <v>7</v>
+      </c>
+      <c r="J128" t="s">
+        <v>8</v>
+      </c>
+      <c r="L128" t="s">
+        <v>1000</v>
+      </c>
+      <c r="M128" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
+        <v>51</v>
+      </c>
+      <c r="B129" t="s">
+        <v>46</v>
+      </c>
+      <c r="C129" t="s">
+        <v>46</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E129" t="s">
+        <v>994</v>
+      </c>
+      <c r="F129" t="s">
+        <v>999</v>
+      </c>
+      <c r="G129" t="s">
+        <v>994</v>
+      </c>
+      <c r="H129" t="s">
+        <v>994</v>
+      </c>
+      <c r="I129" t="s">
+        <v>7</v>
+      </c>
+      <c r="J129" t="s">
+        <v>8</v>
+      </c>
+      <c r="L129" t="s">
+        <v>1000</v>
+      </c>
+      <c r="M129" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>51</v>
+      </c>
+      <c r="B130" t="s">
+        <v>209</v>
+      </c>
+      <c r="C130" t="s">
+        <v>209</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E130" t="s">
+        <v>994</v>
+      </c>
+      <c r="F130" t="s">
+        <v>999</v>
+      </c>
+      <c r="G130" t="s">
+        <v>994</v>
+      </c>
+      <c r="H130" t="s">
+        <v>994</v>
+      </c>
+      <c r="I130" t="s">
+        <v>7</v>
+      </c>
+      <c r="J130" t="s">
+        <v>8</v>
+      </c>
+      <c r="L130" t="s">
+        <v>1000</v>
+      </c>
+      <c r="M130" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>51</v>
+      </c>
+      <c r="B131" t="s">
+        <v>998</v>
+      </c>
+      <c r="C131" t="s">
+        <v>998</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E131" t="s">
+        <v>994</v>
+      </c>
+      <c r="F131" t="s">
+        <v>999</v>
+      </c>
+      <c r="G131" t="s">
+        <v>994</v>
+      </c>
+      <c r="H131" t="s">
+        <v>994</v>
+      </c>
+      <c r="I131" t="s">
+        <v>7</v>
+      </c>
+      <c r="J131" t="s">
+        <v>8</v>
+      </c>
+      <c r="L131" t="s">
+        <v>1000</v>
+      </c>
+      <c r="M131" t="s">
+        <v>1001</v>
       </c>
     </row>
   </sheetData>
@@ -17438,7 +17617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add generic USB type A/B schematic symbol
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2246381-F9BD-4FB4-9D56-6978FE6D9F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBBA7EB-47D9-4886-B8C6-38DEC10F8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4471" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1024">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3113,6 +3113,15 @@
   </si>
   <si>
     <t>Omron Electronics</t>
+  </si>
+  <si>
+    <t>USB_A_B</t>
+  </si>
+  <si>
+    <t>USB_A_PCB</t>
+  </si>
+  <si>
+    <t>Male USB type A connector for direct PCB insertion</t>
   </si>
 </sst>
 </file>
@@ -14183,11 +14192,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O46" sqref="O46"/>
+      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14203,7 +14212,7 @@
     <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="6"/>
@@ -16001,6 +16010,35 @@
       </c>
       <c r="O45" s="6" t="s">
         <v>901</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>1023</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -16358,7 +16396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7899ABE3-AB54-4DD4-A705-E31575AC0031}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>

</xml_diff>

<commit_message>
Add USB type A PCB footprint, change ICSP header
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBBA7EB-47D9-4886-B8C6-38DEC10F8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7351D39-1E0A-4349-9A0D-2E296EC71288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1025">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3097,12 +3097,6 @@
     <t>8-bit AVR microcontroller</t>
   </si>
   <si>
-    <t>ICSP_2x6_header</t>
-  </si>
-  <si>
-    <t>2x6 pin 2.54 mm header for Arduino ICSP</t>
-  </si>
-  <si>
     <t>B3SN-3112P</t>
   </si>
   <si>
@@ -3122,6 +3116,15 @@
   </si>
   <si>
     <t>Male USB type A connector for direct PCB insertion</t>
+  </si>
+  <si>
+    <t>ICSP</t>
+  </si>
+  <si>
+    <t>ICSP_2x3_header</t>
+  </si>
+  <si>
+    <t>2x3 pin 2.54 mm header for Arduino ICSP</t>
   </si>
 </sst>
 </file>
@@ -3512,24 +3515,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15234375" customWidth="1"/>
+    <col min="14" max="14" width="13.53515625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3579,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>902</v>
       </c>
@@ -3595,24 +3598,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.53515625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3662,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>919</v>
       </c>
@@ -3697,7 +3700,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>919</v>
       </c>
@@ -3739,24 +3742,24 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -3879,7 +3882,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>759</v>
       </c>
@@ -3917,7 +3920,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>894</v>
       </c>
@@ -3964,23 +3967,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" customWidth="1"/>
+    <col min="3" max="4" width="20.84375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.69140625" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4027,7 +4030,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>668</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>991</v>
       </c>
@@ -4076,7 +4079,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>991</v>
       </c>
@@ -4105,7 +4108,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>991</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>991</v>
       </c>
@@ -4163,7 +4166,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>991</v>
       </c>
@@ -4192,7 +4195,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>991</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>991</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>991</v>
       </c>
@@ -4279,7 +4282,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>991</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>991</v>
       </c>
@@ -4337,7 +4340,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>991</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>991</v>
       </c>
@@ -4395,7 +4398,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>992</v>
       </c>
@@ -4424,7 +4427,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>992</v>
       </c>
@@ -4453,7 +4456,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>992</v>
       </c>
@@ -4482,7 +4485,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>992</v>
       </c>
@@ -4511,7 +4514,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>992</v>
       </c>
@@ -4540,7 +4543,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>992</v>
       </c>
@@ -4569,7 +4572,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>992</v>
       </c>
@@ -4598,7 +4601,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>992</v>
       </c>
@@ -4627,7 +4630,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>992</v>
       </c>
@@ -4656,7 +4659,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>992</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>992</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>992</v>
       </c>
@@ -4757,25 +4760,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>930</v>
       </c>
@@ -4863,7 +4866,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>717</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>718</v>
       </c>
@@ -4891,7 +4894,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>719</v>
       </c>
@@ -4899,7 +4902,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>898</v>
       </c>
@@ -4907,7 +4910,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>993</v>
       </c>
@@ -4962,23 +4965,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" customWidth="1"/>
+    <col min="14" max="14" width="12.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5025,7 +5028,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>902</v>
       </c>
@@ -5044,26 +5047,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="14.3046875" customWidth="1"/>
+    <col min="6" max="6" width="21.3828125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.15234375" customWidth="1"/>
+    <col min="9" max="9" width="9.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="39.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.3046875" customWidth="1"/>
+    <col min="14" max="14" width="23.15234375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5110,7 +5113,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -5154,7 +5157,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -5198,7 +5201,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -5242,7 +5245,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5286,7 +5289,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -5330,7 +5333,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5374,7 +5377,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5462,7 +5465,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -5506,7 +5509,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -5550,7 +5553,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -5594,7 +5597,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -5638,7 +5641,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5682,7 +5685,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -5770,7 +5773,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -5814,7 +5817,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -5902,7 +5905,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -5946,7 +5949,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -5990,7 +5993,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6034,7 +6037,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -6078,7 +6081,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -6122,7 +6125,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6210,7 +6213,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -6254,7 +6257,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -6298,7 +6301,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -6342,7 +6345,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -6386,7 +6389,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -6430,7 +6433,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -6518,7 +6521,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -6562,7 +6565,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -6606,7 +6609,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -6650,7 +6653,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -6694,7 +6697,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -6738,7 +6741,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -6782,7 +6785,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -6826,7 +6829,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -6870,7 +6873,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -6914,7 +6917,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7002,7 +7005,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7046,7 +7049,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -7090,7 +7093,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7134,7 +7137,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -7178,7 +7181,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -7222,7 +7225,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -7266,7 +7269,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -7310,7 +7313,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -7354,7 +7357,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7398,7 +7401,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -7442,7 +7445,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -7486,7 +7489,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -7530,7 +7533,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -7574,7 +7577,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -7618,7 +7621,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -7662,7 +7665,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -7706,7 +7709,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -7750,7 +7753,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -7794,7 +7797,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -7838,7 +7841,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -7882,7 +7885,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -7926,7 +7929,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -7970,7 +7973,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8014,7 +8017,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -8058,7 +8061,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -8102,7 +8105,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -8146,7 +8149,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -8190,7 +8193,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -8234,7 +8237,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -8278,7 +8281,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -8322,7 +8325,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -8366,7 +8369,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -8410,7 +8413,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -8454,7 +8457,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -8498,7 +8501,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -8542,7 +8545,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -8586,7 +8589,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -8630,7 +8633,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -8674,7 +8677,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -8718,7 +8721,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -8762,7 +8765,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -8806,7 +8809,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -8850,7 +8853,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -8894,7 +8897,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -8938,7 +8941,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -8982,7 +8985,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9026,7 +9029,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -9070,7 +9073,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -9114,7 +9117,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -9158,7 +9161,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -9202,7 +9205,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -9246,7 +9249,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -9290,7 +9293,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -9334,7 +9337,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -9378,7 +9381,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -9422,7 +9425,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -9466,7 +9469,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -9510,7 +9513,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -9554,7 +9557,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -9598,7 +9601,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -9642,7 +9645,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -9686,7 +9689,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -9730,7 +9733,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -9774,7 +9777,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -9818,7 +9821,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -9862,7 +9865,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -9906,7 +9909,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -9950,7 +9953,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -9994,7 +9997,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10038,7 +10041,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -10082,7 +10085,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -10126,7 +10129,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -10170,7 +10173,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -10214,7 +10217,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -10258,7 +10261,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -10302,7 +10305,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -10346,7 +10349,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -10390,7 +10393,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -10434,7 +10437,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -10478,7 +10481,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -10522,7 +10525,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -10566,7 +10569,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -10610,7 +10613,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -10654,7 +10657,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -10695,7 +10698,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -10736,7 +10739,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -10834,25 +10837,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3828125" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10899,7 +10902,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>712</v>
       </c>
@@ -10943,7 +10946,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>713</v>
       </c>
@@ -11002,24 +11005,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.53515625" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11066,7 +11069,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>714</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>714</v>
       </c>
@@ -11154,7 +11157,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>715</v>
       </c>
@@ -11198,7 +11201,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>715</v>
       </c>
@@ -11256,26 +11259,26 @@
       <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" customWidth="1"/>
+    <col min="6" max="6" width="25.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3046875" customWidth="1"/>
+    <col min="8" max="8" width="19.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.84375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11325,7 +11328,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -11372,7 +11375,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -11419,7 +11422,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -11466,7 +11469,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -11513,7 +11516,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -11560,7 +11563,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -11607,7 +11610,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -11654,7 +11657,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -11701,7 +11704,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -11748,7 +11751,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -11795,7 +11798,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -11842,7 +11845,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -11889,7 +11892,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -11936,7 +11939,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -11983,7 +11986,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12030,7 +12033,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -12077,7 +12080,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -12124,7 +12127,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -12171,7 +12174,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -12218,7 +12221,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -12265,7 +12268,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -12312,7 +12315,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -12359,7 +12362,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -12406,7 +12409,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -12453,7 +12456,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -12500,7 +12503,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -12547,7 +12550,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -12594,7 +12597,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -12641,7 +12644,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -12688,7 +12691,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -12735,7 +12738,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -12782,7 +12785,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -12829,7 +12832,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -12876,7 +12879,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -12923,7 +12926,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -12970,7 +12973,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13017,7 +13020,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -13064,7 +13067,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -13114,7 +13117,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -13161,7 +13164,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -13208,7 +13211,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -13255,7 +13258,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -13302,7 +13305,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -13349,7 +13352,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -13396,7 +13399,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -13443,7 +13446,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -13490,7 +13493,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -13537,7 +13540,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -13584,7 +13587,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -13631,7 +13634,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -13678,7 +13681,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -13725,7 +13728,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -13772,7 +13775,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -13819,7 +13822,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -13866,7 +13869,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -13913,7 +13916,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -13960,7 +13963,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14007,7 +14010,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -14051,7 +14054,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -14095,7 +14098,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -14139,7 +14142,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -14195,30 +14198,30 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="6"/>
+    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14265,7 +14268,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -14306,7 +14309,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>628</v>
       </c>
@@ -14344,7 +14347,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>652</v>
       </c>
@@ -14382,7 +14385,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -14423,7 +14426,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>665</v>
       </c>
@@ -14464,7 +14467,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>664</v>
       </c>
@@ -14505,7 +14508,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>785</v>
       </c>
@@ -14546,7 +14549,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>786</v>
       </c>
@@ -14587,7 +14590,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>787</v>
       </c>
@@ -14628,7 +14631,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>788</v>
       </c>
@@ -14669,7 +14672,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>786</v>
       </c>
@@ -14710,7 +14713,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>785</v>
       </c>
@@ -14751,7 +14754,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>805</v>
       </c>
@@ -14792,7 +14795,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>786</v>
       </c>
@@ -14833,7 +14836,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>806</v>
       </c>
@@ -14874,7 +14877,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>787</v>
       </c>
@@ -14915,7 +14918,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>807</v>
       </c>
@@ -14956,7 +14959,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>788</v>
       </c>
@@ -14997,7 +15000,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>808</v>
       </c>
@@ -15038,7 +15041,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>789</v>
       </c>
@@ -15079,7 +15082,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>809</v>
       </c>
@@ -15120,7 +15123,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>790</v>
       </c>
@@ -15161,7 +15164,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>810</v>
       </c>
@@ -15202,7 +15205,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>811</v>
       </c>
@@ -15243,7 +15246,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>812</v>
       </c>
@@ -15284,7 +15287,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>785</v>
       </c>
@@ -15325,7 +15328,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>805</v>
       </c>
@@ -15366,7 +15369,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>786</v>
       </c>
@@ -15407,7 +15410,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>806</v>
       </c>
@@ -15448,7 +15451,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>787</v>
       </c>
@@ -15489,7 +15492,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>807</v>
       </c>
@@ -15530,7 +15533,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>788</v>
       </c>
@@ -15571,7 +15574,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>808</v>
       </c>
@@ -15612,7 +15615,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>789</v>
       </c>
@@ -15653,7 +15656,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>809</v>
       </c>
@@ -15694,7 +15697,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>790</v>
       </c>
@@ -15735,7 +15738,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>810</v>
       </c>
@@ -15770,7 +15773,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>811</v>
       </c>
@@ -15811,7 +15814,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>812</v>
       </c>
@@ -15846,7 +15849,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>805</v>
       </c>
@@ -15887,7 +15890,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>805</v>
       </c>
@@ -15928,7 +15931,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>786</v>
       </c>
@@ -15957,7 +15960,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>788</v>
       </c>
@@ -15986,18 +15989,18 @@
         <v>901</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
-        <v>787</v>
+        <v>1022</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>7</v>
@@ -16006,27 +16009,27 @@
         <v>8</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>1016</v>
+        <v>1024</v>
       </c>
       <c r="O45" s="6" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>7</v>
@@ -16035,10 +16038,10 @@
         <v>16</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -16060,23 +16063,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16123,7 +16126,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>684</v>
       </c>
@@ -16170,7 +16173,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>684</v>
       </c>
@@ -16214,7 +16217,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>698</v>
       </c>
@@ -16275,24 +16278,24 @@
       <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.69140625" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16339,7 +16342,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>709</v>
       </c>
@@ -16377,12 +16380,12 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>711</v>
       </c>
@@ -16401,23 +16404,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16464,7 +16467,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>914</v>
       </c>
@@ -16502,30 +16505,30 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>914</v>
       </c>
       <c r="B3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="E3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="F3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="G3" t="s">
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -16534,7 +16537,7 @@
         <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="O3" t="s">
         <v>901</v>
@@ -16554,26 +16557,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16620,7 +16623,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -16678,26 +16681,26 @@
       <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" customWidth="1"/>
+    <col min="10" max="10" width="12.15234375" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.53515625" customWidth="1"/>
+    <col min="15" max="15" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16747,7 +16750,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -16788,7 +16791,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>514</v>
       </c>
@@ -16829,7 +16832,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>515</v>
       </c>
@@ -16873,7 +16876,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>547</v>
       </c>
@@ -16914,7 +16917,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>548</v>
       </c>
@@ -16955,7 +16958,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>516</v>
       </c>
@@ -16996,7 +16999,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>517</v>
       </c>
@@ -17037,7 +17040,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>518</v>
       </c>
@@ -17078,7 +17081,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>523</v>
       </c>
@@ -17119,7 +17122,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>522</v>
       </c>
@@ -17160,7 +17163,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>556</v>
       </c>
@@ -17201,7 +17204,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>559</v>
       </c>
@@ -17242,7 +17245,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>569</v>
       </c>
@@ -17283,7 +17286,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>573</v>
       </c>
@@ -17324,7 +17327,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>574</v>
       </c>
@@ -17365,7 +17368,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>582</v>
       </c>
@@ -17406,7 +17409,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>588</v>
       </c>
@@ -17447,7 +17450,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>591</v>
       </c>
@@ -17488,7 +17491,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>601</v>
       </c>
@@ -17529,7 +17532,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>606</v>
       </c>
@@ -17570,7 +17573,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>614</v>
       </c>
@@ -17611,7 +17614,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>612</v>
       </c>
@@ -17652,7 +17655,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>859</v>
       </c>
@@ -17693,7 +17696,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>866</v>
       </c>
@@ -17734,7 +17737,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>873</v>
       </c>
@@ -17775,7 +17778,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>880</v>
       </c>
@@ -17816,7 +17819,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>892</v>
       </c>
@@ -17857,7 +17860,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>893</v>
       </c>
@@ -17898,7 +17901,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>936</v>
       </c>
@@ -17939,7 +17942,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>1013</v>
       </c>
@@ -17993,25 +17996,25 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18058,7 +18061,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>670</v>
       </c>
@@ -18105,7 +18108,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>670</v>
       </c>
@@ -18149,7 +18152,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>732</v>
       </c>

</xml_diff>

<commit_message>
Add red and green 1206 LEDs
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7351D39-1E0A-4349-9A0D-2E296EC71288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B52622F-1991-4998-98FC-825CC0F849AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="1030">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3125,6 +3125,21 @@
   </si>
   <si>
     <t>2x3 pin 2.54 mm header for Arduino ICSP</t>
+  </si>
+  <si>
+    <t>LED_1206</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Green 1206 LED</t>
+  </si>
+  <si>
+    <t>Red 1206 LED</t>
   </si>
 </sst>
 </file>
@@ -4753,11 +4768,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4949,6 +4964,64 @@
       </c>
       <c r="O7" t="s">
         <v>902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1026</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1029</v>
+      </c>
+      <c r="O8" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>718</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="O9" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -14197,7 +14270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>

</xml_diff>

<commit_message>
Add 6 pin FTDI connector
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E9A2C3-AC30-42B0-9275-C2DCFC28CE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589E54F7-627E-4349-9197-42697132C123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4511" uniqueCount="1037">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3146,6 +3146,21 @@
   </si>
   <si>
     <t>LED_GREEN_1206</t>
+  </si>
+  <si>
+    <t>2.54mm_1x6_header_horizontal_male</t>
+  </si>
+  <si>
+    <t>Horizontal edge mount 1x6 2.54 mm header</t>
+  </si>
+  <si>
+    <t>61300611121</t>
+  </si>
+  <si>
+    <t>732-5319-ND</t>
+  </si>
+  <si>
+    <t>61300611121_horizontal</t>
   </si>
 </sst>
 </file>
@@ -4776,7 +4791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49CCDDC-BCD9-4891-957C-29E1B55323F5}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
@@ -14274,11 +14289,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -16120,6 +16135,47 @@
         <v>1021</v>
       </c>
       <c r="O46" s="6" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A47" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>951</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="O47" s="6" t="s">
         <v>901</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix incorrect name on 2.54mm_1x6_header_horizontal_male
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3533BF-A76D-406F-AD26-A4A9F02176DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA9B96-FB91-44CB-A5C2-42B4FDE84C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3154,9 +3154,6 @@
     <t>40V, 1A</t>
   </si>
   <si>
-    <t>2.54mm_1x6_header_horizontal</t>
-  </si>
-  <si>
     <t>61300611121</t>
   </si>
   <si>
@@ -3170,6 +3167,9 @@
   </si>
   <si>
     <t>2x3 pin 2.54 mm header for Arduino ICSP</t>
+  </si>
+  <si>
+    <t>2.54mm_1x6_header_horizontal_male</t>
   </si>
 </sst>
 </file>
@@ -14244,7 +14244,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M46" sqref="M46"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16039,22 +16039,22 @@
         <v>786</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>1038</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>1038</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>1039</v>
       </c>
       <c r="O45" s="6" t="s">
         <v>900</v>
@@ -16094,25 +16094,25 @@
         <v>786</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>947</v>
       </c>
       <c r="F47" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" s="6" t="s">
         <v>1035</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>1036</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>7</v>
@@ -16124,7 +16124,7 @@
         <v>950</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="O47" s="6" t="s">
         <v>900</v>

</xml_diff>

<commit_message>
Add TL072 schematic library
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63310EA2-940B-4E0A-AEC4-7DDB0D8A59C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C3003C-4B05-4F54-A460-D48224217EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16809,7 +16809,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17701,7 +17701,7 @@
         <v>597</v>
       </c>
       <c r="P21" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix ATTINY45, add MCP1501
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA9B96-FB91-44CB-A5C2-42B4FDE84C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD62ADD8-1313-431F-931A-52C1C44EDA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4531" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="1074">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3170,6 +3170,108 @@
   </si>
   <si>
     <t>2.54mm_1x6_header_horizontal_male</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>MCP151T-20E/CHY</t>
+  </si>
+  <si>
+    <t>MCP1501</t>
+  </si>
+  <si>
+    <t>MCP1501T-20E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>Voltage Reference</t>
+  </si>
+  <si>
+    <t>2.048 V Voltage reference</t>
+  </si>
+  <si>
+    <t>MCP151T-10E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-12E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-18E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-25E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-30E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-33E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-40E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-45E/CHY</t>
+  </si>
+  <si>
+    <t>MCP151T-50E/CHY</t>
+  </si>
+  <si>
+    <t>MCP1501T-10E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-12E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-18E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-25E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-30E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-33E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1501T-40E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>150-MCP1501T-45E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>150-MCP1501T-50E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>1.024 V Voltage reference</t>
+  </si>
+  <si>
+    <t>1.250 V Voltage reference</t>
+  </si>
+  <si>
+    <t>1.800 V Voltage reference</t>
+  </si>
+  <si>
+    <t>2.500 V Voltage reference</t>
+  </si>
+  <si>
+    <t>3.000 V Voltage reference</t>
+  </si>
+  <si>
+    <t>3.300 V Voltage reference</t>
+  </si>
+  <si>
+    <t>4.096 V Voltage reference</t>
+  </si>
+  <si>
+    <t>4.500 V Voltage reference</t>
+  </si>
+  <si>
+    <t>5.000 V Voltage reference</t>
+  </si>
+  <si>
+    <t>MCP1501x-xx/CHY</t>
   </si>
 </sst>
 </file>
@@ -3560,24 +3662,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15234375" customWidth="1"/>
+    <col min="14" max="14" width="13.53515625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3624,7 +3726,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -3643,24 +3745,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.53515625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3707,7 +3809,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>918</v>
       </c>
@@ -3745,7 +3847,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>918</v>
       </c>
@@ -3787,24 +3889,24 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3953,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -3889,7 +3991,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -3927,7 +4029,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>758</v>
       </c>
@@ -3965,7 +4067,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>893</v>
       </c>
@@ -4012,23 +4114,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" customWidth="1"/>
+    <col min="3" max="4" width="20.84375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.69140625" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4075,7 +4177,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>667</v>
       </c>
@@ -4095,7 +4197,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>990</v>
       </c>
@@ -4124,7 +4226,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>990</v>
       </c>
@@ -4153,7 +4255,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>990</v>
       </c>
@@ -4182,7 +4284,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>990</v>
       </c>
@@ -4211,7 +4313,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>990</v>
       </c>
@@ -4240,7 +4342,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>990</v>
       </c>
@@ -4269,7 +4371,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>990</v>
       </c>
@@ -4298,7 +4400,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>990</v>
       </c>
@@ -4327,7 +4429,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>990</v>
       </c>
@@ -4356,7 +4458,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>990</v>
       </c>
@@ -4385,7 +4487,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>990</v>
       </c>
@@ -4414,7 +4516,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>990</v>
       </c>
@@ -4443,7 +4545,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>991</v>
       </c>
@@ -4472,7 +4574,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>991</v>
       </c>
@@ -4501,7 +4603,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>991</v>
       </c>
@@ -4530,7 +4632,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>991</v>
       </c>
@@ -4559,7 +4661,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>991</v>
       </c>
@@ -4588,7 +4690,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>991</v>
       </c>
@@ -4617,7 +4719,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>991</v>
       </c>
@@ -4646,7 +4748,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>991</v>
       </c>
@@ -4675,7 +4777,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>991</v>
       </c>
@@ -4704,7 +4806,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>991</v>
       </c>
@@ -4733,7 +4835,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>991</v>
       </c>
@@ -4762,7 +4864,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>991</v>
       </c>
@@ -4805,25 +4907,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4870,7 +4972,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>929</v>
       </c>
@@ -4911,7 +5013,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>716</v>
       </c>
@@ -4931,7 +5033,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>717</v>
       </c>
@@ -4939,7 +5041,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>718</v>
       </c>
@@ -4947,7 +5049,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>897</v>
       </c>
@@ -4955,7 +5057,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>992</v>
       </c>
@@ -5010,23 +5112,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" customWidth="1"/>
+    <col min="14" max="14" width="12.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5073,7 +5175,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -5092,26 +5194,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="14.3046875" customWidth="1"/>
+    <col min="6" max="6" width="21.3828125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.15234375" customWidth="1"/>
+    <col min="9" max="9" width="9.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="39.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.3046875" customWidth="1"/>
+    <col min="14" max="14" width="23.15234375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5158,7 +5260,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -5202,7 +5304,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -5246,7 +5348,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -5290,7 +5392,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5334,7 +5436,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -5378,7 +5480,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5422,7 +5524,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -5466,7 +5568,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5510,7 +5612,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -5554,7 +5656,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -5598,7 +5700,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -5642,7 +5744,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -5686,7 +5788,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5730,7 +5832,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -5774,7 +5876,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -5818,7 +5920,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -5862,7 +5964,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -5906,7 +6008,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -5950,7 +6052,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -5994,7 +6096,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -6038,7 +6140,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6082,7 +6184,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -6126,7 +6228,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -6170,7 +6272,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -6214,7 +6316,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6258,7 +6360,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -6302,7 +6404,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -6346,7 +6448,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -6390,7 +6492,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -6434,7 +6536,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -6478,7 +6580,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -6522,7 +6624,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -6566,7 +6668,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -6610,7 +6712,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -6654,7 +6756,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -6698,7 +6800,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -6742,7 +6844,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -6786,7 +6888,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -6830,7 +6932,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -6874,7 +6976,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -6918,7 +7020,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -6962,7 +7064,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -7006,7 +7108,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7050,7 +7152,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7094,7 +7196,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -7138,7 +7240,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7182,7 +7284,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -7226,7 +7328,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -7270,7 +7372,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -7314,7 +7416,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -7358,7 +7460,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -7402,7 +7504,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7446,7 +7548,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -7490,7 +7592,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -7534,7 +7636,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -7578,7 +7680,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -7622,7 +7724,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -7666,7 +7768,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -7710,7 +7812,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -7754,7 +7856,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -7798,7 +7900,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -7842,7 +7944,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -7886,7 +7988,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -7930,7 +8032,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -7974,7 +8076,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -8018,7 +8120,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8062,7 +8164,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -8106,7 +8208,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -8150,7 +8252,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -8194,7 +8296,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -8238,7 +8340,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -8282,7 +8384,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -8326,7 +8428,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -8370,7 +8472,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -8414,7 +8516,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -8458,7 +8560,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -8502,7 +8604,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -8546,7 +8648,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -8590,7 +8692,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -8634,7 +8736,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -8678,7 +8780,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -8722,7 +8824,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -8766,7 +8868,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -8810,7 +8912,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -8854,7 +8956,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -8898,7 +9000,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -8942,7 +9044,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -8986,7 +9088,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -9030,7 +9132,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9074,7 +9176,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -9118,7 +9220,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -9162,7 +9264,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -9206,7 +9308,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -9250,7 +9352,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -9294,7 +9396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -9338,7 +9440,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -9382,7 +9484,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -9426,7 +9528,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -9470,7 +9572,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -9514,7 +9616,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -9558,7 +9660,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -9602,7 +9704,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -9646,7 +9748,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -9690,7 +9792,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -9734,7 +9836,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -9778,7 +9880,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -9822,7 +9924,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -9866,7 +9968,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -9910,7 +10012,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -9954,7 +10056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -9998,7 +10100,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -10042,7 +10144,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10086,7 +10188,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -10130,7 +10232,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -10174,7 +10276,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -10218,7 +10320,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -10262,7 +10364,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -10306,7 +10408,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -10350,7 +10452,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -10394,7 +10496,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -10438,7 +10540,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -10482,7 +10584,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -10526,7 +10628,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -10570,7 +10672,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -10614,7 +10716,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -10658,7 +10760,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -10702,7 +10804,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -10743,7 +10845,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -10784,7 +10886,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -10825,7 +10927,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -10882,25 +10984,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3828125" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10947,7 +11049,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>711</v>
       </c>
@@ -10991,7 +11093,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -11050,24 +11152,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.53515625" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11114,7 +11216,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>713</v>
       </c>
@@ -11158,7 +11260,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>713</v>
       </c>
@@ -11202,7 +11304,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>714</v>
       </c>
@@ -11246,7 +11348,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>714</v>
       </c>
@@ -11304,26 +11406,26 @@
       <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" customWidth="1"/>
+    <col min="6" max="6" width="25.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3046875" customWidth="1"/>
+    <col min="8" max="8" width="19.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.84375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11373,7 +11475,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -11420,7 +11522,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -11467,7 +11569,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -11514,7 +11616,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -11561,7 +11663,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -11608,7 +11710,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -11655,7 +11757,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -11702,7 +11804,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -11749,7 +11851,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -11796,7 +11898,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -11843,7 +11945,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -11890,7 +11992,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -11937,7 +12039,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -11984,7 +12086,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -12031,7 +12133,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12078,7 +12180,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -12125,7 +12227,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -12172,7 +12274,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -12219,7 +12321,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -12266,7 +12368,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -12313,7 +12415,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -12360,7 +12462,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -12407,7 +12509,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -12454,7 +12556,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -12501,7 +12603,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -12548,7 +12650,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -12595,7 +12697,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -12642,7 +12744,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -12689,7 +12791,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -12736,7 +12838,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -12783,7 +12885,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -12830,7 +12932,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -12877,7 +12979,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -12924,7 +13026,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -12971,7 +13073,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -13018,7 +13120,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13065,7 +13167,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -13112,7 +13214,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -13162,7 +13264,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -13209,7 +13311,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -13256,7 +13358,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -13303,7 +13405,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -13350,7 +13452,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -13397,7 +13499,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -13444,7 +13546,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -13491,7 +13593,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -13538,7 +13640,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -13585,7 +13687,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -13632,7 +13734,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -13679,7 +13781,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -13726,7 +13828,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -13773,7 +13875,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -13820,7 +13922,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -13867,7 +13969,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -13914,7 +14016,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -13961,7 +14063,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -14008,7 +14110,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14055,7 +14157,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -14099,7 +14201,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -14143,7 +14245,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -14187,7 +14289,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -14242,31 +14344,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="6"/>
+    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14313,7 +14415,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -14354,7 +14456,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -14392,7 +14494,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>651</v>
       </c>
@@ -14430,7 +14532,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -14471,7 +14573,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>664</v>
       </c>
@@ -14512,7 +14614,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>663</v>
       </c>
@@ -14553,7 +14655,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -14594,7 +14696,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>785</v>
       </c>
@@ -14635,7 +14737,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>786</v>
       </c>
@@ -14676,7 +14778,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>787</v>
       </c>
@@ -14717,7 +14819,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>785</v>
       </c>
@@ -14758,7 +14860,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>784</v>
       </c>
@@ -14799,7 +14901,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>804</v>
       </c>
@@ -14840,7 +14942,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>785</v>
       </c>
@@ -14881,7 +14983,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>805</v>
       </c>
@@ -14922,7 +15024,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>786</v>
       </c>
@@ -14963,7 +15065,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>806</v>
       </c>
@@ -15004,7 +15106,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>787</v>
       </c>
@@ -15045,7 +15147,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>807</v>
       </c>
@@ -15086,7 +15188,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>788</v>
       </c>
@@ -15127,7 +15229,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>808</v>
       </c>
@@ -15168,7 +15270,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>789</v>
       </c>
@@ -15209,7 +15311,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>809</v>
       </c>
@@ -15250,7 +15352,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>810</v>
       </c>
@@ -15291,7 +15393,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>811</v>
       </c>
@@ -15332,7 +15434,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>784</v>
       </c>
@@ -15373,7 +15475,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>804</v>
       </c>
@@ -15414,7 +15516,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>785</v>
       </c>
@@ -15455,7 +15557,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>805</v>
       </c>
@@ -15496,7 +15598,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>786</v>
       </c>
@@ -15537,7 +15639,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>806</v>
       </c>
@@ -15578,7 +15680,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>787</v>
       </c>
@@ -15619,7 +15721,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>807</v>
       </c>
@@ -15660,7 +15762,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>788</v>
       </c>
@@ -15701,7 +15803,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>808</v>
       </c>
@@ -15742,7 +15844,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>789</v>
       </c>
@@ -15783,7 +15885,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>809</v>
       </c>
@@ -15818,7 +15920,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>810</v>
       </c>
@@ -15859,7 +15961,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>811</v>
       </c>
@@ -15894,7 +15996,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>804</v>
       </c>
@@ -15935,7 +16037,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>804</v>
       </c>
@@ -15976,7 +16078,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>785</v>
       </c>
@@ -16005,7 +16107,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>787</v>
       </c>
@@ -16034,7 +16136,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>786</v>
       </c>
@@ -16060,7 +16162,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>1018</v>
       </c>
@@ -16089,7 +16191,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>786</v>
       </c>
@@ -16149,23 +16251,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16212,7 +16314,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>683</v>
       </c>
@@ -16259,7 +16361,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>683</v>
       </c>
@@ -16303,7 +16405,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>697</v>
       </c>
@@ -16364,24 +16466,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.69140625" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16428,7 +16530,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>708</v>
       </c>
@@ -16466,12 +16568,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>710</v>
       </c>
@@ -16526,23 +16628,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16589,7 +16691,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -16627,7 +16729,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>913</v>
       </c>
@@ -16679,26 +16781,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16745,7 +16847,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>912</v>
       </c>
@@ -16796,33 +16898,33 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" customWidth="1"/>
+    <col min="10" max="10" width="12.15234375" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.53515625" customWidth="1"/>
+    <col min="15" max="15" width="16.4609375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16872,7 +16974,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -16913,7 +17015,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>514</v>
       </c>
@@ -16954,7 +17056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>515</v>
       </c>
@@ -16998,7 +17100,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>547</v>
       </c>
@@ -17039,7 +17141,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>548</v>
       </c>
@@ -17080,7 +17182,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>516</v>
       </c>
@@ -17121,7 +17223,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>517</v>
       </c>
@@ -17162,7 +17264,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>518</v>
       </c>
@@ -17203,7 +17305,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>523</v>
       </c>
@@ -17244,7 +17346,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>522</v>
       </c>
@@ -17285,7 +17387,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>556</v>
       </c>
@@ -17326,7 +17428,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>559</v>
       </c>
@@ -17367,7 +17469,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>569</v>
       </c>
@@ -17408,7 +17510,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>573</v>
       </c>
@@ -17449,7 +17551,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>574</v>
       </c>
@@ -17490,7 +17592,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>1021</v>
       </c>
@@ -17531,7 +17633,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>582</v>
       </c>
@@ -17572,7 +17674,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>588</v>
       </c>
@@ -17613,7 +17715,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>591</v>
       </c>
@@ -17654,7 +17756,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>601</v>
       </c>
@@ -17695,7 +17797,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>606</v>
       </c>
@@ -17736,7 +17838,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>614</v>
       </c>
@@ -17777,7 +17879,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>1025</v>
       </c>
@@ -17818,7 +17920,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>612</v>
       </c>
@@ -17859,7 +17961,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>858</v>
       </c>
@@ -17900,7 +18002,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>865</v>
       </c>
@@ -17941,7 +18043,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>872</v>
       </c>
@@ -17982,7 +18084,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>879</v>
       </c>
@@ -18023,7 +18125,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>891</v>
       </c>
@@ -18064,7 +18166,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>892</v>
       </c>
@@ -18105,7 +18207,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>935</v>
       </c>
@@ -18146,15 +18248,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>1012</v>
       </c>
       <c r="B33" t="s">
-        <v>584</v>
+        <v>602</v>
       </c>
       <c r="C33" t="s">
-        <v>584</v>
+        <v>603</v>
       </c>
       <c r="D33" t="s">
         <v>1012</v>
@@ -18182,6 +18284,416 @@
       </c>
       <c r="P33" t="s">
         <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E34" t="s">
+        <v>755</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1064</v>
+      </c>
+      <c r="O34" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P34" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E35" t="s">
+        <v>755</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I35" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1065</v>
+      </c>
+      <c r="O35" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P35" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E36" t="s">
+        <v>755</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1066</v>
+      </c>
+      <c r="O36" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P36" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E37" t="s">
+        <v>755</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I37" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O37" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P37" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E38" t="s">
+        <v>755</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1058</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O38" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P38" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E39" t="s">
+        <v>755</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" t="s">
+        <v>1059</v>
+      </c>
+      <c r="I39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" t="s">
+        <v>1068</v>
+      </c>
+      <c r="O39" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P39" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E40" t="s">
+        <v>755</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" t="s">
+        <v>1069</v>
+      </c>
+      <c r="O40" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P40" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E41" t="s">
+        <v>755</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1061</v>
+      </c>
+      <c r="I41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" t="s">
+        <v>1070</v>
+      </c>
+      <c r="O41" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P41" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E42" t="s">
+        <v>755</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1053</v>
+      </c>
+      <c r="G42" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" t="s">
+        <v>1071</v>
+      </c>
+      <c r="O42" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P42" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E43" t="s">
+        <v>755</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I43" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" t="s">
+        <v>1072</v>
+      </c>
+      <c r="O43" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P43" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -18200,25 +18712,25 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18265,7 +18777,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>669</v>
       </c>
@@ -18312,7 +18824,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>669</v>
       </c>
@@ -18356,7 +18868,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>731</v>
       </c>

</xml_diff>

<commit_message>
Fix LMP91000SD, fix MCP1501, add Feather RP2040 RFM95
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1551DD1E-EAA1-4651-B940-FFA8CE26C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC508F7-1523-4D50-82BF-988960D24C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4675" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4686" uniqueCount="1080">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3281,6 +3281,15 @@
   </si>
   <si>
     <t>5.000 V Voltage reference</t>
+  </si>
+  <si>
+    <t>Feather RP2040 RFM95</t>
+  </si>
+  <si>
+    <t>1528-5714-ND</t>
+  </si>
+  <si>
+    <t>Feather RP2040 with RFM95W LoRa Transceiver</t>
   </si>
 </sst>
 </file>
@@ -3891,26 +3900,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.84375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.69140625" customWidth="1"/>
     <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3931,7 +3939,7 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3978,7 +3986,7 @@
       <c r="E2" t="s">
         <v>623</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>622</v>
       </c>
       <c r="G2" t="s">
@@ -4016,7 +4024,7 @@
       <c r="E3" t="s">
         <v>568</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>605</v>
       </c>
       <c r="G3" t="s">
@@ -4054,7 +4062,7 @@
       <c r="E4" t="s">
         <v>755</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>754</v>
       </c>
       <c r="G4" t="s">
@@ -4092,7 +4100,7 @@
       <c r="E5" t="s">
         <v>894</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>895</v>
       </c>
       <c r="I5" t="s">
@@ -4106,6 +4114,44 @@
       </c>
       <c r="O5" t="s">
         <v>901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E6" t="s">
+        <v>931</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5714</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="O6" t="s">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -16909,9 +16955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add Phoenix Contact 1861933
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC508F7-1523-4D50-82BF-988960D24C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DE836E-6970-416B-8FC9-4A93C3C3F7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4686" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4699" uniqueCount="1085">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3290,6 +3290,21 @@
   </si>
   <si>
     <t>Feather RP2040 with RFM95W LoRa Transceiver</t>
+  </si>
+  <si>
+    <t>1861933</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>277-12124-ND</t>
+  </si>
+  <si>
+    <t>300 V 8 A max</t>
+  </si>
+  <si>
+    <t>2 pin spring lock terminal block</t>
   </si>
 </sst>
 </file>
@@ -3680,24 +3695,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3828125" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.15234375" customWidth="1"/>
-    <col min="14" max="14" width="13.53515625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3744,7 +3759,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -3763,24 +3778,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" customWidth="1"/>
-    <col min="2" max="2" width="13.84375" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3828125" customWidth="1"/>
-    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.53515625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3827,7 +3842,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>918</v>
       </c>
@@ -3865,7 +3880,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>918</v>
       </c>
@@ -3907,23 +3922,23 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3970,7 +3985,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -4008,7 +4023,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -4046,7 +4061,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>758</v>
       </c>
@@ -4084,7 +4099,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>893</v>
       </c>
@@ -4116,7 +4131,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1077</v>
       </c>
@@ -4169,23 +4184,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.53515625" customWidth="1"/>
-    <col min="3" max="4" width="20.84375" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.69140625" customWidth="1"/>
-    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4232,7 +4247,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>667</v>
       </c>
@@ -4252,7 +4267,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>990</v>
       </c>
@@ -4281,7 +4296,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>990</v>
       </c>
@@ -4310,7 +4325,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>990</v>
       </c>
@@ -4339,7 +4354,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>990</v>
       </c>
@@ -4368,7 +4383,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>990</v>
       </c>
@@ -4397,7 +4412,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>990</v>
       </c>
@@ -4426,7 +4441,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>990</v>
       </c>
@@ -4455,7 +4470,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>990</v>
       </c>
@@ -4484,7 +4499,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>990</v>
       </c>
@@ -4513,7 +4528,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>990</v>
       </c>
@@ -4542,7 +4557,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>990</v>
       </c>
@@ -4571,7 +4586,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>990</v>
       </c>
@@ -4600,7 +4615,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>991</v>
       </c>
@@ -4629,7 +4644,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>991</v>
       </c>
@@ -4658,7 +4673,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>991</v>
       </c>
@@ -4687,7 +4702,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>991</v>
       </c>
@@ -4716,7 +4731,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>991</v>
       </c>
@@ -4745,7 +4760,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>991</v>
       </c>
@@ -4774,7 +4789,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>991</v>
       </c>
@@ -4803,7 +4818,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>991</v>
       </c>
@@ -4832,7 +4847,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>991</v>
       </c>
@@ -4861,7 +4876,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>991</v>
       </c>
@@ -4890,7 +4905,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>991</v>
       </c>
@@ -4919,7 +4934,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>991</v>
       </c>
@@ -4962,25 +4977,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3828125" customWidth="1"/>
-    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5027,7 +5042,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>929</v>
       </c>
@@ -5068,7 +5083,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>716</v>
       </c>
@@ -5088,7 +5103,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>717</v>
       </c>
@@ -5096,7 +5111,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>718</v>
       </c>
@@ -5104,7 +5119,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>897</v>
       </c>
@@ -5112,7 +5127,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>992</v>
       </c>
@@ -5167,23 +5182,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.53515625" customWidth="1"/>
-    <col min="14" max="14" width="12.3828125" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5230,7 +5245,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -5249,26 +5264,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.53515625" customWidth="1"/>
-    <col min="5" max="5" width="14.3046875" customWidth="1"/>
-    <col min="6" max="6" width="21.3828125" customWidth="1"/>
-    <col min="7" max="7" width="11.69140625" customWidth="1"/>
-    <col min="8" max="8" width="17.15234375" customWidth="1"/>
-    <col min="9" max="9" width="9.3046875" customWidth="1"/>
-    <col min="10" max="10" width="9.69140625" customWidth="1"/>
-    <col min="11" max="11" width="39.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.3046875" customWidth="1"/>
-    <col min="14" max="14" width="23.15234375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="39.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5315,7 +5330,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -5359,7 +5374,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -5403,7 +5418,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -5447,7 +5462,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5491,7 +5506,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -5535,7 +5550,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5579,7 +5594,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -5623,7 +5638,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5667,7 +5682,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -5711,7 +5726,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -5755,7 +5770,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -5799,7 +5814,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -5843,7 +5858,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5887,7 +5902,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -5931,7 +5946,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -5975,7 +5990,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6019,7 +6034,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -6063,7 +6078,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -6107,7 +6122,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -6151,7 +6166,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -6195,7 +6210,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6239,7 +6254,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -6283,7 +6298,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -6327,7 +6342,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -6371,7 +6386,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6415,7 +6430,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -6459,7 +6474,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -6503,7 +6518,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -6547,7 +6562,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -6591,7 +6606,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -6635,7 +6650,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -6679,7 +6694,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -6723,7 +6738,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -6767,7 +6782,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -6811,7 +6826,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -6855,7 +6870,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -6899,7 +6914,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -6943,7 +6958,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -6987,7 +7002,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -7031,7 +7046,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -7075,7 +7090,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -7119,7 +7134,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -7163,7 +7178,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7207,7 +7222,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7251,7 +7266,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -7295,7 +7310,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7339,7 +7354,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -7383,7 +7398,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -7427,7 +7442,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -7471,7 +7486,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -7515,7 +7530,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -7559,7 +7574,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7603,7 +7618,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -7647,7 +7662,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -7691,7 +7706,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -7735,7 +7750,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -7779,7 +7794,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -7823,7 +7838,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -7867,7 +7882,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -7911,7 +7926,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -7955,7 +7970,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -7999,7 +8014,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -8043,7 +8058,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -8087,7 +8102,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -8131,7 +8146,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -8175,7 +8190,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8219,7 +8234,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -8263,7 +8278,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -8307,7 +8322,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -8351,7 +8366,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -8395,7 +8410,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -8439,7 +8454,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -8483,7 +8498,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -8527,7 +8542,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -8571,7 +8586,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -8615,7 +8630,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -8659,7 +8674,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -8703,7 +8718,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -8747,7 +8762,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -8791,7 +8806,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -8835,7 +8850,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -8879,7 +8894,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -8923,7 +8938,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -8967,7 +8982,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -9011,7 +9026,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -9055,7 +9070,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -9099,7 +9114,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -9143,7 +9158,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -9187,7 +9202,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9231,7 +9246,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -9275,7 +9290,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -9319,7 +9334,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -9363,7 +9378,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -9407,7 +9422,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -9451,7 +9466,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -9495,7 +9510,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -9539,7 +9554,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -9583,7 +9598,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -9627,7 +9642,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -9671,7 +9686,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -9715,7 +9730,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -9759,7 +9774,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -9803,7 +9818,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -9847,7 +9862,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -9891,7 +9906,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -9935,7 +9950,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -9979,7 +9994,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -10023,7 +10038,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -10067,7 +10082,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -10111,7 +10126,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -10155,7 +10170,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -10199,7 +10214,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10243,7 +10258,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -10287,7 +10302,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -10331,7 +10346,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -10375,7 +10390,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -10419,7 +10434,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -10463,7 +10478,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -10507,7 +10522,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -10551,7 +10566,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -10595,7 +10610,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -10639,7 +10654,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -10683,7 +10698,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -10727,7 +10742,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -10771,7 +10786,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -10815,7 +10830,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -10859,7 +10874,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -10900,7 +10915,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -10941,7 +10956,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -10982,7 +10997,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -11039,25 +11054,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.15234375" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.15234375" customWidth="1"/>
-    <col min="9" max="9" width="7.3828125" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.3828125" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.3046875" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11104,7 +11119,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>711</v>
       </c>
@@ -11148,7 +11163,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -11207,24 +11222,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11271,7 +11286,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>713</v>
       </c>
@@ -11315,7 +11330,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>713</v>
       </c>
@@ -11359,7 +11374,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>714</v>
       </c>
@@ -11403,7 +11418,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>714</v>
       </c>
@@ -11461,26 +11476,26 @@
       <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.3828125" customWidth="1"/>
-    <col min="6" max="6" width="25.15234375" customWidth="1"/>
-    <col min="7" max="7" width="12.3046875" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.84375" customWidth="1"/>
-    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11530,7 +11545,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -11577,7 +11592,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -11624,7 +11639,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -11671,7 +11686,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -11718,7 +11733,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -11765,7 +11780,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -11812,7 +11827,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -11859,7 +11874,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -11906,7 +11921,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -11953,7 +11968,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -12000,7 +12015,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -12047,7 +12062,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -12094,7 +12109,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -12141,7 +12156,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -12188,7 +12203,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12235,7 +12250,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -12282,7 +12297,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -12329,7 +12344,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -12376,7 +12391,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -12423,7 +12438,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -12470,7 +12485,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -12517,7 +12532,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -12564,7 +12579,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -12611,7 +12626,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -12658,7 +12673,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -12705,7 +12720,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -12752,7 +12767,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -12799,7 +12814,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -12846,7 +12861,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -12893,7 +12908,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -12940,7 +12955,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -12987,7 +13002,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -13034,7 +13049,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -13081,7 +13096,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -13128,7 +13143,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -13175,7 +13190,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13222,7 +13237,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -13269,7 +13284,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -13319,7 +13334,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -13366,7 +13381,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -13413,7 +13428,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -13460,7 +13475,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -13507,7 +13522,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -13554,7 +13569,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -13601,7 +13616,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -13648,7 +13663,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -13695,7 +13710,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -13742,7 +13757,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -13789,7 +13804,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -13836,7 +13851,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -13883,7 +13898,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -13930,7 +13945,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -13977,7 +13992,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -14024,7 +14039,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -14071,7 +14086,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -14118,7 +14133,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -14165,7 +14180,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14212,7 +14227,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -14256,7 +14271,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -14300,7 +14315,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -14344,7 +14359,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -14397,33 +14412,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.15234375" style="6"/>
+    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14470,7 +14485,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -14511,7 +14526,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -14549,7 +14564,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>651</v>
       </c>
@@ -14587,7 +14602,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -14628,7 +14643,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>664</v>
       </c>
@@ -14669,7 +14684,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>663</v>
       </c>
@@ -14710,7 +14725,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -14751,7 +14766,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>785</v>
       </c>
@@ -14792,7 +14807,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>786</v>
       </c>
@@ -14833,7 +14848,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>787</v>
       </c>
@@ -14874,7 +14889,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>785</v>
       </c>
@@ -14915,7 +14930,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>784</v>
       </c>
@@ -14956,7 +14971,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>804</v>
       </c>
@@ -14997,7 +15012,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>785</v>
       </c>
@@ -15038,7 +15053,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>805</v>
       </c>
@@ -15079,7 +15094,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>786</v>
       </c>
@@ -15120,7 +15135,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>806</v>
       </c>
@@ -15161,7 +15176,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>787</v>
       </c>
@@ -15202,7 +15217,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>807</v>
       </c>
@@ -15243,7 +15258,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>788</v>
       </c>
@@ -15284,7 +15299,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>808</v>
       </c>
@@ -15325,7 +15340,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>789</v>
       </c>
@@ -15366,7 +15381,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>809</v>
       </c>
@@ -15407,7 +15422,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>810</v>
       </c>
@@ -15448,7 +15463,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>811</v>
       </c>
@@ -15489,7 +15504,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>784</v>
       </c>
@@ -15530,7 +15545,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>804</v>
       </c>
@@ -15571,7 +15586,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>785</v>
       </c>
@@ -15612,7 +15627,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>805</v>
       </c>
@@ -15653,7 +15668,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>786</v>
       </c>
@@ -15694,7 +15709,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>806</v>
       </c>
@@ -15735,7 +15750,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>787</v>
       </c>
@@ -15776,7 +15791,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>807</v>
       </c>
@@ -15817,7 +15832,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>788</v>
       </c>
@@ -15858,7 +15873,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>808</v>
       </c>
@@ -15899,7 +15914,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>789</v>
       </c>
@@ -15940,7 +15955,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>809</v>
       </c>
@@ -15975,7 +15990,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>810</v>
       </c>
@@ -16016,7 +16031,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>811</v>
       </c>
@@ -16051,7 +16066,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>804</v>
       </c>
@@ -16092,7 +16107,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>804</v>
       </c>
@@ -16133,7 +16148,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>785</v>
       </c>
@@ -16162,7 +16177,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>787</v>
       </c>
@@ -16191,7 +16206,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>786</v>
       </c>
@@ -16217,7 +16232,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>1018</v>
       </c>
@@ -16246,7 +16261,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>786</v>
       </c>
@@ -16284,6 +16299,47 @@
         <v>1036</v>
       </c>
       <c r="O47" s="6" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>784</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>1083</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="O48" s="6" t="s">
         <v>900</v>
       </c>
     </row>
@@ -16306,23 +16362,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16369,7 +16425,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>683</v>
       </c>
@@ -16416,7 +16472,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>683</v>
       </c>
@@ -16460,7 +16516,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>697</v>
       </c>
@@ -16521,24 +16577,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.69140625" customWidth="1"/>
-    <col min="14" max="14" width="20.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16585,7 +16641,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>708</v>
       </c>
@@ -16623,12 +16679,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>710</v>
       </c>
@@ -16683,23 +16739,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.15234375" customWidth="1"/>
-    <col min="2" max="2" width="14.69140625" customWidth="1"/>
-    <col min="3" max="3" width="15.69140625" customWidth="1"/>
-    <col min="4" max="4" width="16.3046875" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.3046875" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16746,7 +16802,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -16784,7 +16840,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>913</v>
       </c>
@@ -16836,26 +16892,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16902,7 +16958,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>912</v>
       </c>
@@ -16955,31 +17011,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.84375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="6.53515625" customWidth="1"/>
-    <col min="10" max="10" width="12.15234375" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.53515625" customWidth="1"/>
-    <col min="15" max="15" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17029,7 +17085,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -17070,7 +17126,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>514</v>
       </c>
@@ -17111,7 +17167,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>515</v>
       </c>
@@ -17155,7 +17211,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>547</v>
       </c>
@@ -17196,7 +17252,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>548</v>
       </c>
@@ -17237,7 +17293,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>516</v>
       </c>
@@ -17278,7 +17334,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>517</v>
       </c>
@@ -17319,7 +17375,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>518</v>
       </c>
@@ -17360,7 +17416,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>523</v>
       </c>
@@ -17401,7 +17457,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>522</v>
       </c>
@@ -17442,7 +17498,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>556</v>
       </c>
@@ -17483,7 +17539,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>559</v>
       </c>
@@ -17524,7 +17580,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>569</v>
       </c>
@@ -17565,7 +17621,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>573</v>
       </c>
@@ -17606,7 +17662,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>574</v>
       </c>
@@ -17647,7 +17703,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1021</v>
       </c>
@@ -17688,7 +17744,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>582</v>
       </c>
@@ -17729,7 +17785,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>588</v>
       </c>
@@ -17770,7 +17826,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>591</v>
       </c>
@@ -17811,7 +17867,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>601</v>
       </c>
@@ -17852,7 +17908,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>606</v>
       </c>
@@ -17893,7 +17949,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>614</v>
       </c>
@@ -17934,7 +17990,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1025</v>
       </c>
@@ -17975,7 +18031,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>612</v>
       </c>
@@ -18016,7 +18072,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>858</v>
       </c>
@@ -18057,7 +18113,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>865</v>
       </c>
@@ -18098,7 +18154,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>872</v>
       </c>
@@ -18139,7 +18195,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>879</v>
       </c>
@@ -18180,7 +18236,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>891</v>
       </c>
@@ -18221,7 +18277,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>892</v>
       </c>
@@ -18262,7 +18318,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>935</v>
       </c>
@@ -18303,7 +18359,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1012</v>
       </c>
@@ -18341,7 +18397,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1040</v>
       </c>
@@ -18385,7 +18441,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1043</v>
       </c>
@@ -18426,7 +18482,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1043</v>
       </c>
@@ -18467,7 +18523,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1043</v>
       </c>
@@ -18508,7 +18564,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1043</v>
       </c>
@@ -18549,7 +18605,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1043</v>
       </c>
@@ -18590,7 +18646,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1043</v>
       </c>
@@ -18631,7 +18687,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1043</v>
       </c>
@@ -18672,7 +18728,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -18713,7 +18769,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1043</v>
       </c>
@@ -18754,7 +18810,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1043</v>
       </c>
@@ -18811,25 +18867,25 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18876,7 +18932,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>669</v>
       </c>
@@ -18923,7 +18979,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>669</v>
       </c>
@@ -18967,7 +19023,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>731</v>
       </c>

</xml_diff>

<commit_message>
Create symbol for BNO055 breakout
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3AAC54-102A-4A13-8C1E-94A5214100EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8F4360-7BA7-4C3A-A041-FF84D6F3BD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-69" yWindow="-69" windowWidth="24823" windowHeight="15566" tabRatio="905" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4711" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="1093">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3317,6 +3317,18 @@
   </si>
   <si>
     <t>5V 1A LDO linear regulator, 7-35V input</t>
+  </si>
+  <si>
+    <t>BNO055 Breakout</t>
+  </si>
+  <si>
+    <t>2472</t>
+  </si>
+  <si>
+    <t>1528-1426-ND</t>
+  </si>
+  <si>
+    <t>BNO055 IMU breakout</t>
   </si>
 </sst>
 </file>
@@ -3707,24 +3719,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15234375" customWidth="1"/>
+    <col min="14" max="14" width="13.53515625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3771,7 +3783,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -3790,24 +3802,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.53515625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>918</v>
       </c>
@@ -3892,7 +3904,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>918</v>
       </c>
@@ -3927,30 +3939,30 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3997,7 +4009,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -4035,7 +4047,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -4073,7 +4085,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>758</v>
       </c>
@@ -4111,7 +4123,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>893</v>
       </c>
@@ -4143,7 +4155,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1077</v>
       </c>
@@ -4179,6 +4191,44 @@
       </c>
       <c r="O6" t="s">
         <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E7" t="s">
+        <v>931</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="O7" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -4196,23 +4246,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" customWidth="1"/>
+    <col min="3" max="4" width="20.84375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.69140625" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4259,7 +4309,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>667</v>
       </c>
@@ -4279,7 +4329,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>990</v>
       </c>
@@ -4308,7 +4358,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>990</v>
       </c>
@@ -4337,7 +4387,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>990</v>
       </c>
@@ -4366,7 +4416,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>990</v>
       </c>
@@ -4395,7 +4445,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>990</v>
       </c>
@@ -4424,7 +4474,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>990</v>
       </c>
@@ -4453,7 +4503,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>990</v>
       </c>
@@ -4482,7 +4532,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>990</v>
       </c>
@@ -4511,7 +4561,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>990</v>
       </c>
@@ -4540,7 +4590,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>990</v>
       </c>
@@ -4569,7 +4619,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>990</v>
       </c>
@@ -4598,7 +4648,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>990</v>
       </c>
@@ -4627,7 +4677,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>991</v>
       </c>
@@ -4656,7 +4706,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>991</v>
       </c>
@@ -4685,7 +4735,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>991</v>
       </c>
@@ -4714,7 +4764,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>991</v>
       </c>
@@ -4743,7 +4793,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>991</v>
       </c>
@@ -4772,7 +4822,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>991</v>
       </c>
@@ -4801,7 +4851,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>991</v>
       </c>
@@ -4830,7 +4880,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>991</v>
       </c>
@@ -4859,7 +4909,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>991</v>
       </c>
@@ -4888,7 +4938,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>991</v>
       </c>
@@ -4917,7 +4967,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>991</v>
       </c>
@@ -4946,7 +4996,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>991</v>
       </c>
@@ -4989,25 +5039,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5054,7 +5104,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>929</v>
       </c>
@@ -5095,7 +5145,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>716</v>
       </c>
@@ -5115,7 +5165,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>717</v>
       </c>
@@ -5123,7 +5173,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>718</v>
       </c>
@@ -5131,7 +5181,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>897</v>
       </c>
@@ -5139,7 +5189,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>992</v>
       </c>
@@ -5194,23 +5244,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" customWidth="1"/>
+    <col min="14" max="14" width="12.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5257,7 +5307,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -5276,26 +5326,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="14.3046875" customWidth="1"/>
+    <col min="6" max="6" width="21.3828125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.15234375" customWidth="1"/>
+    <col min="9" max="9" width="9.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="39.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.3046875" customWidth="1"/>
+    <col min="14" max="14" width="23.15234375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5342,7 +5392,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -5386,7 +5436,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -5430,7 +5480,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -5474,7 +5524,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5518,7 +5568,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -5562,7 +5612,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5606,7 +5656,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -5650,7 +5700,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5694,7 +5744,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -5738,7 +5788,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -5782,7 +5832,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -5826,7 +5876,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -5870,7 +5920,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5914,7 +5964,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -5958,7 +6008,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -6002,7 +6052,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6046,7 +6096,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -6090,7 +6140,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -6134,7 +6184,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -6178,7 +6228,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -6222,7 +6272,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6266,7 +6316,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -6310,7 +6360,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -6354,7 +6404,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -6398,7 +6448,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6442,7 +6492,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -6486,7 +6536,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -6530,7 +6580,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -6574,7 +6624,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -6618,7 +6668,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -6662,7 +6712,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -6706,7 +6756,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -6750,7 +6800,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -6794,7 +6844,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -6838,7 +6888,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -6882,7 +6932,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -6926,7 +6976,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -6970,7 +7020,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -7014,7 +7064,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -7058,7 +7108,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -7102,7 +7152,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -7146,7 +7196,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -7190,7 +7240,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7234,7 +7284,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7278,7 +7328,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -7322,7 +7372,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7366,7 +7416,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -7410,7 +7460,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -7454,7 +7504,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -7498,7 +7548,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -7542,7 +7592,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -7586,7 +7636,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7630,7 +7680,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -7674,7 +7724,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -7718,7 +7768,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -7762,7 +7812,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -7806,7 +7856,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -7850,7 +7900,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -7894,7 +7944,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -7938,7 +7988,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -7982,7 +8032,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -8026,7 +8076,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -8070,7 +8120,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -8114,7 +8164,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -8158,7 +8208,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -8202,7 +8252,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8246,7 +8296,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -8290,7 +8340,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -8334,7 +8384,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -8378,7 +8428,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -8422,7 +8472,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -8466,7 +8516,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -8510,7 +8560,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -8554,7 +8604,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -8598,7 +8648,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -8642,7 +8692,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -8686,7 +8736,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -8730,7 +8780,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -8774,7 +8824,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -8818,7 +8868,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -8862,7 +8912,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -8906,7 +8956,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -8950,7 +9000,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -8994,7 +9044,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -9038,7 +9088,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -9082,7 +9132,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -9126,7 +9176,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -9170,7 +9220,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -9214,7 +9264,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9258,7 +9308,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -9302,7 +9352,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -9346,7 +9396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -9390,7 +9440,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -9434,7 +9484,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -9478,7 +9528,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -9522,7 +9572,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -9566,7 +9616,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -9610,7 +9660,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -9654,7 +9704,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -9698,7 +9748,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -9742,7 +9792,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -9786,7 +9836,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -9830,7 +9880,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -9874,7 +9924,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -9918,7 +9968,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -9962,7 +10012,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -10006,7 +10056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -10050,7 +10100,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -10094,7 +10144,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -10138,7 +10188,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -10182,7 +10232,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -10226,7 +10276,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10270,7 +10320,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -10314,7 +10364,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -10358,7 +10408,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -10402,7 +10452,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -10446,7 +10496,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -10490,7 +10540,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -10534,7 +10584,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -10578,7 +10628,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -10622,7 +10672,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -10666,7 +10716,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -10710,7 +10760,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -10754,7 +10804,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -10798,7 +10848,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -10842,7 +10892,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -10886,7 +10936,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -10927,7 +10977,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -10968,7 +11018,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -11009,7 +11059,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -11066,25 +11116,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3828125" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11131,7 +11181,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>711</v>
       </c>
@@ -11175,7 +11225,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -11234,24 +11284,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.53515625" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11298,7 +11348,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>713</v>
       </c>
@@ -11342,7 +11392,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>713</v>
       </c>
@@ -11386,7 +11436,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>714</v>
       </c>
@@ -11430,7 +11480,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>714</v>
       </c>
@@ -11488,26 +11538,26 @@
       <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" customWidth="1"/>
+    <col min="6" max="6" width="25.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3046875" customWidth="1"/>
+    <col min="8" max="8" width="19.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.84375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11557,7 +11607,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -11604,7 +11654,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -11651,7 +11701,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -11698,7 +11748,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -11745,7 +11795,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -11792,7 +11842,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -11839,7 +11889,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -11886,7 +11936,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -11933,7 +11983,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -11980,7 +12030,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -12027,7 +12077,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -12074,7 +12124,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -12121,7 +12171,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -12168,7 +12218,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -12215,7 +12265,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12262,7 +12312,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -12309,7 +12359,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -12356,7 +12406,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -12403,7 +12453,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -12450,7 +12500,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -12497,7 +12547,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -12544,7 +12594,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -12591,7 +12641,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -12638,7 +12688,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -12685,7 +12735,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -12732,7 +12782,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -12779,7 +12829,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -12826,7 +12876,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -12873,7 +12923,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -12920,7 +12970,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -12967,7 +13017,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -13014,7 +13064,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -13061,7 +13111,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -13108,7 +13158,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -13155,7 +13205,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -13202,7 +13252,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13249,7 +13299,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -13296,7 +13346,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -13346,7 +13396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -13393,7 +13443,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -13440,7 +13490,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -13487,7 +13537,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -13534,7 +13584,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -13581,7 +13631,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -13628,7 +13678,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -13675,7 +13725,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -13722,7 +13772,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -13769,7 +13819,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -13816,7 +13866,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -13863,7 +13913,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -13910,7 +13960,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -13957,7 +14007,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -14004,7 +14054,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -14051,7 +14101,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -14098,7 +14148,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -14145,7 +14195,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -14192,7 +14242,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14239,7 +14289,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -14283,7 +14333,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -14327,7 +14377,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -14371,7 +14421,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -14431,26 +14481,26 @@
       <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="6"/>
+    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14497,7 +14547,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -14538,7 +14588,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -14576,7 +14626,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>651</v>
       </c>
@@ -14614,7 +14664,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -14655,7 +14705,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>664</v>
       </c>
@@ -14696,7 +14746,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>663</v>
       </c>
@@ -14737,7 +14787,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -14778,7 +14828,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>785</v>
       </c>
@@ -14819,7 +14869,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>786</v>
       </c>
@@ -14860,7 +14910,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>787</v>
       </c>
@@ -14901,7 +14951,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>785</v>
       </c>
@@ -14942,7 +14992,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>784</v>
       </c>
@@ -14983,7 +15033,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>804</v>
       </c>
@@ -15024,7 +15074,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>785</v>
       </c>
@@ -15065,7 +15115,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>805</v>
       </c>
@@ -15106,7 +15156,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>786</v>
       </c>
@@ -15147,7 +15197,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>806</v>
       </c>
@@ -15188,7 +15238,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>787</v>
       </c>
@@ -15229,7 +15279,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>807</v>
       </c>
@@ -15270,7 +15320,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>788</v>
       </c>
@@ -15311,7 +15361,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>808</v>
       </c>
@@ -15352,7 +15402,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>789</v>
       </c>
@@ -15393,7 +15443,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>809</v>
       </c>
@@ -15434,7 +15484,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>810</v>
       </c>
@@ -15475,7 +15525,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>811</v>
       </c>
@@ -15516,7 +15566,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>784</v>
       </c>
@@ -15557,7 +15607,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>804</v>
       </c>
@@ -15598,7 +15648,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>785</v>
       </c>
@@ -15639,7 +15689,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>805</v>
       </c>
@@ -15680,7 +15730,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>786</v>
       </c>
@@ -15721,7 +15771,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>806</v>
       </c>
@@ -15762,7 +15812,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>787</v>
       </c>
@@ -15803,7 +15853,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>807</v>
       </c>
@@ -15844,7 +15894,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>788</v>
       </c>
@@ -15885,7 +15935,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>808</v>
       </c>
@@ -15926,7 +15976,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>789</v>
       </c>
@@ -15967,7 +16017,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>809</v>
       </c>
@@ -16002,7 +16052,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>810</v>
       </c>
@@ -16043,7 +16093,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>811</v>
       </c>
@@ -16078,7 +16128,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>804</v>
       </c>
@@ -16119,7 +16169,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>804</v>
       </c>
@@ -16160,7 +16210,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>785</v>
       </c>
@@ -16189,7 +16239,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>787</v>
       </c>
@@ -16218,7 +16268,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>786</v>
       </c>
@@ -16244,7 +16294,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>1018</v>
       </c>
@@ -16273,7 +16323,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>786</v>
       </c>
@@ -16314,7 +16364,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="6" t="s">
         <v>784</v>
       </c>
@@ -16374,23 +16424,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16437,7 +16487,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>683</v>
       </c>
@@ -16484,7 +16534,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>683</v>
       </c>
@@ -16528,7 +16578,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>697</v>
       </c>
@@ -16589,24 +16639,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.69140625" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16653,7 +16703,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>708</v>
       </c>
@@ -16691,12 +16741,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>710</v>
       </c>
@@ -16751,23 +16801,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16814,7 +16864,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -16852,7 +16902,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>913</v>
       </c>
@@ -16904,26 +16954,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16970,7 +17020,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>912</v>
       </c>
@@ -17023,31 +17073,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" customWidth="1"/>
+    <col min="10" max="10" width="12.15234375" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.53515625" customWidth="1"/>
+    <col min="15" max="15" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -17097,7 +17147,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -17138,7 +17188,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>514</v>
       </c>
@@ -17179,7 +17229,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>515</v>
       </c>
@@ -17223,7 +17273,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>547</v>
       </c>
@@ -17264,7 +17314,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>548</v>
       </c>
@@ -17305,7 +17355,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>516</v>
       </c>
@@ -17346,7 +17396,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>517</v>
       </c>
@@ -17387,7 +17437,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>518</v>
       </c>
@@ -17428,7 +17478,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>523</v>
       </c>
@@ -17469,7 +17519,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>522</v>
       </c>
@@ -17510,7 +17560,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>556</v>
       </c>
@@ -17551,7 +17601,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>559</v>
       </c>
@@ -17592,7 +17642,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>569</v>
       </c>
@@ -17633,7 +17683,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>573</v>
       </c>
@@ -17674,7 +17724,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>574</v>
       </c>
@@ -17715,7 +17765,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>1021</v>
       </c>
@@ -17756,7 +17806,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>582</v>
       </c>
@@ -17797,7 +17847,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>588</v>
       </c>
@@ -17838,7 +17888,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>591</v>
       </c>
@@ -17879,7 +17929,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>601</v>
       </c>
@@ -17920,7 +17970,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>606</v>
       </c>
@@ -17961,7 +18011,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>614</v>
       </c>
@@ -18002,7 +18052,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>1025</v>
       </c>
@@ -18043,7 +18093,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="6">
         <v>7805</v>
       </c>
@@ -18084,7 +18134,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>612</v>
       </c>
@@ -18125,7 +18175,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>858</v>
       </c>
@@ -18166,7 +18216,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>865</v>
       </c>
@@ -18207,7 +18257,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>872</v>
       </c>
@@ -18248,7 +18298,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>879</v>
       </c>
@@ -18289,7 +18339,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>891</v>
       </c>
@@ -18330,7 +18380,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>892</v>
       </c>
@@ -18371,7 +18421,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>935</v>
       </c>
@@ -18412,7 +18462,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>1012</v>
       </c>
@@ -18450,7 +18500,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>1040</v>
       </c>
@@ -18494,7 +18544,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18535,7 +18585,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18576,7 +18626,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18617,7 +18667,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18658,7 +18708,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18699,7 +18749,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18740,7 +18790,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18781,7 +18831,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18822,7 +18872,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18863,7 +18913,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18920,25 +18970,25 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18985,7 +19035,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>669</v>
       </c>
@@ -19032,7 +19082,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>669</v>
       </c>
@@ -19076,7 +19126,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>731</v>
       </c>

</xml_diff>

<commit_message>
Add big easy driver
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8F4360-7BA7-4C3A-A041-FF84D6F3BD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2E03E-ADC5-410C-9C4F-10C454C26908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-69" yWindow="-69" windowWidth="24823" windowHeight="15566" tabRatio="905" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4735" uniqueCount="1098">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3329,6 +3329,21 @@
   </si>
   <si>
     <t>BNO055 IMU breakout</t>
+  </si>
+  <si>
+    <t>ROB-12859</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>Big Easy Driver</t>
+  </si>
+  <si>
+    <t>1568-1066-ND</t>
+  </si>
+  <si>
+    <t>Stepper motor driver</t>
   </si>
 </sst>
 </file>
@@ -3719,24 +3734,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3828125" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.15234375" customWidth="1"/>
-    <col min="14" max="14" width="13.53515625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3783,7 +3798,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -3802,24 +3817,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" customWidth="1"/>
-    <col min="2" max="2" width="13.84375" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3828125" customWidth="1"/>
-    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.53515625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3866,7 +3881,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>918</v>
       </c>
@@ -3904,7 +3919,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>918</v>
       </c>
@@ -3939,30 +3954,30 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4009,7 +4024,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -4047,7 +4062,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -4085,7 +4100,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>758</v>
       </c>
@@ -4123,7 +4138,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>893</v>
       </c>
@@ -4155,7 +4170,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1077</v>
       </c>
@@ -4193,7 +4208,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1089</v>
       </c>
@@ -4228,7 +4243,45 @@
         <v>1092</v>
       </c>
       <c r="O7" t="s">
-        <v>901</v>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1097</v>
+      </c>
+      <c r="O8" t="s">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -4246,23 +4299,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.53515625" customWidth="1"/>
-    <col min="3" max="4" width="20.84375" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.69140625" customWidth="1"/>
-    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4309,7 +4362,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>667</v>
       </c>
@@ -4329,7 +4382,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>990</v>
       </c>
@@ -4358,7 +4411,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>990</v>
       </c>
@@ -4387,7 +4440,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>990</v>
       </c>
@@ -4416,7 +4469,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>990</v>
       </c>
@@ -4445,7 +4498,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>990</v>
       </c>
@@ -4474,7 +4527,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>990</v>
       </c>
@@ -4503,7 +4556,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>990</v>
       </c>
@@ -4532,7 +4585,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>990</v>
       </c>
@@ -4561,7 +4614,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>990</v>
       </c>
@@ -4590,7 +4643,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>990</v>
       </c>
@@ -4619,7 +4672,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>990</v>
       </c>
@@ -4648,7 +4701,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>990</v>
       </c>
@@ -4677,7 +4730,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>991</v>
       </c>
@@ -4706,7 +4759,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>991</v>
       </c>
@@ -4735,7 +4788,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>991</v>
       </c>
@@ -4764,7 +4817,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>991</v>
       </c>
@@ -4793,7 +4846,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>991</v>
       </c>
@@ -4822,7 +4875,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>991</v>
       </c>
@@ -4851,7 +4904,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>991</v>
       </c>
@@ -4880,7 +4933,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>991</v>
       </c>
@@ -4909,7 +4962,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>991</v>
       </c>
@@ -4938,7 +4991,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>991</v>
       </c>
@@ -4967,7 +5020,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>991</v>
       </c>
@@ -4996,7 +5049,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>991</v>
       </c>
@@ -5039,25 +5092,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3828125" customWidth="1"/>
-    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5104,7 +5157,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>929</v>
       </c>
@@ -5145,7 +5198,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>716</v>
       </c>
@@ -5165,7 +5218,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>717</v>
       </c>
@@ -5173,7 +5226,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>718</v>
       </c>
@@ -5181,7 +5234,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>897</v>
       </c>
@@ -5189,7 +5242,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>992</v>
       </c>
@@ -5244,23 +5297,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.53515625" customWidth="1"/>
-    <col min="14" max="14" width="12.3828125" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5307,7 +5360,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O2" s="6" t="s">
         <v>901</v>
       </c>
@@ -5326,26 +5379,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.53515625" customWidth="1"/>
-    <col min="5" max="5" width="14.3046875" customWidth="1"/>
-    <col min="6" max="6" width="21.3828125" customWidth="1"/>
-    <col min="7" max="7" width="11.69140625" customWidth="1"/>
-    <col min="8" max="8" width="17.15234375" customWidth="1"/>
-    <col min="9" max="9" width="9.3046875" customWidth="1"/>
-    <col min="10" max="10" width="9.69140625" customWidth="1"/>
-    <col min="11" max="11" width="39.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.3046875" customWidth="1"/>
-    <col min="14" max="14" width="23.15234375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="39.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5392,7 +5445,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -5436,7 +5489,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -5480,7 +5533,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -5524,7 +5577,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5568,7 +5621,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -5612,7 +5665,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -5656,7 +5709,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -5700,7 +5753,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5744,7 +5797,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -5788,7 +5841,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -5832,7 +5885,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -5876,7 +5929,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -5920,7 +5973,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5964,7 +6017,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -6008,7 +6061,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -6052,7 +6105,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6096,7 +6149,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -6140,7 +6193,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -6184,7 +6237,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -6228,7 +6281,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -6272,7 +6325,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6316,7 +6369,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -6360,7 +6413,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -6404,7 +6457,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -6448,7 +6501,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6492,7 +6545,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -6536,7 +6589,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -6580,7 +6633,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -6624,7 +6677,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -6668,7 +6721,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -6712,7 +6765,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -6756,7 +6809,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -6800,7 +6853,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -6844,7 +6897,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -6888,7 +6941,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -6932,7 +6985,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -6976,7 +7029,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -7020,7 +7073,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -7064,7 +7117,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -7108,7 +7161,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -7152,7 +7205,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -7196,7 +7249,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -7240,7 +7293,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7284,7 +7337,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7328,7 +7381,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -7372,7 +7425,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7416,7 +7469,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -7460,7 +7513,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -7504,7 +7557,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -7548,7 +7601,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -7592,7 +7645,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -7636,7 +7689,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7680,7 +7733,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -7724,7 +7777,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -7768,7 +7821,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -7812,7 +7865,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -7856,7 +7909,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -7900,7 +7953,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -7944,7 +7997,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -7988,7 +8041,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -8032,7 +8085,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -8076,7 +8129,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -8120,7 +8173,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -8164,7 +8217,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -8208,7 +8261,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -8252,7 +8305,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8296,7 +8349,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -8340,7 +8393,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -8384,7 +8437,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -8428,7 +8481,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -8472,7 +8525,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -8516,7 +8569,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -8560,7 +8613,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -8604,7 +8657,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -8648,7 +8701,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -8692,7 +8745,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -8736,7 +8789,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -8780,7 +8833,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -8824,7 +8877,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -8868,7 +8921,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -8912,7 +8965,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -8956,7 +9009,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -9000,7 +9053,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -9044,7 +9097,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -9088,7 +9141,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -9132,7 +9185,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -9176,7 +9229,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -9220,7 +9273,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -9264,7 +9317,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9308,7 +9361,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -9352,7 +9405,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -9396,7 +9449,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -9440,7 +9493,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -9484,7 +9537,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -9528,7 +9581,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -9572,7 +9625,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -9616,7 +9669,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -9660,7 +9713,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -9704,7 +9757,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -9748,7 +9801,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -9792,7 +9845,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -9836,7 +9889,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -9880,7 +9933,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -9924,7 +9977,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -9968,7 +10021,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -10012,7 +10065,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -10056,7 +10109,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -10100,7 +10153,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -10144,7 +10197,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -10188,7 +10241,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -10232,7 +10285,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -10276,7 +10329,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10320,7 +10373,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -10364,7 +10417,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -10408,7 +10461,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -10452,7 +10505,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -10496,7 +10549,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -10540,7 +10593,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -10584,7 +10637,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -10628,7 +10681,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -10672,7 +10725,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -10716,7 +10769,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -10760,7 +10813,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -10804,7 +10857,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -10848,7 +10901,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -10892,7 +10945,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -10936,7 +10989,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -10977,7 +11030,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -11018,7 +11071,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -11059,7 +11112,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -11116,25 +11169,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.15234375" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.15234375" customWidth="1"/>
-    <col min="9" max="9" width="7.3828125" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.3828125" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.3046875" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11181,7 +11234,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>711</v>
       </c>
@@ -11225,7 +11278,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -11284,24 +11337,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11348,7 +11401,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>713</v>
       </c>
@@ -11392,7 +11445,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>713</v>
       </c>
@@ -11436,7 +11489,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>714</v>
       </c>
@@ -11480,7 +11533,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>714</v>
       </c>
@@ -11538,26 +11591,26 @@
       <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.3828125" customWidth="1"/>
-    <col min="6" max="6" width="25.15234375" customWidth="1"/>
-    <col min="7" max="7" width="12.3046875" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.84375" customWidth="1"/>
-    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11607,7 +11660,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -11654,7 +11707,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -11701,7 +11754,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -11748,7 +11801,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -11795,7 +11848,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -11842,7 +11895,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -11889,7 +11942,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -11936,7 +11989,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -11983,7 +12036,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -12030,7 +12083,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -12077,7 +12130,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -12124,7 +12177,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -12171,7 +12224,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -12218,7 +12271,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -12265,7 +12318,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12312,7 +12365,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -12359,7 +12412,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -12406,7 +12459,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -12453,7 +12506,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -12500,7 +12553,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -12547,7 +12600,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -12594,7 +12647,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -12641,7 +12694,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -12688,7 +12741,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -12735,7 +12788,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -12782,7 +12835,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -12829,7 +12882,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -12876,7 +12929,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -12923,7 +12976,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -12970,7 +13023,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -13017,7 +13070,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -13064,7 +13117,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -13111,7 +13164,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -13158,7 +13211,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -13205,7 +13258,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -13252,7 +13305,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13299,7 +13352,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -13346,7 +13399,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -13396,7 +13449,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -13443,7 +13496,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -13490,7 +13543,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -13537,7 +13590,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -13584,7 +13637,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -13631,7 +13684,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -13678,7 +13731,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -13725,7 +13778,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -13772,7 +13825,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -13819,7 +13872,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -13866,7 +13919,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -13913,7 +13966,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -13960,7 +14013,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -14007,7 +14060,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -14054,7 +14107,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -14101,7 +14154,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -14148,7 +14201,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -14195,7 +14248,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -14242,7 +14295,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14289,7 +14342,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -14333,7 +14386,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -14377,7 +14430,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -14421,7 +14474,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -14481,26 +14534,26 @@
       <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.15234375" style="6"/>
+    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14547,7 +14600,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -14588,7 +14641,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -14626,7 +14679,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>651</v>
       </c>
@@ -14664,7 +14717,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -14705,7 +14758,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>664</v>
       </c>
@@ -14746,7 +14799,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>663</v>
       </c>
@@ -14787,7 +14840,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -14828,7 +14881,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>785</v>
       </c>
@@ -14869,7 +14922,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>786</v>
       </c>
@@ -14910,7 +14963,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>787</v>
       </c>
@@ -14951,7 +15004,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>785</v>
       </c>
@@ -14992,7 +15045,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>784</v>
       </c>
@@ -15033,7 +15086,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>804</v>
       </c>
@@ -15074,7 +15127,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>785</v>
       </c>
@@ -15115,7 +15168,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>805</v>
       </c>
@@ -15156,7 +15209,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>786</v>
       </c>
@@ -15197,7 +15250,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>806</v>
       </c>
@@ -15238,7 +15291,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>787</v>
       </c>
@@ -15279,7 +15332,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>807</v>
       </c>
@@ -15320,7 +15373,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>788</v>
       </c>
@@ -15361,7 +15414,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>808</v>
       </c>
@@ -15402,7 +15455,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>789</v>
       </c>
@@ -15443,7 +15496,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>809</v>
       </c>
@@ -15484,7 +15537,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>810</v>
       </c>
@@ -15525,7 +15578,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>811</v>
       </c>
@@ -15566,7 +15619,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>784</v>
       </c>
@@ -15607,7 +15660,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>804</v>
       </c>
@@ -15648,7 +15701,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>785</v>
       </c>
@@ -15689,7 +15742,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>805</v>
       </c>
@@ -15730,7 +15783,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>786</v>
       </c>
@@ -15771,7 +15824,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>806</v>
       </c>
@@ -15812,7 +15865,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>787</v>
       </c>
@@ -15853,7 +15906,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>807</v>
       </c>
@@ -15894,7 +15947,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>788</v>
       </c>
@@ -15935,7 +15988,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>808</v>
       </c>
@@ -15976,7 +16029,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>789</v>
       </c>
@@ -16017,7 +16070,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>809</v>
       </c>
@@ -16052,7 +16105,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>810</v>
       </c>
@@ -16093,7 +16146,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>811</v>
       </c>
@@ -16128,7 +16181,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>804</v>
       </c>
@@ -16169,7 +16222,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>804</v>
       </c>
@@ -16210,7 +16263,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>785</v>
       </c>
@@ -16239,7 +16292,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>787</v>
       </c>
@@ -16268,7 +16321,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>786</v>
       </c>
@@ -16294,7 +16347,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>1018</v>
       </c>
@@ -16323,7 +16376,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>786</v>
       </c>
@@ -16364,7 +16417,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>784</v>
       </c>
@@ -16424,23 +16477,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16487,7 +16540,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>683</v>
       </c>
@@ -16534,7 +16587,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>683</v>
       </c>
@@ -16578,7 +16631,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>697</v>
       </c>
@@ -16639,24 +16692,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.69140625" customWidth="1"/>
-    <col min="14" max="14" width="20.69140625" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16703,7 +16756,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>708</v>
       </c>
@@ -16741,12 +16794,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>710</v>
       </c>
@@ -16801,23 +16854,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.15234375" customWidth="1"/>
-    <col min="2" max="2" width="14.69140625" customWidth="1"/>
-    <col min="3" max="3" width="15.69140625" customWidth="1"/>
-    <col min="4" max="4" width="16.3046875" customWidth="1"/>
-    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.3046875" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16864,7 +16917,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -16902,7 +16955,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>913</v>
       </c>
@@ -16954,26 +17007,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.84375" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17020,7 +17073,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>912</v>
       </c>
@@ -17078,26 +17131,26 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.84375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="6.53515625" customWidth="1"/>
-    <col min="10" max="10" width="12.15234375" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.53515625" customWidth="1"/>
-    <col min="15" max="15" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -17147,7 +17200,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -17188,7 +17241,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>514</v>
       </c>
@@ -17229,7 +17282,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>515</v>
       </c>
@@ -17273,7 +17326,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>547</v>
       </c>
@@ -17314,7 +17367,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>548</v>
       </c>
@@ -17355,7 +17408,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>516</v>
       </c>
@@ -17396,7 +17449,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>517</v>
       </c>
@@ -17437,7 +17490,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>518</v>
       </c>
@@ -17478,7 +17531,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>523</v>
       </c>
@@ -17519,7 +17572,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>522</v>
       </c>
@@ -17560,7 +17613,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>556</v>
       </c>
@@ -17601,7 +17654,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>559</v>
       </c>
@@ -17642,7 +17695,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>569</v>
       </c>
@@ -17683,7 +17736,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>573</v>
       </c>
@@ -17724,7 +17777,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>574</v>
       </c>
@@ -17765,7 +17818,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>1021</v>
       </c>
@@ -17806,7 +17859,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>582</v>
       </c>
@@ -17847,7 +17900,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>588</v>
       </c>
@@ -17888,7 +17941,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>591</v>
       </c>
@@ -17929,7 +17982,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>601</v>
       </c>
@@ -17970,7 +18023,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>606</v>
       </c>
@@ -18011,7 +18064,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>614</v>
       </c>
@@ -18052,7 +18105,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>1025</v>
       </c>
@@ -18093,7 +18146,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>7805</v>
       </c>
@@ -18134,7 +18187,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>612</v>
       </c>
@@ -18175,7 +18228,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>858</v>
       </c>
@@ -18216,7 +18269,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>865</v>
       </c>
@@ -18257,7 +18310,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>872</v>
       </c>
@@ -18298,7 +18351,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>879</v>
       </c>
@@ -18339,7 +18392,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>891</v>
       </c>
@@ -18380,7 +18433,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>892</v>
       </c>
@@ -18421,7 +18474,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>935</v>
       </c>
@@ -18462,7 +18515,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>1012</v>
       </c>
@@ -18500,7 +18553,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>1040</v>
       </c>
@@ -18544,7 +18597,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18585,7 +18638,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18626,7 +18679,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18667,7 +18720,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18708,7 +18761,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18749,7 +18802,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18790,7 +18843,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18831,7 +18884,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18872,7 +18925,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18913,7 +18966,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>1043</v>
       </c>
@@ -18970,25 +19023,25 @@
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.15234375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19035,7 +19088,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>669</v>
       </c>
@@ -19082,7 +19135,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>669</v>
       </c>
@@ -19126,7 +19179,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>731</v>
       </c>

</xml_diff>

<commit_message>
Add 4 pin 100mil header, change 3 pin 100mil header name
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2E03E-ADC5-410C-9C4F-10C454C26908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82B1145-30A9-463F-ABB5-52C4BD2C52CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4735" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="1102">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -2905,9 +2905,6 @@
     <t>250 V 3 A max</t>
   </si>
   <si>
-    <t>2.54mm_header_vertical_male</t>
-  </si>
-  <si>
     <t>Normal clearance</t>
   </si>
   <si>
@@ -3344,6 +3341,21 @@
   </si>
   <si>
     <t>Stepper motor driver</t>
+  </si>
+  <si>
+    <t>61300411121</t>
+  </si>
+  <si>
+    <t>732-5317-ND</t>
+  </si>
+  <si>
+    <t>4 pin vertical 2.54 mm header</t>
+  </si>
+  <si>
+    <t>3x2.54mm_header_vertical_male</t>
+  </si>
+  <si>
+    <t>4x2.54mm_header_vertical_male</t>
   </si>
 </sst>
 </file>
@@ -3956,7 +3968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
@@ -4172,16 +4184,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E6" t="s">
         <v>931</v>
@@ -4193,7 +4205,7 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -4202,7 +4214,7 @@
         <v>16</v>
       </c>
       <c r="M6" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="O6" t="s">
         <v>900</v>
@@ -4210,28 +4222,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E7" t="s">
         <v>931</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
         <v>1090</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1091</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
@@ -4240,7 +4252,7 @@
         <v>16</v>
       </c>
       <c r="M7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="O7" t="s">
         <v>900</v>
@@ -4248,28 +4260,28 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
         <v>1095</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1095</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1094</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>1093</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1096</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
@@ -4278,7 +4290,7 @@
         <v>16</v>
       </c>
       <c r="M8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="O8" t="s">
         <v>900</v>
@@ -4384,16 +4396,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -4402,10 +4414,10 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="O3" t="s">
         <v>900</v>
@@ -4413,16 +4425,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -4431,10 +4443,10 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M4" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="O4" t="s">
         <v>900</v>
@@ -4442,16 +4454,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -4460,10 +4472,10 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="O5" t="s">
         <v>900</v>
@@ -4471,16 +4483,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -4489,10 +4501,10 @@
         <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="O6" t="s">
         <v>900</v>
@@ -4500,16 +4512,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B7" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C7" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D7" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
@@ -4518,10 +4530,10 @@
         <v>8</v>
       </c>
       <c r="K7" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M7" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="O7" t="s">
         <v>900</v>
@@ -4529,16 +4541,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D8" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
@@ -4547,10 +4559,10 @@
         <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M8" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="O8" t="s">
         <v>900</v>
@@ -4558,16 +4570,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B9" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C9" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D9" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
@@ -4576,10 +4588,10 @@
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M9" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="O9" t="s">
         <v>900</v>
@@ -4587,16 +4599,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B10" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C10" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D10" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I10" t="s">
         <v>7</v>
@@ -4605,10 +4617,10 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M10" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="O10" t="s">
         <v>900</v>
@@ -4616,16 +4628,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I11" t="s">
         <v>7</v>
@@ -4634,10 +4646,10 @@
         <v>8</v>
       </c>
       <c r="K11" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M11" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="O11" t="s">
         <v>900</v>
@@ -4645,16 +4657,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B12" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C12" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D12" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I12" t="s">
         <v>7</v>
@@ -4663,10 +4675,10 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M12" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="O12" t="s">
         <v>900</v>
@@ -4674,16 +4686,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B13" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C13" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D13" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I13" t="s">
         <v>7</v>
@@ -4692,10 +4704,10 @@
         <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M13" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="O13" t="s">
         <v>900</v>
@@ -4703,16 +4715,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I14" t="s">
         <v>7</v>
@@ -4721,10 +4733,10 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M14" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="O14" t="s">
         <v>900</v>
@@ -4732,16 +4744,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B15" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C15" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D15" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I15" t="s">
         <v>7</v>
@@ -4750,10 +4762,10 @@
         <v>8</v>
       </c>
       <c r="K15" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M15" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="O15" t="s">
         <v>900</v>
@@ -4761,16 +4773,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B16" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C16" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D16" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I16" t="s">
         <v>7</v>
@@ -4779,10 +4791,10 @@
         <v>8</v>
       </c>
       <c r="K16" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M16" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="O16" t="s">
         <v>900</v>
@@ -4790,16 +4802,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B17" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C17" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D17" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I17" t="s">
         <v>7</v>
@@ -4808,10 +4820,10 @@
         <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M17" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="O17" t="s">
         <v>900</v>
@@ -4819,16 +4831,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B18" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C18" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D18" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I18" t="s">
         <v>7</v>
@@ -4837,10 +4849,10 @@
         <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M18" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="O18" t="s">
         <v>900</v>
@@ -4848,16 +4860,16 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B19" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C19" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D19" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I19" t="s">
         <v>7</v>
@@ -4866,10 +4878,10 @@
         <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M19" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="O19" t="s">
         <v>900</v>
@@ -4877,16 +4889,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B20" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C20" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D20" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I20" t="s">
         <v>7</v>
@@ -4895,10 +4907,10 @@
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="M20" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="O20" t="s">
         <v>900</v>
@@ -4906,16 +4918,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="I21" t="s">
         <v>7</v>
@@ -4924,10 +4936,10 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M21" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="O21" t="s">
         <v>900</v>
@@ -4935,16 +4947,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B22" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C22" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D22" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I22" t="s">
         <v>7</v>
@@ -4953,10 +4965,10 @@
         <v>8</v>
       </c>
       <c r="K22" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M22" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="O22" t="s">
         <v>900</v>
@@ -4964,16 +4976,16 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I23" t="s">
         <v>7</v>
@@ -4982,10 +4994,10 @@
         <v>8</v>
       </c>
       <c r="K23" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M23" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="O23" t="s">
         <v>900</v>
@@ -4993,16 +5005,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="I24" t="s">
         <v>7</v>
@@ -5011,10 +5023,10 @@
         <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M24" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="O24" t="s">
         <v>900</v>
@@ -5022,16 +5034,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B25" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C25" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D25" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I25" t="s">
         <v>7</v>
@@ -5040,10 +5052,10 @@
         <v>8</v>
       </c>
       <c r="K25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M25" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="O25" t="s">
         <v>900</v>
@@ -5051,16 +5063,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B26" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C26" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D26" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I26" t="s">
         <v>7</v>
@@ -5069,10 +5081,10 @@
         <v>8</v>
       </c>
       <c r="K26" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="M26" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="O26" t="s">
         <v>900</v>
@@ -5244,28 +5256,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>991</v>
+      </c>
+      <c r="B7" t="s">
+        <v>991</v>
+      </c>
+      <c r="C7" t="s">
+        <v>991</v>
+      </c>
+      <c r="D7" t="s">
+        <v>991</v>
+      </c>
+      <c r="E7" t="s">
         <v>992</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>991</v>
+      </c>
+      <c r="G7" t="s">
         <v>992</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
         <v>992</v>
-      </c>
-      <c r="D7" t="s">
-        <v>992</v>
-      </c>
-      <c r="E7" t="s">
-        <v>993</v>
-      </c>
-      <c r="F7" t="s">
-        <v>992</v>
-      </c>
-      <c r="G7" t="s">
-        <v>993</v>
-      </c>
-      <c r="H7" t="s">
-        <v>993</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
@@ -5274,10 +5286,10 @@
         <v>16</v>
       </c>
       <c r="L7" t="s">
+        <v>993</v>
+      </c>
+      <c r="M7" t="s">
         <v>994</v>
-      </c>
-      <c r="M7" t="s">
-        <v>995</v>
       </c>
       <c r="O7" t="s">
         <v>901</v>
@@ -10994,37 +11006,37 @@
         <v>51</v>
       </c>
       <c r="B128" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C128" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D128" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E128" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F128" t="s">
+        <v>997</v>
+      </c>
+      <c r="G128" t="s">
+        <v>992</v>
+      </c>
+      <c r="H128" t="s">
+        <v>992</v>
+      </c>
+      <c r="I128" t="s">
+        <v>7</v>
+      </c>
+      <c r="J128" t="s">
+        <v>8</v>
+      </c>
+      <c r="L128" t="s">
         <v>998</v>
       </c>
-      <c r="G128" t="s">
-        <v>993</v>
-      </c>
-      <c r="H128" t="s">
-        <v>993</v>
-      </c>
-      <c r="I128" t="s">
-        <v>7</v>
-      </c>
-      <c r="J128" t="s">
-        <v>8</v>
-      </c>
-      <c r="L128" t="s">
+      <c r="M128" t="s">
         <v>999</v>
-      </c>
-      <c r="M128" t="s">
-        <v>1000</v>
       </c>
       <c r="O128" t="s">
         <v>900</v>
@@ -11041,31 +11053,31 @@
         <v>46</v>
       </c>
       <c r="D129" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E129" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F129" t="s">
+        <v>997</v>
+      </c>
+      <c r="G129" t="s">
+        <v>992</v>
+      </c>
+      <c r="H129" t="s">
+        <v>992</v>
+      </c>
+      <c r="I129" t="s">
+        <v>7</v>
+      </c>
+      <c r="J129" t="s">
+        <v>8</v>
+      </c>
+      <c r="L129" t="s">
         <v>998</v>
       </c>
-      <c r="G129" t="s">
-        <v>993</v>
-      </c>
-      <c r="H129" t="s">
-        <v>993</v>
-      </c>
-      <c r="I129" t="s">
-        <v>7</v>
-      </c>
-      <c r="J129" t="s">
-        <v>8</v>
-      </c>
-      <c r="L129" t="s">
+      <c r="M129" t="s">
         <v>999</v>
-      </c>
-      <c r="M129" t="s">
-        <v>1000</v>
       </c>
       <c r="O129" t="s">
         <v>900</v>
@@ -11082,31 +11094,31 @@
         <v>209</v>
       </c>
       <c r="D130" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E130" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F130" t="s">
+        <v>997</v>
+      </c>
+      <c r="G130" t="s">
+        <v>992</v>
+      </c>
+      <c r="H130" t="s">
+        <v>992</v>
+      </c>
+      <c r="I130" t="s">
+        <v>7</v>
+      </c>
+      <c r="J130" t="s">
+        <v>8</v>
+      </c>
+      <c r="L130" t="s">
         <v>998</v>
       </c>
-      <c r="G130" t="s">
-        <v>993</v>
-      </c>
-      <c r="H130" t="s">
-        <v>993</v>
-      </c>
-      <c r="I130" t="s">
-        <v>7</v>
-      </c>
-      <c r="J130" t="s">
-        <v>8</v>
-      </c>
-      <c r="L130" t="s">
+      <c r="M130" t="s">
         <v>999</v>
-      </c>
-      <c r="M130" t="s">
-        <v>1000</v>
       </c>
       <c r="O130" t="s">
         <v>900</v>
@@ -11117,37 +11129,37 @@
         <v>51</v>
       </c>
       <c r="B131" t="s">
+        <v>996</v>
+      </c>
+      <c r="C131" t="s">
+        <v>996</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E131" t="s">
+        <v>992</v>
+      </c>
+      <c r="F131" t="s">
         <v>997</v>
       </c>
-      <c r="C131" t="s">
-        <v>997</v>
-      </c>
-      <c r="D131" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E131" t="s">
-        <v>993</v>
-      </c>
-      <c r="F131" t="s">
+      <c r="G131" t="s">
+        <v>992</v>
+      </c>
+      <c r="H131" t="s">
+        <v>992</v>
+      </c>
+      <c r="I131" t="s">
+        <v>7</v>
+      </c>
+      <c r="J131" t="s">
+        <v>8</v>
+      </c>
+      <c r="L131" t="s">
         <v>998</v>
       </c>
-      <c r="G131" t="s">
-        <v>993</v>
-      </c>
-      <c r="H131" t="s">
-        <v>993</v>
-      </c>
-      <c r="I131" t="s">
-        <v>7</v>
-      </c>
-      <c r="J131" t="s">
-        <v>8</v>
-      </c>
-      <c r="L131" t="s">
+      <c r="M131" t="s">
         <v>999</v>
-      </c>
-      <c r="M131" t="s">
-        <v>1000</v>
       </c>
       <c r="O131" t="s">
         <v>900</v>
@@ -14347,25 +14359,25 @@
         <v>378</v>
       </c>
       <c r="B59" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D59" t="s">
         <v>1005</v>
       </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
+        <v>992</v>
+      </c>
+      <c r="F59" t="s">
         <v>1005</v>
       </c>
-      <c r="D59" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E59" t="s">
-        <v>993</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1006</v>
-      </c>
       <c r="G59" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="H59" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I59" t="s">
         <v>7</v>
@@ -14374,13 +14386,13 @@
         <v>8</v>
       </c>
       <c r="L59" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M59" t="s">
         <v>493</v>
       </c>
       <c r="O59" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="P59" t="s">
         <v>900</v>
@@ -14397,19 +14409,19 @@
         <v>379</v>
       </c>
       <c r="D60" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E60" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F60" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G60" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="H60" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I60" t="s">
         <v>7</v>
@@ -14418,13 +14430,13 @@
         <v>8</v>
       </c>
       <c r="L60" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M60" t="s">
         <v>493</v>
       </c>
       <c r="O60" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="P60" t="s">
         <v>900</v>
@@ -14441,19 +14453,19 @@
         <v>381</v>
       </c>
       <c r="D61" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E61" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F61" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G61" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="H61" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I61" t="s">
         <v>7</v>
@@ -14462,13 +14474,13 @@
         <v>8</v>
       </c>
       <c r="L61" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M61" t="s">
         <v>493</v>
       </c>
       <c r="O61" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="P61" t="s">
         <v>900</v>
@@ -14485,34 +14497,34 @@
         <v>382</v>
       </c>
       <c r="D62" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E62" t="s">
+        <v>992</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G62" t="s">
+        <v>992</v>
+      </c>
+      <c r="H62" t="s">
+        <v>992</v>
+      </c>
+      <c r="I62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" t="s">
+        <v>8</v>
+      </c>
+      <c r="L62" t="s">
         <v>1009</v>
-      </c>
-      <c r="E62" t="s">
-        <v>993</v>
-      </c>
-      <c r="F62" t="s">
-        <v>1009</v>
-      </c>
-      <c r="G62" t="s">
-        <v>993</v>
-      </c>
-      <c r="H62" t="s">
-        <v>993</v>
-      </c>
-      <c r="I62" t="s">
-        <v>7</v>
-      </c>
-      <c r="J62" t="s">
-        <v>8</v>
-      </c>
-      <c r="L62" t="s">
-        <v>1010</v>
       </c>
       <c r="M62" t="s">
         <v>493</v>
       </c>
       <c r="O62" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="P62" t="s">
         <v>900</v>
@@ -14527,11 +14539,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16227,10 +16239,10 @@
         <v>804</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>951</v>
+        <v>1100</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>951</v>
+        <v>1100</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>948</v>
@@ -16326,22 +16338,22 @@
         <v>786</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>1037</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>1037</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>1038</v>
       </c>
       <c r="O45" s="6" t="s">
         <v>900</v>
@@ -16349,19 +16361,19 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>1018</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>1019</v>
-      </c>
       <c r="C46" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>7</v>
@@ -16370,7 +16382,7 @@
         <v>16</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O46" s="6" t="s">
         <v>900</v>
@@ -16381,25 +16393,25 @@
         <v>786</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>947</v>
       </c>
       <c r="F47" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" s="6" t="s">
         <v>1034</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>1035</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>7</v>
@@ -16411,7 +16423,7 @@
         <v>950</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="O47" s="6" t="s">
         <v>900</v>
@@ -16422,25 +16434,25 @@
         <v>784</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>1080</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>1081</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>1080</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>1082</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>7</v>
@@ -16449,12 +16461,53 @@
         <v>16</v>
       </c>
       <c r="K48" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="M48" s="6" t="s">
         <v>1083</v>
       </c>
-      <c r="M48" s="6" t="s">
-        <v>1084</v>
-      </c>
       <c r="O48" s="6" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="O49" s="6" t="s">
         <v>900</v>
       </c>
     </row>
@@ -16810,31 +16863,31 @@
         <v>706</v>
       </c>
       <c r="D17" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E17" t="s">
         <v>1029</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
         <v>1030</v>
       </c>
-      <c r="F17" t="s">
-        <v>1029</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1032</v>
+      </c>
+      <c r="M17" t="s">
         <v>1031</v>
-      </c>
-      <c r="I17" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1033</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1032</v>
       </c>
       <c r="O17" t="s">
         <v>900</v>
@@ -16960,25 +17013,25 @@
         <v>913</v>
       </c>
       <c r="B3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>1014</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1017</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1014</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1015</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -16987,7 +17040,7 @@
         <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="O3" t="s">
         <v>900</v>
@@ -17820,28 +17873,28 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B17" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C17" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D17" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E17" t="s">
         <v>585</v>
       </c>
       <c r="F17" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
         <v>1021</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1022</v>
       </c>
       <c r="I17" t="s">
         <v>7</v>
@@ -17850,7 +17903,7 @@
         <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="O17" t="s">
         <v>583</v>
@@ -18096,7 +18149,7 @@
         <v>16</v>
       </c>
       <c r="M23" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="O23" t="s">
         <v>610</v>
@@ -18107,7 +18160,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B24" t="s">
         <v>722</v>
@@ -18116,19 +18169,19 @@
         <v>722</v>
       </c>
       <c r="D24" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E24" t="s">
         <v>723</v>
       </c>
       <c r="F24" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" t="s">
         <v>1025</v>
-      </c>
-      <c r="G24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1026</v>
       </c>
       <c r="I24" t="s">
         <v>7</v>
@@ -18137,7 +18190,7 @@
         <v>16</v>
       </c>
       <c r="M24" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="O24" t="s">
         <v>610</v>
@@ -18151,34 +18204,34 @@
         <v>7805</v>
       </c>
       <c r="B25" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D25" t="s">
         <v>1085</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1086</v>
       </c>
       <c r="E25" t="s">
         <v>704</v>
       </c>
       <c r="F25" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
         <v>1086</v>
       </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" t="s">
         <v>1087</v>
-      </c>
-      <c r="I25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="s">
-        <v>1088</v>
       </c>
       <c r="O25" t="s">
         <v>610</v>
@@ -18517,7 +18570,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B34" t="s">
         <v>584</v>
@@ -18526,13 +18579,13 @@
         <v>584</v>
       </c>
       <c r="D34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E34" t="s">
         <v>755</v>
       </c>
       <c r="F34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G34" t="s">
         <v>48</v>
@@ -18544,7 +18597,7 @@
         <v>16</v>
       </c>
       <c r="M34" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="O34" t="s">
         <v>520</v>
@@ -18555,28 +18608,28 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B35" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C35" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D35" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E35" t="s">
         <v>527</v>
       </c>
       <c r="F35" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s">
         <v>1040</v>
-      </c>
-      <c r="G35" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" t="s">
-        <v>1041</v>
       </c>
       <c r="I35" t="s">
         <v>7</v>
@@ -18585,7 +18638,7 @@
         <v>16</v>
       </c>
       <c r="M35" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="N35" t="s">
         <v>414</v>
@@ -18599,28 +18652,28 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B36" t="s">
         <v>1043</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>1044</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>1045</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1046</v>
       </c>
       <c r="E36" t="s">
         <v>755</v>
       </c>
       <c r="F36" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" t="s">
         <v>1046</v>
-      </c>
-      <c r="G36" t="s">
-        <v>48</v>
-      </c>
-      <c r="H36" t="s">
-        <v>1047</v>
       </c>
       <c r="I36" t="s">
         <v>7</v>
@@ -18629,10 +18682,10 @@
         <v>16</v>
       </c>
       <c r="M36" t="s">
+        <v>1047</v>
+      </c>
+      <c r="O36" t="s">
         <v>1048</v>
-      </c>
-      <c r="O36" t="s">
-        <v>1049</v>
       </c>
       <c r="P36" t="s">
         <v>900</v>
@@ -18640,28 +18693,28 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B37" t="s">
         <v>1043</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>1044</v>
       </c>
-      <c r="C37" t="s">
-        <v>1045</v>
-      </c>
       <c r="D37" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E37" t="s">
         <v>755</v>
       </c>
       <c r="F37" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" t="s">
         <v>1050</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" t="s">
-        <v>1051</v>
       </c>
       <c r="I37" t="s">
         <v>7</v>
@@ -18670,10 +18723,10 @@
         <v>16</v>
       </c>
       <c r="M37" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="O37" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P37" t="s">
         <v>900</v>
@@ -18681,28 +18734,28 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B38" t="s">
         <v>1043</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>1044</v>
       </c>
-      <c r="C38" t="s">
-        <v>1045</v>
-      </c>
       <c r="D38" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E38" t="s">
         <v>755</v>
       </c>
       <c r="F38" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" t="s">
         <v>1053</v>
-      </c>
-      <c r="G38" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" t="s">
-        <v>1054</v>
       </c>
       <c r="I38" t="s">
         <v>7</v>
@@ -18711,10 +18764,10 @@
         <v>16</v>
       </c>
       <c r="M38" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="O38" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P38" t="s">
         <v>900</v>
@@ -18722,28 +18775,28 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B39" t="s">
         <v>1043</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>1044</v>
       </c>
-      <c r="C39" t="s">
-        <v>1045</v>
-      </c>
       <c r="D39" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E39" t="s">
         <v>755</v>
       </c>
       <c r="F39" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" t="s">
         <v>1056</v>
-      </c>
-      <c r="G39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H39" t="s">
-        <v>1057</v>
       </c>
       <c r="I39" t="s">
         <v>7</v>
@@ -18752,10 +18805,10 @@
         <v>16</v>
       </c>
       <c r="M39" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="O39" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P39" t="s">
         <v>900</v>
@@ -18763,28 +18816,28 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B40" t="s">
         <v>1043</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>1044</v>
       </c>
-      <c r="C40" t="s">
-        <v>1045</v>
-      </c>
       <c r="D40" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E40" t="s">
         <v>755</v>
       </c>
       <c r="F40" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" t="s">
         <v>1059</v>
-      </c>
-      <c r="G40" t="s">
-        <v>48</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1060</v>
       </c>
       <c r="I40" t="s">
         <v>7</v>
@@ -18793,10 +18846,10 @@
         <v>16</v>
       </c>
       <c r="M40" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="O40" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P40" t="s">
         <v>900</v>
@@ -18804,28 +18857,28 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B41" t="s">
         <v>1043</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>1044</v>
       </c>
-      <c r="C41" t="s">
-        <v>1045</v>
-      </c>
       <c r="D41" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E41" t="s">
         <v>755</v>
       </c>
       <c r="F41" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" t="s">
         <v>1062</v>
-      </c>
-      <c r="G41" t="s">
-        <v>48</v>
-      </c>
-      <c r="H41" t="s">
-        <v>1063</v>
       </c>
       <c r="I41" t="s">
         <v>7</v>
@@ -18834,10 +18887,10 @@
         <v>16</v>
       </c>
       <c r="M41" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="O41" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P41" t="s">
         <v>900</v>
@@ -18845,28 +18898,28 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B42" t="s">
         <v>1043</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>1044</v>
       </c>
-      <c r="C42" t="s">
-        <v>1045</v>
-      </c>
       <c r="D42" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E42" t="s">
         <v>755</v>
       </c>
       <c r="F42" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G42" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" t="s">
         <v>1065</v>
-      </c>
-      <c r="G42" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" t="s">
-        <v>1066</v>
       </c>
       <c r="I42" t="s">
         <v>7</v>
@@ -18875,10 +18928,10 @@
         <v>16</v>
       </c>
       <c r="M42" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="O42" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P42" t="s">
         <v>900</v>
@@ -18886,28 +18939,28 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B43" t="s">
         <v>1043</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>1044</v>
       </c>
-      <c r="C43" t="s">
-        <v>1045</v>
-      </c>
       <c r="D43" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E43" t="s">
         <v>755</v>
       </c>
       <c r="F43" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43" t="s">
         <v>1068</v>
-      </c>
-      <c r="G43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H43" t="s">
-        <v>1069</v>
       </c>
       <c r="I43" t="s">
         <v>7</v>
@@ -18916,10 +18969,10 @@
         <v>16</v>
       </c>
       <c r="M43" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="O43" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P43" t="s">
         <v>900</v>
@@ -18927,28 +18980,28 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B44" t="s">
         <v>1043</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>1044</v>
       </c>
-      <c r="C44" t="s">
-        <v>1045</v>
-      </c>
       <c r="D44" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E44" t="s">
         <v>755</v>
       </c>
       <c r="F44" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H44" t="s">
         <v>1071</v>
-      </c>
-      <c r="G44" t="s">
-        <v>48</v>
-      </c>
-      <c r="H44" t="s">
-        <v>1072</v>
       </c>
       <c r="I44" t="s">
         <v>7</v>
@@ -18957,10 +19010,10 @@
         <v>16</v>
       </c>
       <c r="M44" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="O44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P44" t="s">
         <v>900</v>
@@ -18968,28 +19021,28 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B45" t="s">
         <v>1043</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>1044</v>
       </c>
-      <c r="C45" t="s">
-        <v>1045</v>
-      </c>
       <c r="D45" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E45" t="s">
         <v>755</v>
       </c>
       <c r="F45" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G45" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" t="s">
         <v>1074</v>
-      </c>
-      <c r="G45" t="s">
-        <v>48</v>
-      </c>
-      <c r="H45" t="s">
-        <v>1075</v>
       </c>
       <c r="I45" t="s">
         <v>7</v>
@@ -18998,10 +19051,10 @@
         <v>16</v>
       </c>
       <c r="M45" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="O45" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="P45" t="s">
         <v>900</v>

</xml_diff>

<commit_message>
Add Xilinx Artix 7 FPGAs
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82B1145-30A9-463F-ABB5-52C4BD2C52CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375DC8EF-A059-49CD-91B2-CF4E4B7B1366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4838" uniqueCount="1129">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3356,6 +3356,87 @@
   </si>
   <si>
     <t>4x2.54mm_header_vertical_male</t>
+  </si>
+  <si>
+    <t>7812</t>
+  </si>
+  <si>
+    <t>TO-220</t>
+  </si>
+  <si>
+    <t>L7812CV</t>
+  </si>
+  <si>
+    <t>497-1452-5-ND</t>
+  </si>
+  <si>
+    <t>12V 1.5A linear regulator, 14-35V input</t>
+  </si>
+  <si>
+    <t>Feather RP2040</t>
+  </si>
+  <si>
+    <t>4884</t>
+  </si>
+  <si>
+    <t>1528-4884-ND</t>
+  </si>
+  <si>
+    <t>XC7A100T-1TFG256C</t>
+  </si>
+  <si>
+    <t>Xilinx</t>
+  </si>
+  <si>
+    <t>XC7A100T-1FTG256C</t>
+  </si>
+  <si>
+    <t>122-1882-ND</t>
+  </si>
+  <si>
+    <t>Artix-7 FPGA</t>
+  </si>
+  <si>
+    <t>FTG256</t>
+  </si>
+  <si>
+    <t>XC7AxxT-1FTG256</t>
+  </si>
+  <si>
+    <t>XC7A15T-1TFG256C</t>
+  </si>
+  <si>
+    <t>XC7A35T-1TFG256C</t>
+  </si>
+  <si>
+    <t>XC7A50T-1TFG256C</t>
+  </si>
+  <si>
+    <t>XC7A75T-1TFG256C</t>
+  </si>
+  <si>
+    <t>XC7A15T-1FTG256C</t>
+  </si>
+  <si>
+    <t>XC7A35T-1FTG256C</t>
+  </si>
+  <si>
+    <t>XC7A50T-1FTG256C</t>
+  </si>
+  <si>
+    <t>XC7A75T-1FTG256C</t>
+  </si>
+  <si>
+    <t>122-1930-ND</t>
+  </si>
+  <si>
+    <t>122-1910-ND</t>
+  </si>
+  <si>
+    <t>122-1916-ND</t>
+  </si>
+  <si>
+    <t>XC7A75T-1FTG256C-ND</t>
   </si>
 </sst>
 </file>
@@ -3966,11 +4047,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ED13B0-E19A-4F33-8962-672B4F663FEB}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,7 +4065,7 @@
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4184,28 +4265,28 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="B6" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="C6" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="D6" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="E6" t="s">
         <v>931</v>
       </c>
-      <c r="F6" s="6">
-        <v>5714</v>
+      <c r="F6" s="6" t="s">
+        <v>1108</v>
       </c>
       <c r="G6" t="s">
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>1077</v>
+        <v>1109</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -4214,7 +4295,7 @@
         <v>16</v>
       </c>
       <c r="M6" t="s">
-        <v>1078</v>
+        <v>1107</v>
       </c>
       <c r="O6" t="s">
         <v>900</v>
@@ -4222,28 +4303,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1088</v>
+        <v>1076</v>
       </c>
       <c r="B7" t="s">
-        <v>1088</v>
+        <v>1076</v>
       </c>
       <c r="C7" t="s">
-        <v>1088</v>
+        <v>1076</v>
       </c>
       <c r="D7" t="s">
-        <v>1088</v>
+        <v>1076</v>
       </c>
       <c r="E7" t="s">
         <v>931</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>1089</v>
+      <c r="F7" s="6">
+        <v>5714</v>
       </c>
       <c r="G7" t="s">
         <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>1090</v>
+        <v>1077</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
@@ -4252,7 +4333,7 @@
         <v>16</v>
       </c>
       <c r="M7" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="O7" t="s">
         <v>900</v>
@@ -4260,28 +4341,28 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="B8" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="C8" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="D8" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="E8" t="s">
-        <v>1093</v>
+        <v>931</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="G8" t="s">
         <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
@@ -4290,9 +4371,47 @@
         <v>16</v>
       </c>
       <c r="M8" t="s">
+        <v>1091</v>
+      </c>
+      <c r="O8" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
         <v>1096</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O9" t="s">
         <v>900</v>
       </c>
     </row>
@@ -14541,7 +14660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
     </sheetView>
@@ -17177,11 +17296,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B93A8C-0336-4B42-880D-67109C66C120}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18242,69 +18361,69 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>612</v>
+        <v>1102</v>
       </c>
       <c r="B26" t="s">
-        <v>612</v>
+        <v>1103</v>
       </c>
       <c r="C26" t="s">
-        <v>618</v>
+        <v>1103</v>
       </c>
       <c r="D26" t="s">
-        <v>612</v>
+        <v>1104</v>
       </c>
       <c r="E26" t="s">
         <v>525</v>
       </c>
       <c r="F26" t="s">
-        <v>612</v>
+        <v>1104</v>
       </c>
       <c r="G26" t="s">
         <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>617</v>
+        <v>1105</v>
       </c>
       <c r="I26" t="s">
         <v>7</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M26" t="s">
-        <v>882</v>
+        <v>1106</v>
       </c>
       <c r="O26" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="P26" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>858</v>
+        <v>612</v>
       </c>
       <c r="B27" t="s">
-        <v>859</v>
+        <v>612</v>
       </c>
       <c r="C27" t="s">
-        <v>859</v>
+        <v>618</v>
       </c>
       <c r="D27" t="s">
-        <v>860</v>
+        <v>612</v>
       </c>
       <c r="E27" t="s">
-        <v>861</v>
+        <v>525</v>
       </c>
       <c r="F27" t="s">
-        <v>860</v>
+        <v>612</v>
       </c>
       <c r="G27" t="s">
-        <v>862</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>863</v>
+        <v>617</v>
       </c>
       <c r="I27" t="s">
         <v>7</v>
@@ -18313,39 +18432,39 @@
         <v>16</v>
       </c>
       <c r="M27" t="s">
-        <v>864</v>
+        <v>882</v>
       </c>
       <c r="O27" t="s">
-        <v>521</v>
+        <v>619</v>
       </c>
       <c r="P27" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="B28" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="C28" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="D28" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="E28" t="s">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="F28" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="G28" t="s">
-        <v>48</v>
+        <v>862</v>
       </c>
       <c r="H28" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="I28" t="s">
         <v>7</v>
@@ -18354,10 +18473,10 @@
         <v>16</v>
       </c>
       <c r="M28" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="O28" t="s">
-        <v>871</v>
+        <v>521</v>
       </c>
       <c r="P28" t="s">
         <v>900</v>
@@ -18365,28 +18484,28 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
       <c r="B29" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="C29" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="D29" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="E29" t="s">
-        <v>755</v>
+        <v>868</v>
       </c>
       <c r="F29" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="G29" t="s">
         <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="I29" t="s">
         <v>7</v>
@@ -18395,10 +18514,10 @@
         <v>16</v>
       </c>
       <c r="M29" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="O29" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="P29" t="s">
         <v>900</v>
@@ -18406,28 +18525,28 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="B30" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="C30" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="D30" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="E30" t="s">
-        <v>527</v>
+        <v>755</v>
       </c>
       <c r="F30" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="G30" t="s">
         <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="I30" t="s">
         <v>7</v>
@@ -18436,10 +18555,10 @@
         <v>16</v>
       </c>
       <c r="M30" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="O30" t="s">
-        <v>619</v>
+        <v>876</v>
       </c>
       <c r="P30" t="s">
         <v>900</v>
@@ -18447,28 +18566,28 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>891</v>
+        <v>879</v>
       </c>
       <c r="B31" t="s">
-        <v>890</v>
+        <v>879</v>
       </c>
       <c r="C31" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="D31" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="E31" t="s">
         <v>527</v>
       </c>
       <c r="F31" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="G31" t="s">
         <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
       <c r="I31" t="s">
         <v>7</v>
@@ -18477,7 +18596,7 @@
         <v>16</v>
       </c>
       <c r="M31" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="O31" t="s">
         <v>619</v>
@@ -18488,7 +18607,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B32" t="s">
         <v>890</v>
@@ -18497,19 +18616,19 @@
         <v>890</v>
       </c>
       <c r="D32" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="E32" t="s">
         <v>527</v>
       </c>
       <c r="F32" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="G32" t="s">
         <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="I32" t="s">
         <v>7</v>
@@ -18518,7 +18637,7 @@
         <v>16</v>
       </c>
       <c r="M32" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="O32" t="s">
         <v>619</v>
@@ -18529,40 +18648,40 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>935</v>
+        <v>892</v>
       </c>
       <c r="B33" t="s">
-        <v>616</v>
+        <v>890</v>
       </c>
       <c r="C33" t="s">
-        <v>616</v>
+        <v>890</v>
       </c>
       <c r="D33" t="s">
-        <v>936</v>
+        <v>887</v>
       </c>
       <c r="E33" t="s">
         <v>527</v>
       </c>
       <c r="F33" t="s">
-        <v>936</v>
+        <v>887</v>
       </c>
       <c r="G33" t="s">
         <v>48</v>
       </c>
       <c r="H33" t="s">
-        <v>937</v>
+        <v>888</v>
       </c>
       <c r="I33" t="s">
         <v>7</v>
       </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M33" t="s">
-        <v>939</v>
+        <v>889</v>
       </c>
       <c r="O33" t="s">
-        <v>938</v>
+        <v>619</v>
       </c>
       <c r="P33" t="s">
         <v>900</v>
@@ -18570,37 +18689,40 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>1011</v>
+        <v>935</v>
       </c>
       <c r="B34" t="s">
-        <v>584</v>
+        <v>616</v>
       </c>
       <c r="C34" t="s">
-        <v>584</v>
+        <v>616</v>
       </c>
       <c r="D34" t="s">
-        <v>1011</v>
+        <v>936</v>
       </c>
       <c r="E34" t="s">
-        <v>755</v>
+        <v>527</v>
       </c>
       <c r="F34" t="s">
-        <v>1011</v>
+        <v>936</v>
       </c>
       <c r="G34" t="s">
         <v>48</v>
       </c>
+      <c r="H34" t="s">
+        <v>937</v>
+      </c>
       <c r="I34" t="s">
         <v>7</v>
       </c>
       <c r="J34" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M34" t="s">
-        <v>1012</v>
+        <v>939</v>
       </c>
       <c r="O34" t="s">
-        <v>520</v>
+        <v>938</v>
       </c>
       <c r="P34" t="s">
         <v>900</v>
@@ -18608,28 +18730,25 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>1039</v>
+        <v>1011</v>
       </c>
       <c r="B35" t="s">
-        <v>1039</v>
+        <v>584</v>
       </c>
       <c r="C35" t="s">
-        <v>1039</v>
+        <v>584</v>
       </c>
       <c r="D35" t="s">
-        <v>1039</v>
+        <v>1011</v>
       </c>
       <c r="E35" t="s">
-        <v>527</v>
+        <v>755</v>
       </c>
       <c r="F35" t="s">
-        <v>1039</v>
+        <v>1011</v>
       </c>
       <c r="G35" t="s">
         <v>48</v>
-      </c>
-      <c r="H35" t="s">
-        <v>1040</v>
       </c>
       <c r="I35" t="s">
         <v>7</v>
@@ -18638,13 +18757,10 @@
         <v>16</v>
       </c>
       <c r="M35" t="s">
-        <v>1041</v>
-      </c>
-      <c r="N35" t="s">
-        <v>414</v>
+        <v>1012</v>
       </c>
       <c r="O35" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P35" t="s">
         <v>900</v>
@@ -18652,28 +18768,28 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="B36" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="C36" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
       <c r="D36" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="E36" t="s">
-        <v>755</v>
+        <v>527</v>
       </c>
       <c r="F36" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="G36" t="s">
         <v>48</v>
       </c>
       <c r="H36" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="I36" t="s">
         <v>7</v>
@@ -18682,10 +18798,13 @@
         <v>16</v>
       </c>
       <c r="M36" t="s">
-        <v>1047</v>
+        <v>1041</v>
+      </c>
+      <c r="N36" t="s">
+        <v>414</v>
       </c>
       <c r="O36" t="s">
-        <v>1048</v>
+        <v>521</v>
       </c>
       <c r="P36" t="s">
         <v>900</v>
@@ -18702,19 +18821,19 @@
         <v>1044</v>
       </c>
       <c r="D37" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="E37" t="s">
         <v>755</v>
       </c>
       <c r="F37" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="G37" t="s">
         <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="I37" t="s">
         <v>7</v>
@@ -18723,7 +18842,7 @@
         <v>16</v>
       </c>
       <c r="M37" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="O37" t="s">
         <v>1048</v>
@@ -18743,19 +18862,19 @@
         <v>1044</v>
       </c>
       <c r="D38" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="E38" t="s">
         <v>755</v>
       </c>
       <c r="F38" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="G38" t="s">
         <v>48</v>
       </c>
       <c r="H38" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="I38" t="s">
         <v>7</v>
@@ -18764,7 +18883,7 @@
         <v>16</v>
       </c>
       <c r="M38" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="O38" t="s">
         <v>1048</v>
@@ -18784,19 +18903,19 @@
         <v>1044</v>
       </c>
       <c r="D39" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="E39" t="s">
         <v>755</v>
       </c>
       <c r="F39" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="G39" t="s">
         <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="I39" t="s">
         <v>7</v>
@@ -18805,7 +18924,7 @@
         <v>16</v>
       </c>
       <c r="M39" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="O39" t="s">
         <v>1048</v>
@@ -18825,19 +18944,19 @@
         <v>1044</v>
       </c>
       <c r="D40" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="E40" t="s">
         <v>755</v>
       </c>
       <c r="F40" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="G40" t="s">
         <v>48</v>
       </c>
       <c r="H40" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="I40" t="s">
         <v>7</v>
@@ -18846,7 +18965,7 @@
         <v>16</v>
       </c>
       <c r="M40" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="O40" t="s">
         <v>1048</v>
@@ -18866,19 +18985,19 @@
         <v>1044</v>
       </c>
       <c r="D41" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="E41" t="s">
         <v>755</v>
       </c>
       <c r="F41" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G41" t="s">
         <v>48</v>
       </c>
       <c r="H41" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="I41" t="s">
         <v>7</v>
@@ -18887,7 +19006,7 @@
         <v>16</v>
       </c>
       <c r="M41" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="O41" t="s">
         <v>1048</v>
@@ -18907,19 +19026,19 @@
         <v>1044</v>
       </c>
       <c r="D42" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="E42" t="s">
         <v>755</v>
       </c>
       <c r="F42" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="G42" t="s">
         <v>48</v>
       </c>
       <c r="H42" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="I42" t="s">
         <v>7</v>
@@ -18928,7 +19047,7 @@
         <v>16</v>
       </c>
       <c r="M42" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="O42" t="s">
         <v>1048</v>
@@ -18948,19 +19067,19 @@
         <v>1044</v>
       </c>
       <c r="D43" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="E43" t="s">
         <v>755</v>
       </c>
       <c r="F43" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="G43" t="s">
         <v>48</v>
       </c>
       <c r="H43" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="I43" t="s">
         <v>7</v>
@@ -18969,7 +19088,7 @@
         <v>16</v>
       </c>
       <c r="M43" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="O43" t="s">
         <v>1048</v>
@@ -18989,19 +19108,19 @@
         <v>1044</v>
       </c>
       <c r="D44" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="E44" t="s">
         <v>755</v>
       </c>
       <c r="F44" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="G44" t="s">
         <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="I44" t="s">
         <v>7</v>
@@ -19010,7 +19129,7 @@
         <v>16</v>
       </c>
       <c r="M44" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="O44" t="s">
         <v>1048</v>
@@ -19030,19 +19149,19 @@
         <v>1044</v>
       </c>
       <c r="D45" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="E45" t="s">
         <v>755</v>
       </c>
       <c r="F45" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="G45" t="s">
         <v>48</v>
       </c>
       <c r="H45" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="I45" t="s">
         <v>7</v>
@@ -19051,12 +19170,258 @@
         <v>16</v>
       </c>
       <c r="M45" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="O45" t="s">
         <v>1048</v>
       </c>
       <c r="P45" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E46" t="s">
+        <v>755</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I46" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" t="s">
+        <v>1075</v>
+      </c>
+      <c r="O46" t="s">
+        <v>1048</v>
+      </c>
+      <c r="P46" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I47" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O47" t="s">
+        <v>565</v>
+      </c>
+      <c r="P47" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" t="s">
+        <v>16</v>
+      </c>
+      <c r="M48" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O48" t="s">
+        <v>565</v>
+      </c>
+      <c r="P48" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G49" t="s">
+        <v>48</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O49" t="s">
+        <v>565</v>
+      </c>
+      <c r="P49" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I50" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" t="s">
+        <v>16</v>
+      </c>
+      <c r="M50" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O50" t="s">
+        <v>565</v>
+      </c>
+      <c r="P50" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I51" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O51" t="s">
+        <v>565</v>
+      </c>
+      <c r="P51" t="s">
         <v>900</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start adding audio jacks
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB88AFFD-598B-4B69-B8E0-3A3BDC24D97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE78F700-188E-4D6C-8801-988FEAC96010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5638" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5662" uniqueCount="1301">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -3923,6 +3923,36 @@
   </si>
   <si>
     <t>22uH</t>
+  </si>
+  <si>
+    <t>Conn-TRS</t>
+  </si>
+  <si>
+    <t>Conn-TS</t>
+  </si>
+  <si>
+    <t>SJ-63062A</t>
+  </si>
+  <si>
+    <t>Same Sky</t>
+  </si>
+  <si>
+    <t>2223-SJ-63062A-ND</t>
+  </si>
+  <si>
+    <t>Mono 1/4" audio jack</t>
+  </si>
+  <si>
+    <t>Stereo 1/8" headphone jack</t>
+  </si>
+  <si>
+    <t>STX-3000</t>
+  </si>
+  <si>
+    <t>Kycon Inc</t>
+  </si>
+  <si>
+    <t>2092-STX-3000-ND</t>
   </si>
 </sst>
 </file>
@@ -4313,24 +4343,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15234375" customWidth="1"/>
+    <col min="14" max="14" width="13.53515625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4377,7 +4407,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>900</v>
       </c>
@@ -4396,24 +4426,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.53515625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4460,7 +4490,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>917</v>
       </c>
@@ -4498,7 +4528,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>917</v>
       </c>
@@ -4540,23 +4570,23 @@
       <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.15234375" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4603,7 +4633,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -4641,7 +4671,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -4679,7 +4709,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>757</v>
       </c>
@@ -4717,7 +4747,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>892</v>
       </c>
@@ -4749,7 +4779,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1106</v>
       </c>
@@ -4787,7 +4817,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1075</v>
       </c>
@@ -4825,7 +4855,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1087</v>
       </c>
@@ -4863,7 +4893,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>1093</v>
       </c>
@@ -4916,23 +4946,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" customWidth="1"/>
+    <col min="3" max="4" width="20.84375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.69140625" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4979,7 +5009,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>666</v>
       </c>
@@ -4999,7 +5029,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>988</v>
       </c>
@@ -5028,7 +5058,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>988</v>
       </c>
@@ -5057,7 +5087,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>988</v>
       </c>
@@ -5086,7 +5116,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>988</v>
       </c>
@@ -5115,7 +5145,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>988</v>
       </c>
@@ -5144,7 +5174,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>988</v>
       </c>
@@ -5173,7 +5203,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>988</v>
       </c>
@@ -5202,7 +5232,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>988</v>
       </c>
@@ -5231,7 +5261,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>988</v>
       </c>
@@ -5260,7 +5290,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>988</v>
       </c>
@@ -5289,7 +5319,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>988</v>
       </c>
@@ -5318,7 +5348,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>988</v>
       </c>
@@ -5347,7 +5377,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>989</v>
       </c>
@@ -5376,7 +5406,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>989</v>
       </c>
@@ -5405,7 +5435,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>989</v>
       </c>
@@ -5434,7 +5464,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>989</v>
       </c>
@@ -5463,7 +5493,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>989</v>
       </c>
@@ -5492,7 +5522,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>989</v>
       </c>
@@ -5521,7 +5551,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>989</v>
       </c>
@@ -5550,7 +5580,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>989</v>
       </c>
@@ -5579,7 +5609,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>989</v>
       </c>
@@ -5608,7 +5638,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>989</v>
       </c>
@@ -5637,7 +5667,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>989</v>
       </c>
@@ -5666,7 +5696,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>989</v>
       </c>
@@ -5709,25 +5739,25 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="13" max="13" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5774,7 +5804,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>928</v>
       </c>
@@ -5815,7 +5845,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>715</v>
       </c>
@@ -5835,7 +5865,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>716</v>
       </c>
@@ -5843,7 +5873,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>717</v>
       </c>
@@ -5851,7 +5881,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>896</v>
       </c>
@@ -5859,7 +5889,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>990</v>
       </c>
@@ -5914,23 +5944,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" customWidth="1"/>
+    <col min="14" max="14" width="12.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5977,7 +6007,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>900</v>
       </c>
@@ -5996,26 +6026,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="14.3046875" customWidth="1"/>
+    <col min="6" max="6" width="21.3828125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.15234375" customWidth="1"/>
+    <col min="9" max="9" width="9.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="39.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.3046875" customWidth="1"/>
+    <col min="14" max="14" width="23.15234375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6062,7 +6092,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -6106,7 +6136,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -6150,7 +6180,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -6194,7 +6224,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -6238,7 +6268,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -6282,7 +6312,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -6326,7 +6356,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -6370,7 +6400,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -6414,7 +6444,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -6458,7 +6488,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -6502,7 +6532,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -6546,7 +6576,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -6590,7 +6620,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -6634,7 +6664,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -6678,7 +6708,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -6722,7 +6752,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -6766,7 +6796,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -6810,7 +6840,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -6854,7 +6884,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -6898,7 +6928,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -6942,7 +6972,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -6986,7 +7016,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -7030,7 +7060,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -7074,7 +7104,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -7118,7 +7148,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -7162,7 +7192,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -7206,7 +7236,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -7250,7 +7280,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -7294,7 +7324,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -7338,7 +7368,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -7382,7 +7412,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -7426,7 +7456,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -7470,7 +7500,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -7514,7 +7544,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -7558,7 +7588,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -7602,7 +7632,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -7646,7 +7676,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -7690,7 +7720,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -7734,7 +7764,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -7778,7 +7808,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -7822,7 +7852,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -7866,7 +7896,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -7910,7 +7940,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -7954,7 +7984,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -7998,7 +8028,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -8042,7 +8072,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -8086,7 +8116,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -8130,7 +8160,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -8174,7 +8204,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -8218,7 +8248,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -8262,7 +8292,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -8306,7 +8336,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -8350,7 +8380,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -8394,7 +8424,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -8438,7 +8468,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -8482,7 +8512,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -8526,7 +8556,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -8570,7 +8600,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -8614,7 +8644,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -8658,7 +8688,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -8702,7 +8732,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -8746,7 +8776,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -8790,7 +8820,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -8834,7 +8864,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -8878,7 +8908,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -8922,7 +8952,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -8966,7 +8996,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -9010,7 +9040,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -9054,7 +9084,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -9098,7 +9128,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -9142,7 +9172,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -9186,7 +9216,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -9230,7 +9260,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -9274,7 +9304,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -9318,7 +9348,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -9362,7 +9392,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -9406,7 +9436,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -9450,7 +9480,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -9494,7 +9524,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -9538,7 +9568,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -9582,7 +9612,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -9626,7 +9656,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -9670,7 +9700,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -9714,7 +9744,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -9758,7 +9788,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -9802,7 +9832,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -9846,7 +9876,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -9890,7 +9920,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -9934,7 +9964,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -9978,7 +10008,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -10022,7 +10052,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -10066,7 +10096,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -10110,7 +10140,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -10154,7 +10184,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -10198,7 +10228,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -10242,7 +10272,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -10286,7 +10316,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -10330,7 +10360,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -10374,7 +10404,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -10418,7 +10448,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -10462,7 +10492,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -10506,7 +10536,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -10550,7 +10580,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -10594,7 +10624,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -10638,7 +10668,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -10682,7 +10712,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -10726,7 +10756,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -10770,7 +10800,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -10814,7 +10844,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -10858,7 +10888,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -10902,7 +10932,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -10946,7 +10976,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -10990,7 +11020,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -11034,7 +11064,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -11078,7 +11108,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -11122,7 +11152,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -11166,7 +11196,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -11210,7 +11240,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -11254,7 +11284,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -11298,7 +11328,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -11342,7 +11372,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -11386,7 +11416,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -11430,7 +11460,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -11474,7 +11504,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -11518,7 +11548,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -11562,7 +11592,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -11606,7 +11636,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -11647,7 +11677,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -11688,7 +11718,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -11729,7 +11759,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -11786,25 +11816,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3828125" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11851,7 +11881,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>710</v>
       </c>
@@ -11895,7 +11925,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>711</v>
       </c>
@@ -11954,24 +11984,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.53515625" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12018,7 +12048,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>712</v>
       </c>
@@ -12062,7 +12092,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -12106,7 +12136,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>713</v>
       </c>
@@ -12150,7 +12180,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>713</v>
       </c>
@@ -12208,26 +12238,26 @@
       <selection pane="bottomLeft" activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" customWidth="1"/>
+    <col min="6" max="6" width="25.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3046875" customWidth="1"/>
+    <col min="8" max="8" width="29.3046875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.84375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12277,7 +12307,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -12324,7 +12354,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -12371,7 +12401,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -12418,7 +12448,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -12465,7 +12495,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -12512,7 +12542,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -12559,7 +12589,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -12606,7 +12636,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -12653,7 +12683,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -12700,7 +12730,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -12747,7 +12777,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -12794,7 +12824,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -12841,7 +12871,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -12888,7 +12918,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -12935,7 +12965,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -12982,7 +13012,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -13029,7 +13059,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -13076,7 +13106,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -13123,7 +13153,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -13170,7 +13200,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -13217,7 +13247,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -13264,7 +13294,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -13311,7 +13341,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -13358,7 +13388,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -13405,7 +13435,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -13452,7 +13482,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -13499,7 +13529,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -13546,7 +13576,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -13593,7 +13623,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -13640,7 +13670,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -13687,7 +13717,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -13734,7 +13764,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -13781,7 +13811,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -13828,7 +13858,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -13875,7 +13905,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -13922,7 +13952,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -13969,7 +13999,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -14016,7 +14046,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -14063,7 +14093,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -14110,7 +14140,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -14157,7 +14187,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -14204,7 +14234,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -14251,7 +14281,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -14298,7 +14328,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -14345,7 +14375,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -14392,7 +14422,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -14439,7 +14469,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -14486,7 +14516,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -14533,7 +14563,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -14580,7 +14610,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -14627,7 +14657,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -14674,7 +14704,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -14721,7 +14751,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -14768,7 +14798,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -14815,7 +14845,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -14862,7 +14892,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -14909,7 +14939,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -14956,7 +14986,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -15003,7 +15033,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -15050,7 +15080,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -15097,7 +15127,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -15144,7 +15174,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>378</v>
       </c>
@@ -15191,7 +15221,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>378</v>
       </c>
@@ -15238,7 +15268,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>378</v>
       </c>
@@ -15285,7 +15315,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>378</v>
       </c>
@@ -15332,7 +15362,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>378</v>
       </c>
@@ -15379,7 +15409,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>378</v>
       </c>
@@ -15426,7 +15456,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>378</v>
       </c>
@@ -15473,7 +15503,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>378</v>
       </c>
@@ -15520,7 +15550,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>378</v>
       </c>
@@ -15567,7 +15597,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>378</v>
       </c>
@@ -15614,7 +15644,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>378</v>
       </c>
@@ -15661,7 +15691,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>378</v>
       </c>
@@ -15708,7 +15738,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>378</v>
       </c>
@@ -15755,7 +15785,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>378</v>
       </c>
@@ -15805,7 +15835,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>378</v>
       </c>
@@ -15852,7 +15882,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>378</v>
       </c>
@@ -15899,7 +15929,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -15946,7 +15976,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>378</v>
       </c>
@@ -15993,7 +16023,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>378</v>
       </c>
@@ -16040,7 +16070,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>378</v>
       </c>
@@ -16087,7 +16117,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>378</v>
       </c>
@@ -16134,7 +16164,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>378</v>
       </c>
@@ -16181,7 +16211,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>378</v>
       </c>
@@ -16228,7 +16258,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>378</v>
       </c>
@@ -16275,7 +16305,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>378</v>
       </c>
@@ -16322,7 +16352,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>378</v>
       </c>
@@ -16369,7 +16399,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>378</v>
       </c>
@@ -16416,7 +16446,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>378</v>
       </c>
@@ -16463,7 +16493,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>378</v>
       </c>
@@ -16510,7 +16540,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>378</v>
       </c>
@@ -16557,7 +16587,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>378</v>
       </c>
@@ -16604,7 +16634,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>378</v>
       </c>
@@ -16651,7 +16681,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>378</v>
       </c>
@@ -16698,7 +16728,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>378</v>
       </c>
@@ -16745,7 +16775,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>378</v>
       </c>
@@ -16789,7 +16819,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>378</v>
       </c>
@@ -16833,7 +16863,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -16877,7 +16907,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -16930,33 +16960,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
+      <selection pane="bottomLeft" activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="6"/>
+    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -17003,7 +17033,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -17044,7 +17074,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>626</v>
       </c>
@@ -17082,7 +17112,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>650</v>
       </c>
@@ -17120,7 +17150,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -17161,7 +17191,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>663</v>
       </c>
@@ -17202,7 +17232,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>662</v>
       </c>
@@ -17243,7 +17273,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>783</v>
       </c>
@@ -17284,7 +17314,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>784</v>
       </c>
@@ -17325,7 +17355,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>785</v>
       </c>
@@ -17366,7 +17396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>786</v>
       </c>
@@ -17407,7 +17437,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>784</v>
       </c>
@@ -17448,7 +17478,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>783</v>
       </c>
@@ -17489,7 +17519,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>803</v>
       </c>
@@ -17530,7 +17560,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>784</v>
       </c>
@@ -17571,7 +17601,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>804</v>
       </c>
@@ -17612,7 +17642,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>785</v>
       </c>
@@ -17653,7 +17683,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>805</v>
       </c>
@@ -17694,7 +17724,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>786</v>
       </c>
@@ -17735,7 +17765,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>806</v>
       </c>
@@ -17776,7 +17806,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>787</v>
       </c>
@@ -17817,7 +17847,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>807</v>
       </c>
@@ -17858,7 +17888,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>788</v>
       </c>
@@ -17899,7 +17929,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>808</v>
       </c>
@@ -17940,7 +17970,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>809</v>
       </c>
@@ -17981,7 +18011,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>810</v>
       </c>
@@ -18022,7 +18052,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>783</v>
       </c>
@@ -18063,7 +18093,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>803</v>
       </c>
@@ -18104,7 +18134,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>784</v>
       </c>
@@ -18145,7 +18175,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>804</v>
       </c>
@@ -18186,7 +18216,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>785</v>
       </c>
@@ -18227,7 +18257,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>805</v>
       </c>
@@ -18268,7 +18298,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>786</v>
       </c>
@@ -18309,7 +18339,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>806</v>
       </c>
@@ -18350,7 +18380,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>787</v>
       </c>
@@ -18391,7 +18421,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>807</v>
       </c>
@@ -18432,7 +18462,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>788</v>
       </c>
@@ -18473,7 +18503,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>808</v>
       </c>
@@ -18508,7 +18538,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>809</v>
       </c>
@@ -18549,7 +18579,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>810</v>
       </c>
@@ -18584,7 +18614,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>803</v>
       </c>
@@ -18625,7 +18655,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>803</v>
       </c>
@@ -18666,7 +18696,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>784</v>
       </c>
@@ -18695,7 +18725,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>786</v>
       </c>
@@ -18724,7 +18754,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>785</v>
       </c>
@@ -18750,7 +18780,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>1016</v>
       </c>
@@ -18779,7 +18809,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>785</v>
       </c>
@@ -18820,7 +18850,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="6" t="s">
         <v>783</v>
       </c>
@@ -18861,7 +18891,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="6" t="s">
         <v>784</v>
       </c>
@@ -18902,7 +18932,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="6" t="s">
         <v>1236</v>
       </c>
@@ -18943,7 +18973,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>1256</v>
       </c>
@@ -18982,6 +19012,82 @@
       </c>
       <c r="O51" s="6" t="s">
         <v>899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A52" s="6" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>1300</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>1297</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A53" s="6" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -19003,23 +19109,23 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19066,7 +19172,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>682</v>
       </c>
@@ -19113,7 +19219,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>682</v>
       </c>
@@ -19157,7 +19263,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>696</v>
       </c>
@@ -19218,24 +19324,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.69140625" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19282,7 +19388,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>707</v>
       </c>
@@ -19320,12 +19426,12 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>709</v>
       </c>
@@ -19380,23 +19486,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19443,7 +19549,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>912</v>
       </c>
@@ -19481,7 +19587,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>912</v>
       </c>
@@ -19533,26 +19639,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19599,7 +19705,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>911</v>
       </c>
@@ -19657,26 +19763,26 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" customWidth="1"/>
+    <col min="10" max="10" width="12.15234375" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.53515625" customWidth="1"/>
+    <col min="15" max="15" width="16.53515625" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -19726,7 +19832,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -19767,7 +19873,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>569</v>
       </c>
@@ -19808,7 +19914,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>573</v>
       </c>
@@ -19849,7 +19955,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>574</v>
       </c>
@@ -19890,7 +19996,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>1010</v>
       </c>
@@ -19928,7 +20034,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>1019</v>
       </c>
@@ -19969,7 +20075,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>582</v>
       </c>
@@ -20010,7 +20116,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>514</v>
       </c>
@@ -20051,7 +20157,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>515</v>
       </c>
@@ -20095,7 +20201,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>547</v>
       </c>
@@ -20136,7 +20242,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>548</v>
       </c>
@@ -20177,7 +20283,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>516</v>
       </c>
@@ -20218,7 +20324,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>517</v>
       </c>
@@ -20259,7 +20365,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>518</v>
       </c>
@@ -20300,7 +20406,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>523</v>
       </c>
@@ -20341,7 +20447,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>522</v>
       </c>
@@ -20382,7 +20488,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>857</v>
       </c>
@@ -20423,7 +20529,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>1038</v>
       </c>
@@ -20467,7 +20573,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>588</v>
       </c>
@@ -20508,7 +20614,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>591</v>
       </c>
@@ -20549,7 +20655,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>601</v>
       </c>
@@ -20590,7 +20696,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>1260</v>
       </c>
@@ -20631,7 +20737,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>1282</v>
       </c>
@@ -20672,7 +20778,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>871</v>
       </c>
@@ -20713,7 +20819,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>606</v>
       </c>
@@ -20754,7 +20860,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>613</v>
       </c>
@@ -20795,7 +20901,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>1023</v>
       </c>
@@ -20836,7 +20942,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="6">
         <v>7805</v>
       </c>
@@ -20877,7 +20983,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>1101</v>
       </c>
@@ -20918,7 +21024,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>1209</v>
       </c>
@@ -20959,7 +21065,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>1226</v>
       </c>
@@ -21000,7 +21106,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>1220</v>
       </c>
@@ -21041,7 +21147,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>1220</v>
       </c>
@@ -21082,7 +21188,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21123,7 +21229,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21164,7 +21270,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21205,7 +21311,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21246,7 +21352,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21287,7 +21393,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21328,7 +21434,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21369,7 +21475,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21410,7 +21516,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21451,7 +21557,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>1041</v>
       </c>
@@ -21492,7 +21598,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>611</v>
       </c>
@@ -21533,7 +21639,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>878</v>
       </c>
@@ -21574,7 +21680,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>890</v>
       </c>
@@ -21615,7 +21721,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" s="6" t="s">
         <v>891</v>
       </c>
@@ -21656,7 +21762,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" s="6" t="s">
         <v>864</v>
       </c>
@@ -21697,7 +21803,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" s="6" t="s">
         <v>934</v>
       </c>
@@ -21738,7 +21844,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>1115</v>
       </c>
@@ -21779,7 +21885,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" s="6" t="s">
         <v>1115</v>
       </c>
@@ -21820,7 +21926,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" s="6" t="s">
         <v>1115</v>
       </c>
@@ -21861,7 +21967,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" s="6" t="s">
         <v>1115</v>
       </c>
@@ -21902,7 +22008,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" s="6" t="s">
         <v>1115</v>
       </c>
@@ -21943,7 +22049,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" s="6" t="s">
         <v>556</v>
       </c>
@@ -21984,7 +22090,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" s="6" t="s">
         <v>559</v>
       </c>
@@ -22025,7 +22131,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" s="6" t="s">
         <v>1253</v>
       </c>
@@ -22077,31 +22183,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9A30D3-6C2F-40AA-A14D-6B8FBBCB1DF8}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.69140625" customWidth="1"/>
+    <col min="5" max="5" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.53515625" customWidth="1"/>
+    <col min="12" max="12" width="16.69140625" customWidth="1"/>
+    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -22148,7 +22254,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>668</v>
       </c>
@@ -22195,7 +22301,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>668</v>
       </c>
@@ -22239,7 +22345,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>668</v>
       </c>
@@ -22283,7 +22389,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>668</v>
       </c>
@@ -22327,7 +22433,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>668</v>
       </c>
@@ -22371,7 +22477,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>668</v>
       </c>
@@ -22415,7 +22521,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>668</v>
       </c>
@@ -22459,7 +22565,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>668</v>
       </c>
@@ -22503,7 +22609,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>668</v>
       </c>
@@ -22547,7 +22653,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>730</v>
       </c>
@@ -22591,7 +22697,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>730</v>
       </c>

</xml_diff>

<commit_message>
Add barrel power jack
</commit_message>
<xml_diff>
--- a/Moonlight_Library.xlsx
+++ b/Moonlight_Library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium\Libraries\Moonlight_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Altium\Libraries\Moonlight_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFB93E7-0BC5-41E3-8CC8-56FFC8CBF96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377FDD75-B68C-4D15-82BC-893D1EB6E32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="905" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors Polar" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5754" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5766" uniqueCount="1336">
   <si>
     <t>Symbol Ref</t>
   </si>
@@ -4046,6 +4046,18 @@
   </si>
   <si>
     <t>ASEM</t>
+  </si>
+  <si>
+    <t>PJ-102B</t>
+  </si>
+  <si>
+    <t>CP-102B-ND</t>
+  </si>
+  <si>
+    <t>5.5mm OD, 2.5mm ID barrel power jack</t>
+  </si>
+  <si>
+    <t>Conn-Barrel_Power_SW</t>
   </si>
 </sst>
 </file>
@@ -4436,24 +4448,24 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3828125" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15234375" customWidth="1"/>
+    <col min="14" max="14" width="13.53515625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4500,7 +4512,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>896</v>
       </c>
@@ -4519,24 +4531,24 @@
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3828125" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.53515625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4583,7 +4595,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>913</v>
       </c>
@@ -4621,7 +4633,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>913</v>
       </c>
@@ -4663,23 +4675,23 @@
       <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.15234375" customWidth="1"/>
+    <col min="14" max="14" width="14.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>604</v>
       </c>
@@ -4764,7 +4776,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>605</v>
       </c>
@@ -4802,7 +4814,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>754</v>
       </c>
@@ -4840,7 +4852,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>889</v>
       </c>
@@ -4872,7 +4884,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1102</v>
       </c>
@@ -4910,7 +4922,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1071</v>
       </c>
@@ -4948,7 +4960,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1083</v>
       </c>
@@ -4986,7 +4998,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>1089</v>
       </c>
@@ -5039,23 +5051,23 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53515625" customWidth="1"/>
+    <col min="3" max="4" width="20.84375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.69140625" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5102,7 +5114,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>666</v>
       </c>
@@ -5122,7 +5134,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>984</v>
       </c>
@@ -5151,7 +5163,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>984</v>
       </c>
@@ -5180,7 +5192,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>984</v>
       </c>
@@ -5209,7 +5221,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>984</v>
       </c>
@@ -5238,7 +5250,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>984</v>
       </c>
@@ -5267,7 +5279,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>984</v>
       </c>
@@ -5296,7 +5308,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>984</v>
       </c>
@@ -5325,7 +5337,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>984</v>
       </c>
@@ -5354,7 +5366,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>984</v>
       </c>
@@ -5383,7 +5395,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>984</v>
       </c>
@@ -5412,7 +5424,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>984</v>
       </c>
@@ -5441,7 +5453,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>984</v>
       </c>
@@ -5470,7 +5482,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>985</v>
       </c>
@@ -5499,7 +5511,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>985</v>
       </c>
@@ -5528,7 +5540,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>985</v>
       </c>
@@ -5557,7 +5569,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>985</v>
       </c>
@@ -5586,7 +5598,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>985</v>
       </c>
@@ -5615,7 +5627,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>985</v>
       </c>
@@ -5644,7 +5656,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>985</v>
       </c>
@@ -5673,7 +5685,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>985</v>
       </c>
@@ -5702,7 +5714,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>985</v>
       </c>
@@ -5731,7 +5743,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>985</v>
       </c>
@@ -5760,7 +5772,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>985</v>
       </c>
@@ -5789,7 +5801,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>985</v>
       </c>
@@ -5832,26 +5844,26 @@
       <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.15234375" customWidth="1"/>
+    <col min="3" max="3" width="14.3828125" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="30.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
+    <col min="13" max="13" width="30.15234375" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5898,7 +5910,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>924</v>
       </c>
@@ -5939,7 +5951,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1305</v>
       </c>
@@ -5980,7 +5992,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>1305</v>
       </c>
@@ -6021,7 +6033,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>1305</v>
       </c>
@@ -6062,7 +6074,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1305</v>
       </c>
@@ -6103,7 +6115,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1305</v>
       </c>
@@ -6144,7 +6156,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>986</v>
       </c>
@@ -6199,23 +6211,23 @@
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" customWidth="1"/>
+    <col min="14" max="14" width="12.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6262,7 +6274,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="O2" s="6" t="s">
         <v>896</v>
       </c>
@@ -6281,26 +6293,26 @@
       <selection pane="bottomLeft" activeCell="O132" sqref="O132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="14.3046875" customWidth="1"/>
+    <col min="6" max="6" width="21.3828125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.15234375" customWidth="1"/>
+    <col min="9" max="9" width="9.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="39.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.3046875" customWidth="1"/>
+    <col min="14" max="14" width="23.15234375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6347,7 +6359,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -6391,7 +6403,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -6435,7 +6447,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -6479,7 +6491,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -6523,7 +6535,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -6567,7 +6579,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
@@ -6611,7 +6623,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -6655,7 +6667,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -6699,7 +6711,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -6743,7 +6755,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -6787,7 +6799,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -6831,7 +6843,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -6875,7 +6887,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -6919,7 +6931,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -6963,7 +6975,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -7007,7 +7019,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -7051,7 +7063,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -7095,7 +7107,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -7139,7 +7151,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -7183,7 +7195,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -7227,7 +7239,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -7271,7 +7283,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -7315,7 +7327,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -7359,7 +7371,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -7403,7 +7415,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -7447,7 +7459,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -7491,7 +7503,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -7535,7 +7547,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
@@ -7579,7 +7591,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -7623,7 +7635,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -7667,7 +7679,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -7711,7 +7723,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -7755,7 +7767,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -7799,7 +7811,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -7843,7 +7855,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -7887,7 +7899,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -7931,7 +7943,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -7975,7 +7987,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -8019,7 +8031,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -8063,7 +8075,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -8107,7 +8119,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -8151,7 +8163,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -8195,7 +8207,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -8239,7 +8251,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -8283,7 +8295,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -8327,7 +8339,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -8371,7 +8383,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -8415,7 +8427,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -8459,7 +8471,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -8503,7 +8515,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -8547,7 +8559,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -8591,7 +8603,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -8635,7 +8647,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -8679,7 +8691,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -8723,7 +8735,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -8767,7 +8779,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -8811,7 +8823,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
@@ -8855,7 +8867,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -8899,7 +8911,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
@@ -8943,7 +8955,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>51</v>
       </c>
@@ -8987,7 +8999,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -9031,7 +9043,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -9075,7 +9087,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>51</v>
       </c>
@@ -9119,7 +9131,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>51</v>
       </c>
@@ -9163,7 +9175,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -9207,7 +9219,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -9251,7 +9263,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
@@ -9295,7 +9307,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>51</v>
       </c>
@@ -9339,7 +9351,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>51</v>
       </c>
@@ -9383,7 +9395,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
@@ -9427,7 +9439,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>51</v>
       </c>
@@ -9471,7 +9483,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
@@ -9515,7 +9527,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>51</v>
       </c>
@@ -9559,7 +9571,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>51</v>
       </c>
@@ -9603,7 +9615,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -9647,7 +9659,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -9691,7 +9703,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -9735,7 +9747,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -9779,7 +9791,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>51</v>
       </c>
@@ -9823,7 +9835,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>51</v>
       </c>
@@ -9867,7 +9879,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>51</v>
       </c>
@@ -9911,7 +9923,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -9955,7 +9967,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>51</v>
       </c>
@@ -9999,7 +10011,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>51</v>
       </c>
@@ -10043,7 +10055,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>51</v>
       </c>
@@ -10087,7 +10099,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -10131,7 +10143,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>51</v>
       </c>
@@ -10175,7 +10187,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>51</v>
       </c>
@@ -10219,7 +10231,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>51</v>
       </c>
@@ -10263,7 +10275,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>51</v>
       </c>
@@ -10307,7 +10319,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
@@ -10351,7 +10363,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
@@ -10395,7 +10407,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>51</v>
       </c>
@@ -10439,7 +10451,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -10483,7 +10495,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
@@ -10527,7 +10539,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -10571,7 +10583,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -10615,7 +10627,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>51</v>
       </c>
@@ -10659,7 +10671,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -10703,7 +10715,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>51</v>
       </c>
@@ -10747,7 +10759,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>51</v>
       </c>
@@ -10791,7 +10803,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -10835,7 +10847,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -10879,7 +10891,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>51</v>
       </c>
@@ -10923,7 +10935,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>51</v>
       </c>
@@ -10967,7 +10979,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>51</v>
       </c>
@@ -11011,7 +11023,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>51</v>
       </c>
@@ -11055,7 +11067,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>51</v>
       </c>
@@ -11099,7 +11111,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>51</v>
       </c>
@@ -11143,7 +11155,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
@@ -11187,7 +11199,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>51</v>
       </c>
@@ -11231,7 +11243,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>51</v>
       </c>
@@ -11275,7 +11287,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
@@ -11319,7 +11331,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>51</v>
       </c>
@@ -11363,7 +11375,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>51</v>
       </c>
@@ -11407,7 +11419,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>51</v>
       </c>
@@ -11451,7 +11463,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -11495,7 +11507,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>51</v>
       </c>
@@ -11539,7 +11551,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
@@ -11583,7 +11595,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>51</v>
       </c>
@@ -11627,7 +11639,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>51</v>
       </c>
@@ -11671,7 +11683,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
         <v>51</v>
       </c>
@@ -11715,7 +11727,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -11759,7 +11771,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>51</v>
       </c>
@@ -11803,7 +11815,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -11847,7 +11859,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -11891,7 +11903,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>51</v>
       </c>
@@ -11932,7 +11944,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>51</v>
       </c>
@@ -11973,7 +11985,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>51</v>
       </c>
@@ -12014,7 +12026,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>51</v>
       </c>
@@ -12071,25 +12083,25 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.15234375" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="9" max="9" width="7.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3828125" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12136,7 +12148,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>710</v>
       </c>
@@ -12180,7 +12192,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>711</v>
       </c>
@@ -12239,24 +12251,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.53515625" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12303,7 +12315,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>712</v>
       </c>
@@ -12347,7 +12359,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>712</v>
       </c>
@@ -12391,7 +12403,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>713</v>
       </c>
@@ -12435,7 +12447,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>713</v>
       </c>
@@ -12493,26 +12505,26 @@
       <selection pane="bottomLeft" activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" customWidth="1"/>
+    <col min="6" max="6" width="25.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3046875" customWidth="1"/>
+    <col min="8" max="8" width="29.3046875" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.53515625" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.84375" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12562,7 +12574,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>378</v>
       </c>
@@ -12609,7 +12621,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -12656,7 +12668,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>378</v>
       </c>
@@ -12703,7 +12715,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>378</v>
       </c>
@@ -12750,7 +12762,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -12797,7 +12809,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -12844,7 +12856,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>378</v>
       </c>
@@ -12891,7 +12903,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -12938,7 +12950,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>378</v>
       </c>
@@ -12985,7 +12997,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -13032,7 +13044,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>378</v>
       </c>
@@ -13079,7 +13091,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>378</v>
       </c>
@@ -13126,7 +13138,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -13173,7 +13185,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>378</v>
       </c>
@@ -13220,7 +13232,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -13267,7 +13279,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -13314,7 +13326,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>378</v>
       </c>
@@ -13361,7 +13373,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>378</v>
       </c>
@@ -13408,7 +13420,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>378</v>
       </c>
@@ -13455,7 +13467,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>378</v>
       </c>
@@ -13502,7 +13514,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>378</v>
       </c>
@@ -13549,7 +13561,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>378</v>
       </c>
@@ -13596,7 +13608,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -13643,7 +13655,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -13690,7 +13702,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>378</v>
       </c>
@@ -13737,7 +13749,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>378</v>
       </c>
@@ -13784,7 +13796,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>378</v>
       </c>
@@ -13831,7 +13843,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>378</v>
       </c>
@@ -13878,7 +13890,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -13925,7 +13937,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>378</v>
       </c>
@@ -13972,7 +13984,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -14019,7 +14031,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>378</v>
       </c>
@@ -14066,7 +14078,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>378</v>
       </c>
@@ -14113,7 +14125,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -14160,7 +14172,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -14207,7 +14219,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>378</v>
       </c>
@@ -14254,7 +14266,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>378</v>
       </c>
@@ -14301,7 +14313,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>378</v>
       </c>
@@ -14348,7 +14360,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>378</v>
       </c>
@@ -14395,7 +14407,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>378</v>
       </c>
@@ -14442,7 +14454,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -14489,7 +14501,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>378</v>
       </c>
@@ -14536,7 +14548,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>378</v>
       </c>
@@ -14583,7 +14595,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>378</v>
       </c>
@@ -14630,7 +14642,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -14677,7 +14689,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>378</v>
       </c>
@@ -14724,7 +14736,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>378</v>
       </c>
@@ -14771,7 +14783,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -14818,7 +14830,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>378</v>
       </c>
@@ -14865,7 +14877,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>378</v>
       </c>
@@ -14912,7 +14924,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>378</v>
       </c>
@@ -14959,7 +14971,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>378</v>
       </c>
@@ -15006,7 +15018,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>378</v>
       </c>
@@ -15053,7 +15065,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -15100,7 +15112,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -15147,7 +15159,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>378</v>
       </c>
@@ -15194,7 +15206,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>378</v>
       </c>
@@ -15241,7 +15253,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -15288,7 +15300,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>378</v>
       </c>
@@ -15335,7 +15347,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>378</v>
       </c>
@@ -15382,7 +15394,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -15429,7 +15441,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>378</v>
       </c>
@@ -15476,7 +15488,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>378</v>
       </c>
@@ -15523,7 +15535,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>378</v>
       </c>
@@ -15570,7 +15582,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>378</v>
       </c>
@@ -15617,7 +15629,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>378</v>
       </c>
@@ -15664,7 +15676,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>378</v>
       </c>
@@ -15711,7 +15723,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>378</v>
       </c>
@@ -15758,7 +15770,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>378</v>
       </c>
@@ -15805,7 +15817,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>378</v>
       </c>
@@ -15852,7 +15864,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>378</v>
       </c>
@@ -15899,7 +15911,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>378</v>
       </c>
@@ -15946,7 +15958,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>378</v>
       </c>
@@ -15993,7 +16005,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>378</v>
       </c>
@@ -16040,7 +16052,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>378</v>
       </c>
@@ -16090,7 +16102,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>378</v>
       </c>
@@ -16137,7 +16149,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>378</v>
       </c>
@@ -16184,7 +16196,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -16231,7 +16243,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>378</v>
       </c>
@@ -16278,7 +16290,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>378</v>
       </c>
@@ -16325,7 +16337,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>378</v>
       </c>
@@ -16372,7 +16384,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>378</v>
       </c>
@@ -16419,7 +16431,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>378</v>
       </c>
@@ -16466,7 +16478,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>378</v>
       </c>
@@ -16513,7 +16525,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>378</v>
       </c>
@@ -16560,7 +16572,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>378</v>
       </c>
@@ -16607,7 +16619,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>378</v>
       </c>
@@ -16654,7 +16666,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>378</v>
       </c>
@@ -16701,7 +16713,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>378</v>
       </c>
@@ -16748,7 +16760,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>378</v>
       </c>
@@ -16795,7 +16807,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>378</v>
       </c>
@@ -16842,7 +16854,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>378</v>
       </c>
@@ -16889,7 +16901,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>378</v>
       </c>
@@ -16936,7 +16948,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>378</v>
       </c>
@@ -16983,7 +16995,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>378</v>
       </c>
@@ -17030,7 +17042,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>378</v>
       </c>
@@ -17074,7 +17086,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>378</v>
       </c>
@@ -17118,7 +17130,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -17162,7 +17174,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -17215,34 +17227,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B37CA7-39F5-4590-9442-BABE9105E2A2}">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.15234375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.84375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.69140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="6"/>
+    <col min="13" max="13" width="46.15234375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.53515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -17289,7 +17301,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -17330,7 +17342,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>626</v>
       </c>
@@ -17368,7 +17380,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>650</v>
       </c>
@@ -17406,7 +17418,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>733910060</v>
       </c>
@@ -17447,7 +17459,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>663</v>
       </c>
@@ -17488,7 +17500,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>662</v>
       </c>
@@ -17529,7 +17541,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>780</v>
       </c>
@@ -17570,7 +17582,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>781</v>
       </c>
@@ -17611,7 +17623,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>782</v>
       </c>
@@ -17652,7 +17664,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>783</v>
       </c>
@@ -17693,7 +17705,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>781</v>
       </c>
@@ -17734,7 +17746,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>780</v>
       </c>
@@ -17775,7 +17787,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>800</v>
       </c>
@@ -17816,7 +17828,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>781</v>
       </c>
@@ -17857,7 +17869,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>801</v>
       </c>
@@ -17898,7 +17910,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>782</v>
       </c>
@@ -17939,7 +17951,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>802</v>
       </c>
@@ -17980,7 +17992,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>783</v>
       </c>
@@ -18021,7 +18033,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>803</v>
       </c>
@@ -18062,7 +18074,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>784</v>
       </c>
@@ -18103,7 +18115,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>804</v>
       </c>
@@ -18144,7 +18156,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>785</v>
       </c>
@@ -18185,7 +18197,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>805</v>
       </c>
@@ -18226,7 +18238,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>806</v>
       </c>
@@ -18267,7 +18279,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>807</v>
       </c>
@@ -18308,7 +18320,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>780</v>
       </c>
@@ -18349,7 +18361,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>800</v>
       </c>
@@ -18390,7 +18402,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>781</v>
       </c>
@@ -18431,7 +18443,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>801</v>
       </c>
@@ -18472,7 +18484,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>782</v>
       </c>
@@ -18513,7 +18525,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>802</v>
       </c>
@@ -18554,7 +18566,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>783</v>
       </c>
@@ -18595,7 +18607,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>803</v>
       </c>
@@ -18636,7 +18648,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>784</v>
       </c>
@@ -18677,7 +18689,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>804</v>
       </c>
@@ -18718,7 +18730,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>785</v>
       </c>
@@ -18759,7 +18771,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>805</v>
       </c>
@@ -18794,7 +18806,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>806</v>
       </c>
@@ -18835,7 +18847,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>807</v>
       </c>
@@ -18870,7 +18882,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>800</v>
       </c>
@@ -18911,7 +18923,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>800</v>
       </c>
@@ -18952,7 +18964,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>783</v>
       </c>
@@ -18993,7 +19005,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>781</v>
       </c>
@@ -19022,7 +19034,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>783</v>
       </c>
@@ -19051,7 +19063,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>782</v>
       </c>
@@ -19077,7 +19089,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>1012</v>
       </c>
@@ -19106,7 +19118,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A48" s="6" t="s">
         <v>782</v>
       </c>
@@ -19147,7 +19159,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="6" t="s">
         <v>780</v>
       </c>
@@ -19188,7 +19200,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="6" t="s">
         <v>781</v>
       </c>
@@ -19229,7 +19241,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>1232</v>
       </c>
@@ -19270,7 +19282,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="6" t="s">
         <v>1252</v>
       </c>
@@ -19311,7 +19323,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="6" t="s">
         <v>1287</v>
       </c>
@@ -19349,7 +19361,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="6" t="s">
         <v>1288</v>
       </c>
@@ -19384,6 +19396,44 @@
         <v>1292</v>
       </c>
       <c r="O54" s="6" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A55" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O55" s="6" t="s">
         <v>895</v>
       </c>
     </row>
@@ -19401,30 +19451,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9E494C-24C8-4E07-BD6A-CAFA4CACF635}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.69140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.53515625" customWidth="1"/>
+    <col min="4" max="4" width="23.69140625" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19471,7 +19521,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>682</v>
       </c>
@@ -19518,7 +19568,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>682</v>
       </c>
@@ -19562,7 +19612,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>696</v>
       </c>
@@ -19609,7 +19659,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>1322</v>
       </c>
@@ -19650,7 +19700,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1331</v>
       </c>
@@ -19705,24 +19755,24 @@
       <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3828125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.69140625" customWidth="1"/>
+    <col min="14" max="14" width="20.69140625" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19769,7 +19819,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>707</v>
       </c>
@@ -19807,12 +19857,12 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>709</v>
       </c>
@@ -19867,23 +19917,23 @@
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="5" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.3046875" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19930,7 +19980,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>908</v>
       </c>
@@ -19968,7 +20018,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>908</v>
       </c>
@@ -20020,26 +20070,26 @@
       <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.3828125" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.84375" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20086,7 +20136,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>907</v>
       </c>
@@ -20144,26 +20194,26 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" customWidth="1"/>
+    <col min="10" max="10" width="12.15234375" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.53515625" customWidth="1"/>
+    <col min="15" max="15" width="16.53515625" customWidth="1"/>
+    <col min="16" max="16" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -20213,7 +20263,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -20254,7 +20304,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>569</v>
       </c>
@@ -20295,7 +20345,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>573</v>
       </c>
@@ -20336,7 +20386,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>574</v>
       </c>
@@ -20377,7 +20427,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>1006</v>
       </c>
@@ -20415,7 +20465,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>1015</v>
       </c>
@@ -20456,7 +20506,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>582</v>
       </c>
@@ -20497,7 +20547,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>514</v>
       </c>
@@ -20538,7 +20588,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>515</v>
       </c>
@@ -20582,7 +20632,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>547</v>
       </c>
@@ -20623,7 +20673,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>548</v>
       </c>
@@ -20664,7 +20714,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>516</v>
       </c>
@@ -20705,7 +20755,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>517</v>
       </c>
@@ -20746,7 +20796,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>518</v>
       </c>
@@ -20787,7 +20837,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>523</v>
       </c>
@@ -20828,7 +20878,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>522</v>
       </c>
@@ -20869,7 +20919,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>854</v>
       </c>
@@ -20910,7 +20960,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>1034</v>
       </c>
@@ -20954,7 +21004,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>588</v>
       </c>
@@ -20995,7 +21045,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>591</v>
       </c>
@@ -21036,7 +21086,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>601</v>
       </c>
@@ -21077,7 +21127,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>1256</v>
       </c>
@@ -21118,7 +21168,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>1278</v>
       </c>
@@ -21159,7 +21209,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>868</v>
       </c>
@@ -21200,7 +21250,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>606</v>
       </c>
@@ -21241,7 +21291,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>613</v>
       </c>
@@ -21282,7 +21332,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>1019</v>
       </c>
@@ -21323,7 +21373,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="6">
         <v>7805</v>
       </c>
@@ -21364,7 +21414,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>1097</v>
       </c>
@@ -21405,7 +21455,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
         <v>1205</v>
       </c>
@@ -21446,7 +21496,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>1222</v>
       </c>
@@ -21487,7 +21537,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
         <v>1216</v>
       </c>
@@ -21528,7 +21578,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>1216</v>
       </c>
@@ -21569,7 +21619,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21610,7 +21660,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21651,7 +21701,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21692,7 +21742,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21733,7 +21783,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21774,7 +21824,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21815,7 +21865,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21856,7 +21906,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21897,7 +21947,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21938,7 +21988,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>1037</v>
       </c>
@@ -21979,7 +22029,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>611</v>
       </c>
@@ -22020,7 +22070,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>875</v>
       </c>
@@ -22061,7 +22111,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" s="6" t="s">
         <v>887</v>
       </c>
@@ -22102,7 +22152,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48" s="6" t="s">
         <v>888</v>
       </c>
@@ -22143,7 +22193,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49" s="6" t="s">
         <v>861</v>
       </c>
@@ -22184,7 +22234,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A50" s="6" t="s">
         <v>930</v>
       </c>
@@ -22225,7 +22275,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>1111</v>
       </c>
@@ -22266,7 +22316,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A52" s="6" t="s">
         <v>1111</v>
       </c>
@@ -22307,7 +22357,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A53" s="6" t="s">
         <v>1111</v>
       </c>
@@ -22348,7 +22398,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A54" s="6" t="s">
         <v>1111</v>
       </c>
@@ -22389,7 +22439,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A55" s="6" t="s">
         <v>1111</v>
       </c>
@@ -22430,7 +22480,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A56" s="6" t="s">
         <v>556</v>
       </c>
@@ -22471,7 +22521,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A57" s="6" t="s">
         <v>559</v>
       </c>
@@ -22512,7 +22562,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A58" s="6" t="s">
         <v>1249</v>
       </c>
@@ -22569,26 +22619,26 @@
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
+    <col min="3" max="3" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.69140625" customWidth="1"/>
+    <col min="5" max="5" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.53515625" customWidth="1"/>
+    <col min="12" max="12" width="16.69140625" customWidth="1"/>
+    <col min="13" max="13" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -22635,7 +22685,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>668</v>
       </c>
@@ -22682,7 +22732,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>668</v>
       </c>
@@ -22726,7 +22776,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>668</v>
       </c>
@@ -22770,7 +22820,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>668</v>
       </c>
@@ -22814,7 +22864,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>668</v>
       </c>
@@ -22858,7 +22908,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>668</v>
       </c>
@@ -22902,7 +22952,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>668</v>
       </c>
@@ -22946,7 +22996,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>668</v>
       </c>
@@ -22990,7 +23040,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>668</v>
       </c>
@@ -23034,7 +23084,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>727</v>
       </c>
@@ -23078,7 +23128,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>727</v>
       </c>

</xml_diff>